<commit_message>
Cassette: Play, Break Windows/Free Key (script-15) Cutscene: Purple Tentacle chases Sandy (script-150)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.200\home\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="644">
   <si>
     <t>Purpose</t>
   </si>
@@ -1955,6 +1955,18 @@
   </si>
   <si>
     <t>Flashlight has Battery</t>
+  </si>
+  <si>
+    <t>1 = Old battery</t>
+  </si>
+  <si>
+    <t>2 = Good Battery</t>
+  </si>
+  <si>
+    <t>Door: Kitchen</t>
+  </si>
+  <si>
+    <t>Window Break</t>
   </si>
 </sst>
 </file>
@@ -2286,7 +2298,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,8 +2522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,8 +3275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21463,8 +21475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22431,7 +22443,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>136</v>
       </c>
@@ -22442,7 +22454,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>126</v>
       </c>
@@ -22450,12 +22462,21 @@
         <v>638</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>31</v>
       </c>
       <c r="C83" t="s">
         <v>639</v>
+      </c>
+      <c r="E83" t="s">
+        <v>229</v>
+      </c>
+      <c r="F83" t="s">
+        <v>640</v>
+      </c>
+      <c r="G83" t="s">
+        <v>641</v>
       </c>
     </row>
   </sheetData>
@@ -22466,10 +22487,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22597,6 +22618,14 @@
         <v>585</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>643</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22606,8 +22635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H275"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25107,7 +25136,7 @@
         <v>35</v>
       </c>
       <c r="C226" t="s">
-        <v>10</v>
+        <v>642</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cutscene: Purple Tentacle reacts to police badge (script-154)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="1"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="645">
   <si>
     <t>Purpose</t>
   </si>
@@ -478,9 +478,6 @@
     <t>Memoir: Writing</t>
   </si>
   <si>
-    <t>Casette: Play, Break Windows/Free Key</t>
-  </si>
-  <si>
     <t>Telescope: Rotate</t>
   </si>
   <si>
@@ -1967,6 +1964,12 @@
   </si>
   <si>
     <t>Window Break</t>
+  </si>
+  <si>
+    <t>Cassette: Play, Break Windows/Free Key</t>
+  </si>
+  <si>
+    <t>script-154</t>
   </si>
 </sst>
 </file>
@@ -2309,7 +2312,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
@@ -2350,7 +2353,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -2358,7 +2361,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -2366,7 +2369,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -2382,7 +2385,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,7 +2393,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2401,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2414,7 +2417,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2422,7 +2425,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2430,7 +2433,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,7 +2441,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,7 +2449,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,7 +2457,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2465,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,7 +2481,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2486,7 +2489,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2497,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2505,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,7 +2513,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2522,7 +2525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -2540,10 +2543,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>530</v>
+      </c>
+      <c r="D1" t="s">
         <v>531</v>
-      </c>
-      <c r="D1" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2551,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2565,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2579,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2593,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2607,13 +2610,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,7 +2624,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2635,7 +2638,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2649,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -2663,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -2677,7 +2680,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2691,7 +2694,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2705,7 +2708,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2719,7 +2722,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -2733,7 +2736,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -2747,7 +2750,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -2761,7 +2764,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2775,7 +2778,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -2789,7 +2792,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -2803,7 +2806,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -2817,7 +2820,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -2845,7 +2848,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -2859,7 +2862,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -2873,7 +2876,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -2887,7 +2890,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -2901,7 +2904,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -2915,7 +2918,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -2929,7 +2932,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -2943,7 +2946,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2957,7 +2960,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -2971,7 +2974,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -2985,7 +2988,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -2999,7 +3002,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3013,7 +3016,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3027,7 +3030,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3041,7 +3044,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -3055,7 +3058,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -3069,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -3083,7 +3086,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,7 +3094,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -3105,7 +3108,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3119,7 +3122,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3133,7 +3136,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -3147,7 +3150,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3161,7 +3164,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3175,7 +3178,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3189,7 +3192,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3200,7 +3203,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3214,7 +3217,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -3228,7 +3231,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3242,7 +3245,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3256,7 +3259,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -3275,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3309,7 @@
         <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3350,7 +3353,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3361,7 +3364,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3372,7 +3375,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3383,7 +3386,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3394,7 +3397,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3427,7 +3430,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3438,7 +3441,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3449,7 +3452,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3460,7 +3463,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3471,7 +3474,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>643</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3482,7 +3485,7 @@
         <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3493,7 +3496,7 @@
         <v>18</v>
       </c>
       <c r="D18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3504,7 +3507,7 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3515,7 +3518,7 @@
         <v>18</v>
       </c>
       <c r="D20" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3526,7 +3529,7 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3537,7 +3540,7 @@
         <v>18</v>
       </c>
       <c r="D22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3548,7 +3551,7 @@
         <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3559,7 +3562,7 @@
         <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3570,7 +3573,7 @@
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,7 +3584,7 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,7 +3595,7 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3603,7 +3606,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3614,7 +3617,7 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3625,7 +3628,7 @@
         <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3678,7 +3681,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3689,7 +3692,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="E35" t="s">
         <v>91</v>
@@ -3703,7 +3706,7 @@
         <v>18</v>
       </c>
       <c r="D36" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3714,7 +3717,7 @@
         <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3725,7 +3728,7 @@
         <v>2</v>
       </c>
       <c r="D38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3736,7 +3739,7 @@
         <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3747,7 +3750,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3758,7 +3761,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,7 +3811,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3819,7 +3822,7 @@
         <v>18</v>
       </c>
       <c r="D46" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3830,7 +3833,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3841,7 +3844,7 @@
         <v>18</v>
       </c>
       <c r="D48" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3852,7 +3855,7 @@
         <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="50" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3863,7 +3866,7 @@
         <v>18</v>
       </c>
       <c r="D50" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3871,7 +3874,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3882,7 +3885,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3893,7 +3896,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3915,7 +3918,7 @@
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="56" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3927,7 +3930,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -20318,10 +20321,10 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F57" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="58" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20332,10 +20335,10 @@
         <v>2</v>
       </c>
       <c r="D58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F58" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20346,10 +20349,10 @@
         <v>2</v>
       </c>
       <c r="D59" t="s">
+        <v>225</v>
+      </c>
+      <c r="F59" t="s">
         <v>226</v>
-      </c>
-      <c r="F59" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="60" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20360,7 +20363,7 @@
         <v>18</v>
       </c>
       <c r="D60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20371,7 +20374,7 @@
         <v>18</v>
       </c>
       <c r="D61" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20382,7 +20385,7 @@
         <v>18</v>
       </c>
       <c r="D62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20393,7 +20396,7 @@
         <v>18</v>
       </c>
       <c r="D63" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="64" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20404,7 +20407,7 @@
         <v>18</v>
       </c>
       <c r="D64" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -20415,7 +20418,7 @@
         <v>18</v>
       </c>
       <c r="D65" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -20426,7 +20429,7 @@
         <v>18</v>
       </c>
       <c r="D66" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -20445,7 +20448,7 @@
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -20456,7 +20459,7 @@
         <v>18</v>
       </c>
       <c r="D69" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -20464,10 +20467,10 @@
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F70" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -20478,7 +20481,7 @@
         <v>18</v>
       </c>
       <c r="D71" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -20486,7 +20489,7 @@
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -20497,7 +20500,7 @@
         <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -20508,7 +20511,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -20519,7 +20522,7 @@
         <v>18</v>
       </c>
       <c r="D75" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -20530,7 +20533,7 @@
         <v>18</v>
       </c>
       <c r="D76" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -20541,7 +20544,7 @@
         <v>18</v>
       </c>
       <c r="D77" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -20552,7 +20555,7 @@
         <v>18</v>
       </c>
       <c r="D78" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -20563,7 +20566,7 @@
         <v>18</v>
       </c>
       <c r="D79" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -20574,7 +20577,7 @@
         <v>18</v>
       </c>
       <c r="D80" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -20585,7 +20588,7 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -20596,10 +20599,10 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
+        <v>267</v>
+      </c>
+      <c r="F82" t="s">
         <v>268</v>
-      </c>
-      <c r="F82" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -20610,10 +20613,10 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
+        <v>416</v>
+      </c>
+      <c r="F83" t="s">
         <v>417</v>
-      </c>
-      <c r="F83" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -20624,7 +20627,7 @@
         <v>2</v>
       </c>
       <c r="D84" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -20635,7 +20638,7 @@
         <v>2</v>
       </c>
       <c r="D85" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -20646,7 +20649,7 @@
         <v>18</v>
       </c>
       <c r="D86" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -20657,7 +20660,7 @@
         <v>18</v>
       </c>
       <c r="D87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -20668,7 +20671,7 @@
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -20693,7 +20696,7 @@
         <v>18</v>
       </c>
       <c r="D90" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -20704,7 +20707,7 @@
         <v>2</v>
       </c>
       <c r="D91" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -20729,7 +20732,7 @@
         <v>2</v>
       </c>
       <c r="D93" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -20740,7 +20743,7 @@
         <v>2</v>
       </c>
       <c r="D94" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -20751,7 +20754,7 @@
         <v>18</v>
       </c>
       <c r="D95" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -20762,7 +20765,7 @@
         <v>18</v>
       </c>
       <c r="D96" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -20773,7 +20776,7 @@
         <v>18</v>
       </c>
       <c r="D97" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -20784,7 +20787,7 @@
         <v>18</v>
       </c>
       <c r="D98" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -20795,7 +20798,7 @@
         <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -20806,10 +20809,10 @@
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F100" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -20820,7 +20823,7 @@
         <v>2</v>
       </c>
       <c r="D101" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -20831,7 +20834,7 @@
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -20842,7 +20845,7 @@
         <v>2</v>
       </c>
       <c r="D103" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -20853,7 +20856,7 @@
         <v>18</v>
       </c>
       <c r="D104" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -20864,7 +20867,7 @@
         <v>18</v>
       </c>
       <c r="D105" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -20875,7 +20878,7 @@
         <v>18</v>
       </c>
       <c r="D106" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -20886,7 +20889,7 @@
         <v>18</v>
       </c>
       <c r="D107" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -20908,7 +20911,7 @@
         <v>18</v>
       </c>
       <c r="D109" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -20919,7 +20922,7 @@
         <v>18</v>
       </c>
       <c r="D110" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -20930,7 +20933,7 @@
         <v>18</v>
       </c>
       <c r="D111" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -20941,10 +20944,10 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
+        <v>310</v>
+      </c>
+      <c r="F112" t="s">
         <v>311</v>
-      </c>
-      <c r="F112" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -20955,10 +20958,10 @@
         <v>2</v>
       </c>
       <c r="D113" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F113" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -20969,7 +20972,7 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="E114" t="s">
         <v>92</v>
@@ -20983,7 +20986,7 @@
         <v>18</v>
       </c>
       <c r="D115" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -20994,7 +20997,7 @@
         <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -21005,7 +21008,7 @@
         <v>18</v>
       </c>
       <c r="D117" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -21016,7 +21019,7 @@
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -21027,7 +21030,7 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -21038,7 +21041,7 @@
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -21049,7 +21052,7 @@
         <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -21060,7 +21063,7 @@
         <v>18</v>
       </c>
       <c r="D122" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -21071,7 +21074,7 @@
         <v>18</v>
       </c>
       <c r="D123" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -21082,7 +21085,7 @@
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -21107,7 +21110,7 @@
         <v>18</v>
       </c>
       <c r="D126" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -21118,7 +21121,7 @@
         <v>18</v>
       </c>
       <c r="D127" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -21129,7 +21132,7 @@
         <v>18</v>
       </c>
       <c r="D128" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -21154,7 +21157,7 @@
         <v>18</v>
       </c>
       <c r="D130" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -21165,7 +21168,7 @@
         <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -21176,10 +21179,10 @@
         <v>18</v>
       </c>
       <c r="D132" t="s">
+        <v>635</v>
+      </c>
+      <c r="F132" t="s">
         <v>636</v>
-      </c>
-      <c r="F132" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -21190,7 +21193,7 @@
         <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -21212,7 +21215,7 @@
         <v>18</v>
       </c>
       <c r="D135" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -21223,7 +21226,7 @@
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -21234,7 +21237,7 @@
         <v>18</v>
       </c>
       <c r="D137" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -21245,7 +21248,7 @@
         <v>18</v>
       </c>
       <c r="D138" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -21256,7 +21259,7 @@
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -21267,10 +21270,10 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F140" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -21281,7 +21284,7 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -21306,7 +21309,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -21314,7 +21317,7 @@
         <v>145</v>
       </c>
       <c r="D144" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -21339,7 +21342,7 @@
         <v>18</v>
       </c>
       <c r="D146" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E146" t="s">
         <v>81</v>
@@ -21367,7 +21370,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -21378,10 +21381,10 @@
         <v>2</v>
       </c>
       <c r="D149" t="s">
+        <v>344</v>
+      </c>
+      <c r="E149" t="s">
         <v>345</v>
-      </c>
-      <c r="E149" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -21392,7 +21395,7 @@
         <v>18</v>
       </c>
       <c r="D150" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -21403,7 +21406,7 @@
         <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -21414,7 +21417,7 @@
         <v>18</v>
       </c>
       <c r="D152" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -21425,7 +21428,7 @@
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -21436,7 +21439,7 @@
         <v>18</v>
       </c>
       <c r="D154" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -21447,10 +21450,10 @@
         <v>18</v>
       </c>
       <c r="D155" t="s">
+        <v>350</v>
+      </c>
+      <c r="E155" t="s">
         <v>351</v>
-      </c>
-      <c r="E155" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -21473,10 +21476,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21528,7 +21531,7 @@
         <v>62</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -21631,7 +21634,7 @@
         <v>67</v>
       </c>
       <c r="F10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -21676,13 +21679,13 @@
         <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="E13" t="s">
+        <v>228</v>
+      </c>
+      <c r="F13" t="s">
         <v>229</v>
-      </c>
-      <c r="F13" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -21712,7 +21715,7 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D16" t="s">
         <v>84</v>
@@ -21820,7 +21823,7 @@
         <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -21828,7 +21831,7 @@
         <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -21836,7 +21839,7 @@
         <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -21844,7 +21847,7 @@
         <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -21852,7 +21855,7 @@
         <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -21860,7 +21863,7 @@
         <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -21868,7 +21871,7 @@
         <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -21876,7 +21879,7 @@
         <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -21884,7 +21887,7 @@
         <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -21892,7 +21895,7 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -21900,7 +21903,7 @@
         <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -21908,7 +21911,7 @@
         <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -21916,22 +21919,22 @@
         <v>57</v>
       </c>
       <c r="C40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E40" t="s">
         <v>183</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>184</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>185</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>186</v>
       </c>
-      <c r="H40" t="s">
+      <c r="I40" t="s">
         <v>187</v>
-      </c>
-      <c r="I40" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -21939,7 +21942,7 @@
         <v>58</v>
       </c>
       <c r="C41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -21947,7 +21950,7 @@
         <v>59</v>
       </c>
       <c r="C42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -21955,7 +21958,7 @@
         <v>60</v>
       </c>
       <c r="C43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -21963,7 +21966,7 @@
         <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -22036,7 +22039,7 @@
         <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -22044,7 +22047,7 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -22052,7 +22055,7 @@
         <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -22060,7 +22063,7 @@
         <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -22068,22 +22071,22 @@
         <v>76</v>
       </c>
       <c r="C53" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E53" t="s">
+        <v>214</v>
+      </c>
+      <c r="F53" t="s">
         <v>215</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>216</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
+        <v>302</v>
+      </c>
+      <c r="I53" t="s">
         <v>217</v>
-      </c>
-      <c r="H53" t="s">
-        <v>303</v>
-      </c>
-      <c r="I53" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -22091,13 +22094,13 @@
         <v>78</v>
       </c>
       <c r="C54" t="s">
+        <v>220</v>
+      </c>
+      <c r="E54" t="s">
         <v>221</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>222</v>
-      </c>
-      <c r="F54" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -22105,13 +22108,13 @@
         <v>96</v>
       </c>
       <c r="C55" t="s">
+        <v>227</v>
+      </c>
+      <c r="E55" t="s">
         <v>228</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>229</v>
-      </c>
-      <c r="F55" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -22119,19 +22122,19 @@
         <v>66</v>
       </c>
       <c r="C56" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E56" t="s">
+        <v>240</v>
+      </c>
+      <c r="F56" t="s">
+        <v>435</v>
+      </c>
+      <c r="G56" t="s">
         <v>241</v>
       </c>
-      <c r="F56" t="s">
-        <v>436</v>
-      </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>242</v>
-      </c>
-      <c r="H56" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -22139,7 +22142,7 @@
         <v>11</v>
       </c>
       <c r="C57" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -22147,16 +22150,16 @@
         <v>27</v>
       </c>
       <c r="C58" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E58" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F58" t="s">
+        <v>253</v>
+      </c>
+      <c r="G58" t="s">
         <v>254</v>
-      </c>
-      <c r="G58" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -22164,19 +22167,19 @@
         <v>22</v>
       </c>
       <c r="C59" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F59" t="s">
+        <v>253</v>
+      </c>
+      <c r="G59" t="s">
         <v>254</v>
       </c>
-      <c r="G59" t="s">
-        <v>255</v>
-      </c>
       <c r="H59" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -22184,16 +22187,16 @@
         <v>24</v>
       </c>
       <c r="C60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E60" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F60" t="s">
+        <v>253</v>
+      </c>
+      <c r="G60" t="s">
         <v>254</v>
-      </c>
-      <c r="G60" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -22201,13 +22204,13 @@
         <v>64</v>
       </c>
       <c r="C61" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E61" t="s">
+        <v>228</v>
+      </c>
+      <c r="F61" t="s">
         <v>229</v>
-      </c>
-      <c r="F61" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -22215,10 +22218,10 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E62" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -22226,16 +22229,16 @@
         <v>63</v>
       </c>
       <c r="C63" t="s">
+        <v>262</v>
+      </c>
+      <c r="E63" t="s">
+        <v>240</v>
+      </c>
+      <c r="F63" t="s">
         <v>263</v>
       </c>
-      <c r="E63" t="s">
-        <v>241</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="G63" t="s">
         <v>264</v>
-      </c>
-      <c r="G63" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -22243,13 +22246,13 @@
         <v>23</v>
       </c>
       <c r="C64" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E64" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F64" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -22257,22 +22260,22 @@
         <v>13</v>
       </c>
       <c r="C65" t="s">
+        <v>291</v>
+      </c>
+      <c r="E65" t="s">
         <v>292</v>
       </c>
-      <c r="E65" t="s">
+      <c r="F65" t="s">
+        <v>297</v>
+      </c>
+      <c r="G65" t="s">
         <v>293</v>
       </c>
-      <c r="F65" t="s">
-        <v>298</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>294</v>
       </c>
-      <c r="H65" t="s">
-        <v>295</v>
-      </c>
       <c r="I65" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -22280,19 +22283,19 @@
         <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E66" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F66" t="s">
+        <v>303</v>
+      </c>
+      <c r="G66" t="s">
         <v>304</v>
       </c>
-      <c r="G66" t="s">
-        <v>305</v>
-      </c>
       <c r="H66" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -22300,13 +22303,13 @@
         <v>56</v>
       </c>
       <c r="C67" t="s">
+        <v>315</v>
+      </c>
+      <c r="E67" t="s">
         <v>316</v>
       </c>
-      <c r="E67" t="s">
+      <c r="F67" t="s">
         <v>317</v>
-      </c>
-      <c r="F67" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -22314,13 +22317,13 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
+        <v>632</v>
+      </c>
+      <c r="F68" t="s">
         <v>633</v>
       </c>
-      <c r="F68" t="s">
-        <v>634</v>
-      </c>
       <c r="G68" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -22333,7 +22336,7 @@
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -22341,19 +22344,19 @@
         <v>108</v>
       </c>
       <c r="C71" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E71" t="s">
+        <v>325</v>
+      </c>
+      <c r="F71" t="s">
         <v>326</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="s">
         <v>327</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>328</v>
-      </c>
-      <c r="H71" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -22371,10 +22374,10 @@
         <v>19</v>
       </c>
       <c r="C74" t="s">
+        <v>333</v>
+      </c>
+      <c r="E74" t="s">
         <v>334</v>
-      </c>
-      <c r="E74" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -22382,10 +22385,10 @@
         <v>79</v>
       </c>
       <c r="C75" t="s">
+        <v>352</v>
+      </c>
+      <c r="E75" t="s">
         <v>353</v>
-      </c>
-      <c r="E75" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -22393,13 +22396,13 @@
         <v>80</v>
       </c>
       <c r="C76" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E76" t="s">
+        <v>228</v>
+      </c>
+      <c r="F76" t="s">
         <v>229</v>
-      </c>
-      <c r="F76" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -22407,13 +22410,13 @@
         <v>84</v>
       </c>
       <c r="C77" t="s">
+        <v>419</v>
+      </c>
+      <c r="E77" t="s">
+        <v>228</v>
+      </c>
+      <c r="F77" t="s">
         <v>420</v>
-      </c>
-      <c r="E77" t="s">
-        <v>229</v>
-      </c>
-      <c r="F77" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -22421,10 +22424,10 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E78" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -22432,7 +22435,7 @@
         <v>83</v>
       </c>
       <c r="C79" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -22440,7 +22443,7 @@
         <v>137</v>
       </c>
       <c r="C80" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -22448,10 +22451,10 @@
         <v>136</v>
       </c>
       <c r="C81" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E81" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -22459,7 +22462,7 @@
         <v>126</v>
       </c>
       <c r="C82" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -22467,16 +22470,24 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
+        <v>638</v>
+      </c>
+      <c r="E83" t="s">
+        <v>228</v>
+      </c>
+      <c r="F83" t="s">
         <v>639</v>
       </c>
-      <c r="E83" t="s">
-        <v>229</v>
-      </c>
-      <c r="F83" t="s">
+      <c r="G83" t="s">
         <v>640</v>
       </c>
-      <c r="G83" t="s">
-        <v>641</v>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>135</v>
+      </c>
+      <c r="C84" t="s">
+        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -22503,7 +22514,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -22511,7 +22522,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -22519,7 +22530,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -22527,7 +22538,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -22543,7 +22554,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -22551,7 +22562,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -22559,7 +22570,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -22567,7 +22578,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -22575,7 +22586,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -22583,7 +22594,7 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -22591,7 +22602,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -22599,7 +22610,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -22607,7 +22618,7 @@
         <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -22615,7 +22626,7 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -22623,7 +22634,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -22636,7 +22647,7 @@
   <dimension ref="A1:H275"/>
   <sheetViews>
     <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="C99" sqref="C99"/>
+      <selection activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22657,10 +22668,10 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
@@ -22823,7 +22834,7 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -23249,10 +23260,10 @@
         <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D55" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -23260,7 +23271,7 @@
         <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -23268,7 +23279,7 @@
         <v>90</v>
       </c>
       <c r="C57" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -23276,7 +23287,7 @@
         <v>51</v>
       </c>
       <c r="C58" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
@@ -23287,7 +23298,7 @@
         <v>446</v>
       </c>
       <c r="C59" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -23309,7 +23320,7 @@
         <v>130</v>
       </c>
       <c r="C61" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -23320,7 +23331,7 @@
         <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -23331,7 +23342,7 @@
         <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -23342,7 +23353,7 @@
         <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -23353,7 +23364,7 @@
         <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -23364,7 +23375,7 @@
         <v>340</v>
       </c>
       <c r="C66" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -23375,7 +23386,7 @@
         <v>341</v>
       </c>
       <c r="C67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -23386,7 +23397,7 @@
         <v>343</v>
       </c>
       <c r="C68" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -23397,7 +23408,7 @@
         <v>345</v>
       </c>
       <c r="C69" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -23408,7 +23419,7 @@
         <v>123</v>
       </c>
       <c r="C70" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -23419,7 +23430,7 @@
         <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -23430,7 +23441,7 @@
         <v>325</v>
       </c>
       <c r="C72" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -23452,7 +23463,7 @@
         <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -23463,7 +23474,7 @@
         <v>337</v>
       </c>
       <c r="C75" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -23474,7 +23485,7 @@
         <v>338</v>
       </c>
       <c r="C76" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -23485,7 +23496,7 @@
         <v>339</v>
       </c>
       <c r="C77" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -23496,7 +23507,7 @@
         <v>108</v>
       </c>
       <c r="C78" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -23518,7 +23529,7 @@
         <v>134</v>
       </c>
       <c r="C80" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -23529,7 +23540,7 @@
         <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -23540,7 +23551,7 @@
         <v>275</v>
       </c>
       <c r="C82" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -23551,7 +23562,7 @@
         <v>326</v>
       </c>
       <c r="C83" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -23562,7 +23573,7 @@
         <v>327</v>
       </c>
       <c r="C84" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -23573,7 +23584,7 @@
         <v>328</v>
       </c>
       <c r="C85" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -23584,7 +23595,7 @@
         <v>329</v>
       </c>
       <c r="C86" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -23628,7 +23639,7 @@
         <v>39</v>
       </c>
       <c r="C90" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -23639,7 +23650,7 @@
         <v>43</v>
       </c>
       <c r="C91" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -23650,7 +23661,7 @@
         <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -23672,7 +23683,7 @@
         <v>41</v>
       </c>
       <c r="C94" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -23705,7 +23716,7 @@
         <v>273</v>
       </c>
       <c r="C97" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -23716,7 +23727,7 @@
         <v>47</v>
       </c>
       <c r="C98" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -23727,7 +23738,7 @@
         <v>207</v>
       </c>
       <c r="C99" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -23738,7 +23749,7 @@
         <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -23749,7 +23760,7 @@
         <v>179</v>
       </c>
       <c r="C101" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -23760,13 +23771,13 @@
         <v>180</v>
       </c>
       <c r="C102" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G102" t="s">
         <v>55</v>
       </c>
       <c r="H102" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -23788,7 +23799,7 @@
         <v>378</v>
       </c>
       <c r="C104" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -23854,7 +23865,7 @@
         <v>347</v>
       </c>
       <c r="C110" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -23865,7 +23876,7 @@
         <v>348</v>
       </c>
       <c r="C111" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -23876,7 +23887,7 @@
         <v>416</v>
       </c>
       <c r="C112" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -23887,7 +23898,7 @@
         <v>196</v>
       </c>
       <c r="C113" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -23898,7 +23909,7 @@
         <v>201</v>
       </c>
       <c r="C114" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -23909,7 +23920,7 @@
         <v>414</v>
       </c>
       <c r="C115" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -23920,7 +23931,7 @@
         <v>198</v>
       </c>
       <c r="C116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -23931,7 +23942,7 @@
         <v>197</v>
       </c>
       <c r="C117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -23942,7 +23953,7 @@
         <v>293</v>
       </c>
       <c r="C118" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -23953,7 +23964,7 @@
         <v>200</v>
       </c>
       <c r="C119" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -23986,7 +23997,7 @@
         <v>51</v>
       </c>
       <c r="C122" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -23997,7 +24008,7 @@
         <v>280</v>
       </c>
       <c r="C123" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -24019,7 +24030,7 @@
         <v>54</v>
       </c>
       <c r="C125" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24030,7 +24041,7 @@
         <v>50</v>
       </c>
       <c r="C126" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24041,7 +24052,7 @@
         <v>234</v>
       </c>
       <c r="C127" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24052,7 +24063,7 @@
         <v>52</v>
       </c>
       <c r="C128" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -24063,7 +24074,7 @@
         <v>55</v>
       </c>
       <c r="C129" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -24074,7 +24085,7 @@
         <v>100</v>
       </c>
       <c r="C130" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -24085,7 +24096,7 @@
         <v>57</v>
       </c>
       <c r="C131" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -24096,7 +24107,7 @@
         <v>58</v>
       </c>
       <c r="C132" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -24107,7 +24118,7 @@
         <v>59</v>
       </c>
       <c r="C133" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -24118,7 +24129,7 @@
         <v>60</v>
       </c>
       <c r="C134" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -24129,7 +24140,7 @@
         <v>56</v>
       </c>
       <c r="C135" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -24140,7 +24151,7 @@
         <v>61</v>
       </c>
       <c r="C136" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -24162,7 +24173,7 @@
         <v>277</v>
       </c>
       <c r="C138" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -24173,7 +24184,7 @@
         <v>279</v>
       </c>
       <c r="C139" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -24195,7 +24206,7 @@
         <v>312</v>
       </c>
       <c r="C141" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -24206,7 +24217,7 @@
         <v>81</v>
       </c>
       <c r="C142" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -24217,7 +24228,7 @@
         <v>311</v>
       </c>
       <c r="C143" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -24228,7 +24239,7 @@
         <v>85</v>
       </c>
       <c r="C144" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -24239,7 +24250,7 @@
         <v>266</v>
       </c>
       <c r="C145" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -24250,7 +24261,7 @@
         <v>82</v>
       </c>
       <c r="C146" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -24261,7 +24272,7 @@
         <v>83</v>
       </c>
       <c r="C147" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -24272,7 +24283,7 @@
         <v>84</v>
       </c>
       <c r="C148" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -24283,7 +24294,7 @@
         <v>212</v>
       </c>
       <c r="C149" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -24294,7 +24305,7 @@
         <v>239</v>
       </c>
       <c r="C150" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -24305,7 +24316,7 @@
         <v>86</v>
       </c>
       <c r="C151" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -24316,7 +24327,7 @@
         <v>87</v>
       </c>
       <c r="C152" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -24327,7 +24338,7 @@
         <v>88</v>
       </c>
       <c r="C153" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -24338,7 +24349,7 @@
         <v>89</v>
       </c>
       <c r="C154" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -24349,7 +24360,7 @@
         <v>90</v>
       </c>
       <c r="C155" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
@@ -24360,7 +24371,7 @@
         <v>309</v>
       </c>
       <c r="C156" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -24371,7 +24382,7 @@
         <v>233</v>
       </c>
       <c r="C157" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -24393,7 +24404,7 @@
         <v>110</v>
       </c>
       <c r="C159" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -24404,7 +24415,7 @@
         <v>111</v>
       </c>
       <c r="C160" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -24415,7 +24426,7 @@
         <v>112</v>
       </c>
       <c r="C161" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -24426,7 +24437,7 @@
         <v>113</v>
       </c>
       <c r="C162" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -24437,7 +24448,7 @@
         <v>114</v>
       </c>
       <c r="C163" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -24448,7 +24459,7 @@
         <v>115</v>
       </c>
       <c r="C164" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -24459,7 +24470,7 @@
         <v>116</v>
       </c>
       <c r="C165" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -24470,7 +24481,7 @@
         <v>117</v>
       </c>
       <c r="C166" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -24481,7 +24492,7 @@
         <v>12</v>
       </c>
       <c r="C167" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -24492,7 +24503,7 @@
         <v>119</v>
       </c>
       <c r="C168" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -24514,7 +24525,7 @@
         <v>334</v>
       </c>
       <c r="C170" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -24525,7 +24536,7 @@
         <v>268</v>
       </c>
       <c r="C171" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -24536,7 +24547,7 @@
         <v>118</v>
       </c>
       <c r="C172" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -24547,7 +24558,7 @@
         <v>101</v>
       </c>
       <c r="C173" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -24558,7 +24569,7 @@
         <v>153</v>
       </c>
       <c r="C174" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -24569,7 +24580,7 @@
         <v>331</v>
       </c>
       <c r="C175" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -24580,7 +24591,7 @@
         <v>332</v>
       </c>
       <c r="C176" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -24591,7 +24602,7 @@
         <v>330</v>
       </c>
       <c r="C177" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -24602,7 +24613,7 @@
         <v>26</v>
       </c>
       <c r="C178" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -24613,7 +24624,7 @@
         <v>120</v>
       </c>
       <c r="C179" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -24624,7 +24635,7 @@
         <v>335</v>
       </c>
       <c r="C180" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -24657,10 +24668,10 @@
         <v>103</v>
       </c>
       <c r="C183" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D183" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -24671,7 +24682,7 @@
         <v>156</v>
       </c>
       <c r="C184" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -24682,7 +24693,7 @@
         <v>235</v>
       </c>
       <c r="C185" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -24693,7 +24704,7 @@
         <v>315</v>
       </c>
       <c r="C186" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -24704,7 +24715,7 @@
         <v>316</v>
       </c>
       <c r="C187" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -24715,7 +24726,7 @@
         <v>319</v>
       </c>
       <c r="C188" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -24726,7 +24737,7 @@
         <v>318</v>
       </c>
       <c r="C189" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -24737,7 +24748,7 @@
         <v>320</v>
       </c>
       <c r="C190" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -24759,7 +24770,7 @@
         <v>154</v>
       </c>
       <c r="C192" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -24770,7 +24781,7 @@
         <v>357</v>
       </c>
       <c r="C193" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -24781,7 +24792,7 @@
         <v>159</v>
       </c>
       <c r="C194" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -24792,10 +24803,10 @@
         <v>158</v>
       </c>
       <c r="C195" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D195" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -24806,7 +24817,7 @@
         <v>231</v>
       </c>
       <c r="C196" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -24817,7 +24828,7 @@
         <v>358</v>
       </c>
       <c r="C197" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -24828,7 +24839,7 @@
         <v>155</v>
       </c>
       <c r="C198" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -24839,7 +24850,7 @@
         <v>359</v>
       </c>
       <c r="C199" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -24850,7 +24861,7 @@
         <v>157</v>
       </c>
       <c r="C200" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -24861,7 +24872,7 @@
         <v>356</v>
       </c>
       <c r="C201" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -24872,7 +24883,7 @@
         <v>184</v>
       </c>
       <c r="C202" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -24883,7 +24894,7 @@
         <v>185</v>
       </c>
       <c r="C203" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -24894,7 +24905,7 @@
         <v>186</v>
       </c>
       <c r="C204" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -24905,7 +24916,7 @@
         <v>187</v>
       </c>
       <c r="C205" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -24916,7 +24927,7 @@
         <v>188</v>
       </c>
       <c r="C206" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -24927,7 +24938,7 @@
         <v>208</v>
       </c>
       <c r="C207" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -24938,7 +24949,7 @@
         <v>300</v>
       </c>
       <c r="C208" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
@@ -24949,7 +24960,7 @@
         <v>303</v>
       </c>
       <c r="C209" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
@@ -24960,7 +24971,7 @@
         <v>310</v>
       </c>
       <c r="C210" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
@@ -24982,7 +24993,7 @@
         <v>72</v>
       </c>
       <c r="C212" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -24993,7 +25004,7 @@
         <v>74</v>
       </c>
       <c r="C213" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -25004,7 +25015,7 @@
         <v>210</v>
       </c>
       <c r="C214" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -25015,7 +25026,7 @@
         <v>294</v>
       </c>
       <c r="C215" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -25026,7 +25037,7 @@
         <v>295</v>
       </c>
       <c r="C216" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -25037,7 +25048,7 @@
         <v>296</v>
       </c>
       <c r="C217" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -25048,7 +25059,7 @@
         <v>297</v>
       </c>
       <c r="C218" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -25070,7 +25081,7 @@
         <v>299</v>
       </c>
       <c r="C220" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -25081,7 +25092,7 @@
         <v>301</v>
       </c>
       <c r="C221" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -25092,7 +25103,7 @@
         <v>302</v>
       </c>
       <c r="C222" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
@@ -25103,7 +25114,7 @@
         <v>437</v>
       </c>
       <c r="C223" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -25114,7 +25125,7 @@
         <v>438</v>
       </c>
       <c r="C224" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -25136,7 +25147,7 @@
         <v>35</v>
       </c>
       <c r="C226" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -25147,7 +25158,7 @@
         <v>36</v>
       </c>
       <c r="C227" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -25169,7 +25180,7 @@
         <v>209</v>
       </c>
       <c r="C229" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -25180,7 +25191,7 @@
         <v>269</v>
       </c>
       <c r="C230" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -25191,7 +25202,7 @@
         <v>270</v>
       </c>
       <c r="C231" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -25202,7 +25213,7 @@
         <v>271</v>
       </c>
       <c r="C232" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -25224,7 +25235,7 @@
         <v>342</v>
       </c>
       <c r="C234" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -25235,7 +25246,7 @@
         <v>344</v>
       </c>
       <c r="C235" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -25246,7 +25257,7 @@
         <v>242</v>
       </c>
       <c r="C236" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -25257,7 +25268,7 @@
         <v>274</v>
       </c>
       <c r="C237" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -25268,7 +25279,7 @@
         <v>195</v>
       </c>
       <c r="C238" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -25279,7 +25290,7 @@
         <v>131</v>
       </c>
       <c r="C239" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -25290,7 +25301,7 @@
         <v>235</v>
       </c>
       <c r="C240" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -25301,7 +25312,7 @@
         <v>192</v>
       </c>
       <c r="C241" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -25312,7 +25323,7 @@
         <v>439</v>
       </c>
       <c r="C242" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -25323,7 +25334,7 @@
         <v>194</v>
       </c>
       <c r="C243" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -25334,7 +25345,7 @@
         <v>393</v>
       </c>
       <c r="C244" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -25345,7 +25356,7 @@
         <v>394</v>
       </c>
       <c r="C245" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -25356,7 +25367,7 @@
         <v>396</v>
       </c>
       <c r="C246" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -25367,7 +25378,7 @@
         <v>397</v>
       </c>
       <c r="C247" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -25378,7 +25389,7 @@
         <v>238</v>
       </c>
       <c r="C248" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -25400,10 +25411,10 @@
         <v>7</v>
       </c>
       <c r="C250" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D250" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -25414,10 +25425,10 @@
         <v>8</v>
       </c>
       <c r="C251" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D251" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -25428,10 +25439,10 @@
         <v>9</v>
       </c>
       <c r="C252" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D252" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -25442,10 +25453,10 @@
         <v>10</v>
       </c>
       <c r="C253" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D253" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -25456,10 +25467,10 @@
         <v>11</v>
       </c>
       <c r="C254" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D254" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -25470,7 +25481,7 @@
         <v>73</v>
       </c>
       <c r="C255" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -25503,7 +25514,7 @@
         <v>253</v>
       </c>
       <c r="C258" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -25514,7 +25525,7 @@
         <v>137</v>
       </c>
       <c r="C259" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -25525,7 +25536,7 @@
         <v>418</v>
       </c>
       <c r="C260" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -25536,7 +25547,7 @@
         <v>419</v>
       </c>
       <c r="C261" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -25547,7 +25558,7 @@
         <v>420</v>
       </c>
       <c r="C262" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -25558,7 +25569,7 @@
         <v>421</v>
       </c>
       <c r="C263" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -25569,7 +25580,7 @@
         <v>417</v>
       </c>
       <c r="C264" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -25580,7 +25591,7 @@
         <v>145</v>
       </c>
       <c r="C265" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -25591,7 +25602,7 @@
         <v>349</v>
       </c>
       <c r="C266" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -25602,7 +25613,7 @@
         <v>351</v>
       </c>
       <c r="C267" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -25613,7 +25624,7 @@
         <v>352</v>
       </c>
       <c r="C268" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -25624,7 +25635,7 @@
         <v>350</v>
       </c>
       <c r="C269" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -25635,7 +25646,7 @@
         <v>408</v>
       </c>
       <c r="C270" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -25646,7 +25657,7 @@
         <v>143</v>
       </c>
       <c r="C271" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -25679,7 +25690,7 @@
         <v>252</v>
       </c>
       <c r="C274" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -25690,7 +25701,7 @@
         <v>353</v>
       </c>
       <c r="C275" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
   </sheetData>
@@ -25714,12 +25725,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B2">
         <v>7572</v>
@@ -25736,7 +25747,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B3">
         <v>5235</v>
@@ -25756,13 +25767,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B4">
         <v>3621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D4">
         <v>1230</v>
@@ -25776,7 +25787,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B5">
         <v>3412</v>
@@ -25791,7 +25802,7 @@
         <v>1977</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
   </sheetData>
@@ -25828,84 +25839,84 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B4" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Green Tentacle: Block player passing (script-158)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -1084,12 +1084,6 @@
     <t>Purple Tentacle: Move between points</t>
   </si>
   <si>
-    <t>Weird Ed: WalkTo ?</t>
-  </si>
-  <si>
-    <t>Green Tentacle: Block player until Fed</t>
-  </si>
-  <si>
     <t>script-45</t>
   </si>
   <si>
@@ -1970,6 +1964,12 @@
   </si>
   <si>
     <t>script-154</t>
+  </si>
+  <si>
+    <t>Weird Ed: Walk around the Lab Entry</t>
+  </si>
+  <si>
+    <t>Green Tentacle: Block player passing</t>
   </si>
 </sst>
 </file>
@@ -2301,7 +2301,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2525,8 +2525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2543,10 +2543,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D1" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2568,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2582,7 +2582,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2596,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2610,13 +2610,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2624,7 +2624,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2638,7 +2638,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2652,7 +2652,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -2666,7 +2666,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -2680,7 +2680,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2694,7 +2694,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2708,7 +2708,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -2722,7 +2722,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -2736,7 +2736,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -2750,7 +2750,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -2764,7 +2764,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -2778,7 +2778,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -2792,7 +2792,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -2806,7 +2806,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -2820,7 +2820,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -2848,7 +2848,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -2862,7 +2862,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -2876,7 +2876,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -2890,7 +2890,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -2904,7 +2904,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -2918,7 +2918,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -2932,7 +2932,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -2946,7 +2946,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -2960,7 +2960,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -2974,7 +2974,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -2988,7 +2988,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3002,7 +3002,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3016,7 +3016,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3030,7 +3030,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3044,7 +3044,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -3058,7 +3058,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -3072,7 +3072,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -3086,7 +3086,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3094,7 +3094,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -3108,7 +3108,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3122,7 +3122,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3136,7 +3136,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -3150,7 +3150,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3164,7 +3164,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3178,7 +3178,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3192,7 +3192,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3203,7 +3203,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3217,7 +3217,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -3231,7 +3231,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3245,7 +3245,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3259,7 +3259,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -3278,8 +3278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+      <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,7 +3353,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3364,7 +3364,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3375,7 +3375,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3430,7 +3430,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3452,7 +3452,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3463,7 +3463,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3474,7 +3474,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3584,7 +3584,7 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3595,7 +3595,7 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3606,7 +3606,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3617,7 +3617,7 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3681,7 +3681,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3692,7 +3692,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="E35" t="s">
         <v>91</v>
@@ -3811,7 +3811,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,7 +3874,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3885,7 +3885,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3896,7 +3896,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3918,7 +3918,7 @@
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="56" spans="1:16384" x14ac:dyDescent="0.25">
@@ -3930,7 +3930,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -20613,10 +20613,10 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="F83" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -20798,7 +20798,7 @@
         <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -20809,7 +20809,7 @@
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="F100" t="s">
         <v>290</v>
@@ -20856,7 +20856,7 @@
         <v>18</v>
       </c>
       <c r="D104" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -20867,7 +20867,7 @@
         <v>18</v>
       </c>
       <c r="D105" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -20889,7 +20889,7 @@
         <v>18</v>
       </c>
       <c r="D107" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -20972,7 +20972,7 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E114" t="s">
         <v>92</v>
@@ -20986,7 +20986,7 @@
         <v>18</v>
       </c>
       <c r="D115" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -20997,7 +20997,7 @@
         <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -21041,7 +21041,7 @@
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -21168,7 +21168,7 @@
         <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -21179,10 +21179,10 @@
         <v>18</v>
       </c>
       <c r="D132" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F132" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -21237,7 +21237,7 @@
         <v>18</v>
       </c>
       <c r="D137" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -21270,10 +21270,10 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="F140" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -21284,7 +21284,7 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -21309,7 +21309,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -21342,7 +21342,7 @@
         <v>18</v>
       </c>
       <c r="D146" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="E146" t="s">
         <v>81</v>
@@ -21428,7 +21428,7 @@
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -21439,7 +21439,7 @@
         <v>18</v>
       </c>
       <c r="D154" t="s">
-        <v>349</v>
+        <v>643</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -21450,10 +21450,10 @@
         <v>18</v>
       </c>
       <c r="D155" t="s">
-        <v>350</v>
+        <v>644</v>
       </c>
       <c r="E155" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -21478,8 +21478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21679,7 +21679,7 @@
         <v>110</v>
       </c>
       <c r="C13" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="E13" t="s">
         <v>228</v>
@@ -21715,7 +21715,7 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="D16" t="s">
         <v>84</v>
@@ -22128,7 +22128,7 @@
         <v>240</v>
       </c>
       <c r="F56" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G56" t="s">
         <v>241</v>
@@ -22179,7 +22179,7 @@
         <v>254</v>
       </c>
       <c r="H59" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -22283,7 +22283,7 @@
         <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="E66" t="s">
         <v>305</v>
@@ -22295,7 +22295,7 @@
         <v>304</v>
       </c>
       <c r="H66" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -22317,10 +22317,10 @@
         <v>18</v>
       </c>
       <c r="C68" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="F68" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="G68" t="s">
         <v>319</v>
@@ -22336,7 +22336,7 @@
         <v>67</v>
       </c>
       <c r="C70" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -22385,10 +22385,10 @@
         <v>79</v>
       </c>
       <c r="C75" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="E75" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -22396,7 +22396,7 @@
         <v>80</v>
       </c>
       <c r="C76" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="E76" t="s">
         <v>228</v>
@@ -22410,13 +22410,13 @@
         <v>84</v>
       </c>
       <c r="C77" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="E77" t="s">
         <v>228</v>
       </c>
       <c r="F77" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -22424,7 +22424,7 @@
         <v>75</v>
       </c>
       <c r="C78" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E78" t="s">
         <v>297</v>
@@ -22435,7 +22435,7 @@
         <v>83</v>
       </c>
       <c r="C79" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -22443,7 +22443,7 @@
         <v>137</v>
       </c>
       <c r="C80" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -22451,7 +22451,7 @@
         <v>136</v>
       </c>
       <c r="C81" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="E81" t="s">
         <v>229</v>
@@ -22462,7 +22462,7 @@
         <v>126</v>
       </c>
       <c r="C82" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -22470,16 +22470,16 @@
         <v>31</v>
       </c>
       <c r="C83" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="E83" t="s">
         <v>228</v>
       </c>
       <c r="F83" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G83" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -22487,7 +22487,7 @@
         <v>135</v>
       </c>
       <c r="C84" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
   </sheetData>
@@ -22514,7 +22514,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -22522,7 +22522,7 @@
         <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -22530,7 +22530,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -22538,7 +22538,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -22554,7 +22554,7 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -22562,7 +22562,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -22570,7 +22570,7 @@
         <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -22578,7 +22578,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -22586,7 +22586,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -22594,7 +22594,7 @@
         <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -22602,7 +22602,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -22610,7 +22610,7 @@
         <v>54</v>
       </c>
       <c r="B13" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -22626,7 +22626,7 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -22634,7 +22634,7 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
   </sheetData>
@@ -22668,10 +22668,10 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="F1" s="1"/>
       <c r="G1" s="1" t="s">
@@ -22834,7 +22834,7 @@
         <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -23260,10 +23260,10 @@
         <v>124</v>
       </c>
       <c r="C55" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D55" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -23298,7 +23298,7 @@
         <v>446</v>
       </c>
       <c r="C59" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -23320,7 +23320,7 @@
         <v>130</v>
       </c>
       <c r="C61" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -23331,7 +23331,7 @@
         <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -23342,7 +23342,7 @@
         <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -23353,7 +23353,7 @@
         <v>127</v>
       </c>
       <c r="C64" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -23364,7 +23364,7 @@
         <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -23375,7 +23375,7 @@
         <v>340</v>
       </c>
       <c r="C66" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -23386,7 +23386,7 @@
         <v>341</v>
       </c>
       <c r="C67" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -23397,7 +23397,7 @@
         <v>343</v>
       </c>
       <c r="C68" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -23408,7 +23408,7 @@
         <v>345</v>
       </c>
       <c r="C69" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -23419,7 +23419,7 @@
         <v>123</v>
       </c>
       <c r="C70" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -23430,7 +23430,7 @@
         <v>121</v>
       </c>
       <c r="C71" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -23441,7 +23441,7 @@
         <v>325</v>
       </c>
       <c r="C72" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -23463,7 +23463,7 @@
         <v>125</v>
       </c>
       <c r="C74" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -23474,7 +23474,7 @@
         <v>337</v>
       </c>
       <c r="C75" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -23485,7 +23485,7 @@
         <v>338</v>
       </c>
       <c r="C76" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -23496,7 +23496,7 @@
         <v>339</v>
       </c>
       <c r="C77" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -23507,7 +23507,7 @@
         <v>108</v>
       </c>
       <c r="C78" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -23529,7 +23529,7 @@
         <v>134</v>
       </c>
       <c r="C80" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -23540,7 +23540,7 @@
         <v>138</v>
       </c>
       <c r="C81" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -23551,7 +23551,7 @@
         <v>275</v>
       </c>
       <c r="C82" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -23562,7 +23562,7 @@
         <v>326</v>
       </c>
       <c r="C83" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -23573,7 +23573,7 @@
         <v>327</v>
       </c>
       <c r="C84" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -23584,7 +23584,7 @@
         <v>328</v>
       </c>
       <c r="C85" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -23595,7 +23595,7 @@
         <v>329</v>
       </c>
       <c r="C86" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -23639,7 +23639,7 @@
         <v>39</v>
       </c>
       <c r="C90" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -23650,7 +23650,7 @@
         <v>43</v>
       </c>
       <c r="C91" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -23661,7 +23661,7 @@
         <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -23683,7 +23683,7 @@
         <v>41</v>
       </c>
       <c r="C94" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -23716,7 +23716,7 @@
         <v>273</v>
       </c>
       <c r="C97" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -23727,7 +23727,7 @@
         <v>47</v>
       </c>
       <c r="C98" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
@@ -23738,7 +23738,7 @@
         <v>207</v>
       </c>
       <c r="C99" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -23749,7 +23749,7 @@
         <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
@@ -23760,7 +23760,7 @@
         <v>179</v>
       </c>
       <c r="C101" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -23771,13 +23771,13 @@
         <v>180</v>
       </c>
       <c r="C102" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="G102" t="s">
         <v>55</v>
       </c>
       <c r="H102" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -23799,7 +23799,7 @@
         <v>378</v>
       </c>
       <c r="C104" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
@@ -23865,7 +23865,7 @@
         <v>347</v>
       </c>
       <c r="C110" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -23876,7 +23876,7 @@
         <v>348</v>
       </c>
       <c r="C111" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -23887,7 +23887,7 @@
         <v>416</v>
       </c>
       <c r="C112" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -23898,7 +23898,7 @@
         <v>196</v>
       </c>
       <c r="C113" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -23909,7 +23909,7 @@
         <v>201</v>
       </c>
       <c r="C114" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -23920,7 +23920,7 @@
         <v>414</v>
       </c>
       <c r="C115" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -23931,7 +23931,7 @@
         <v>198</v>
       </c>
       <c r="C116" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -23942,7 +23942,7 @@
         <v>197</v>
       </c>
       <c r="C117" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
@@ -23953,7 +23953,7 @@
         <v>293</v>
       </c>
       <c r="C118" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -23964,7 +23964,7 @@
         <v>200</v>
       </c>
       <c r="C119" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -24008,7 +24008,7 @@
         <v>280</v>
       </c>
       <c r="C123" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -24030,7 +24030,7 @@
         <v>54</v>
       </c>
       <c r="C125" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24041,7 +24041,7 @@
         <v>50</v>
       </c>
       <c r="C126" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24052,7 +24052,7 @@
         <v>234</v>
       </c>
       <c r="C127" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24063,7 +24063,7 @@
         <v>52</v>
       </c>
       <c r="C128" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
@@ -24074,7 +24074,7 @@
         <v>55</v>
       </c>
       <c r="C129" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
@@ -24085,7 +24085,7 @@
         <v>100</v>
       </c>
       <c r="C130" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
@@ -24096,7 +24096,7 @@
         <v>57</v>
       </c>
       <c r="C131" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
@@ -24107,7 +24107,7 @@
         <v>58</v>
       </c>
       <c r="C132" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
@@ -24118,7 +24118,7 @@
         <v>59</v>
       </c>
       <c r="C133" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
@@ -24129,7 +24129,7 @@
         <v>60</v>
       </c>
       <c r="C134" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
@@ -24140,7 +24140,7 @@
         <v>56</v>
       </c>
       <c r="C135" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
@@ -24151,7 +24151,7 @@
         <v>61</v>
       </c>
       <c r="C136" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
@@ -24173,7 +24173,7 @@
         <v>277</v>
       </c>
       <c r="C138" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
@@ -24184,7 +24184,7 @@
         <v>279</v>
       </c>
       <c r="C139" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
@@ -24206,7 +24206,7 @@
         <v>312</v>
       </c>
       <c r="C141" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
@@ -24217,7 +24217,7 @@
         <v>81</v>
       </c>
       <c r="C142" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
@@ -24228,7 +24228,7 @@
         <v>311</v>
       </c>
       <c r="C143" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -24239,7 +24239,7 @@
         <v>85</v>
       </c>
       <c r="C144" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
@@ -24250,7 +24250,7 @@
         <v>266</v>
       </c>
       <c r="C145" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
@@ -24261,7 +24261,7 @@
         <v>82</v>
       </c>
       <c r="C146" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
@@ -24272,7 +24272,7 @@
         <v>83</v>
       </c>
       <c r="C147" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
@@ -24283,7 +24283,7 @@
         <v>84</v>
       </c>
       <c r="C148" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -24294,7 +24294,7 @@
         <v>212</v>
       </c>
       <c r="C149" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
@@ -24305,7 +24305,7 @@
         <v>239</v>
       </c>
       <c r="C150" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -24316,7 +24316,7 @@
         <v>86</v>
       </c>
       <c r="C151" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
@@ -24327,7 +24327,7 @@
         <v>87</v>
       </c>
       <c r="C152" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
@@ -24338,7 +24338,7 @@
         <v>88</v>
       </c>
       <c r="C153" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
@@ -24349,7 +24349,7 @@
         <v>89</v>
       </c>
       <c r="C154" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
@@ -24371,7 +24371,7 @@
         <v>309</v>
       </c>
       <c r="C156" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
@@ -24382,7 +24382,7 @@
         <v>233</v>
       </c>
       <c r="C157" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
@@ -24404,7 +24404,7 @@
         <v>110</v>
       </c>
       <c r="C159" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
@@ -24415,7 +24415,7 @@
         <v>111</v>
       </c>
       <c r="C160" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -24426,7 +24426,7 @@
         <v>112</v>
       </c>
       <c r="C161" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -24437,7 +24437,7 @@
         <v>113</v>
       </c>
       <c r="C162" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -24448,7 +24448,7 @@
         <v>114</v>
       </c>
       <c r="C163" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -24459,7 +24459,7 @@
         <v>115</v>
       </c>
       <c r="C164" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -24470,7 +24470,7 @@
         <v>116</v>
       </c>
       <c r="C165" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -24481,7 +24481,7 @@
         <v>117</v>
       </c>
       <c r="C166" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -24503,7 +24503,7 @@
         <v>119</v>
       </c>
       <c r="C168" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -24525,7 +24525,7 @@
         <v>334</v>
       </c>
       <c r="C170" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -24536,7 +24536,7 @@
         <v>268</v>
       </c>
       <c r="C171" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -24547,7 +24547,7 @@
         <v>118</v>
       </c>
       <c r="C172" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -24558,7 +24558,7 @@
         <v>101</v>
       </c>
       <c r="C173" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -24569,7 +24569,7 @@
         <v>153</v>
       </c>
       <c r="C174" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -24580,7 +24580,7 @@
         <v>331</v>
       </c>
       <c r="C175" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -24591,7 +24591,7 @@
         <v>332</v>
       </c>
       <c r="C176" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -24602,7 +24602,7 @@
         <v>330</v>
       </c>
       <c r="C177" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -24613,7 +24613,7 @@
         <v>26</v>
       </c>
       <c r="C178" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -24624,7 +24624,7 @@
         <v>120</v>
       </c>
       <c r="C179" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -24635,7 +24635,7 @@
         <v>335</v>
       </c>
       <c r="C180" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -24668,10 +24668,10 @@
         <v>103</v>
       </c>
       <c r="C183" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D183" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -24682,7 +24682,7 @@
         <v>156</v>
       </c>
       <c r="C184" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -24693,7 +24693,7 @@
         <v>235</v>
       </c>
       <c r="C185" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -24704,7 +24704,7 @@
         <v>315</v>
       </c>
       <c r="C186" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -24715,7 +24715,7 @@
         <v>316</v>
       </c>
       <c r="C187" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -24726,7 +24726,7 @@
         <v>319</v>
       </c>
       <c r="C188" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -24737,7 +24737,7 @@
         <v>318</v>
       </c>
       <c r="C189" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -24748,7 +24748,7 @@
         <v>320</v>
       </c>
       <c r="C190" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -24770,7 +24770,7 @@
         <v>154</v>
       </c>
       <c r="C192" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -24781,7 +24781,7 @@
         <v>357</v>
       </c>
       <c r="C193" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -24792,7 +24792,7 @@
         <v>159</v>
       </c>
       <c r="C194" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -24803,10 +24803,10 @@
         <v>158</v>
       </c>
       <c r="C195" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="D195" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -24817,7 +24817,7 @@
         <v>231</v>
       </c>
       <c r="C196" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -24828,7 +24828,7 @@
         <v>358</v>
       </c>
       <c r="C197" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
@@ -24839,7 +24839,7 @@
         <v>155</v>
       </c>
       <c r="C198" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -24850,7 +24850,7 @@
         <v>359</v>
       </c>
       <c r="C199" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -24861,7 +24861,7 @@
         <v>157</v>
       </c>
       <c r="C200" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -24872,7 +24872,7 @@
         <v>356</v>
       </c>
       <c r="C201" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -24883,7 +24883,7 @@
         <v>184</v>
       </c>
       <c r="C202" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -24894,7 +24894,7 @@
         <v>185</v>
       </c>
       <c r="C203" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -24905,7 +24905,7 @@
         <v>186</v>
       </c>
       <c r="C204" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
@@ -24916,7 +24916,7 @@
         <v>187</v>
       </c>
       <c r="C205" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -24927,7 +24927,7 @@
         <v>188</v>
       </c>
       <c r="C206" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
@@ -24938,7 +24938,7 @@
         <v>208</v>
       </c>
       <c r="C207" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -24993,7 +24993,7 @@
         <v>72</v>
       </c>
       <c r="C212" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
@@ -25004,7 +25004,7 @@
         <v>74</v>
       </c>
       <c r="C213" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
@@ -25015,7 +25015,7 @@
         <v>210</v>
       </c>
       <c r="C214" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
@@ -25026,7 +25026,7 @@
         <v>294</v>
       </c>
       <c r="C215" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
@@ -25037,7 +25037,7 @@
         <v>295</v>
       </c>
       <c r="C216" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
@@ -25048,7 +25048,7 @@
         <v>296</v>
       </c>
       <c r="C217" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
@@ -25059,7 +25059,7 @@
         <v>297</v>
       </c>
       <c r="C218" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
@@ -25081,7 +25081,7 @@
         <v>299</v>
       </c>
       <c r="C220" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
@@ -25092,7 +25092,7 @@
         <v>301</v>
       </c>
       <c r="C221" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
@@ -25114,7 +25114,7 @@
         <v>437</v>
       </c>
       <c r="C223" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
@@ -25125,7 +25125,7 @@
         <v>438</v>
       </c>
       <c r="C224" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -25147,7 +25147,7 @@
         <v>35</v>
       </c>
       <c r="C226" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
@@ -25158,7 +25158,7 @@
         <v>36</v>
       </c>
       <c r="C227" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -25180,7 +25180,7 @@
         <v>209</v>
       </c>
       <c r="C229" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -25191,7 +25191,7 @@
         <v>269</v>
       </c>
       <c r="C230" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -25202,7 +25202,7 @@
         <v>270</v>
       </c>
       <c r="C231" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -25213,7 +25213,7 @@
         <v>271</v>
       </c>
       <c r="C232" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -25235,7 +25235,7 @@
         <v>342</v>
       </c>
       <c r="C234" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -25246,7 +25246,7 @@
         <v>344</v>
       </c>
       <c r="C235" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -25257,7 +25257,7 @@
         <v>242</v>
       </c>
       <c r="C236" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -25268,7 +25268,7 @@
         <v>274</v>
       </c>
       <c r="C237" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -25279,7 +25279,7 @@
         <v>195</v>
       </c>
       <c r="C238" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -25290,7 +25290,7 @@
         <v>131</v>
       </c>
       <c r="C239" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -25301,7 +25301,7 @@
         <v>235</v>
       </c>
       <c r="C240" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -25312,7 +25312,7 @@
         <v>192</v>
       </c>
       <c r="C241" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -25323,7 +25323,7 @@
         <v>439</v>
       </c>
       <c r="C242" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -25334,7 +25334,7 @@
         <v>194</v>
       </c>
       <c r="C243" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -25345,7 +25345,7 @@
         <v>393</v>
       </c>
       <c r="C244" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
@@ -25356,7 +25356,7 @@
         <v>394</v>
       </c>
       <c r="C245" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -25367,7 +25367,7 @@
         <v>396</v>
       </c>
       <c r="C246" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
@@ -25378,7 +25378,7 @@
         <v>397</v>
       </c>
       <c r="C247" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -25389,7 +25389,7 @@
         <v>238</v>
       </c>
       <c r="C248" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -25411,10 +25411,10 @@
         <v>7</v>
       </c>
       <c r="C250" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D250" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -25425,10 +25425,10 @@
         <v>8</v>
       </c>
       <c r="C251" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D251" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
@@ -25439,10 +25439,10 @@
         <v>9</v>
       </c>
       <c r="C252" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D252" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -25453,10 +25453,10 @@
         <v>10</v>
       </c>
       <c r="C253" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D253" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
@@ -25467,10 +25467,10 @@
         <v>11</v>
       </c>
       <c r="C254" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D254" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -25481,7 +25481,7 @@
         <v>73</v>
       </c>
       <c r="C255" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -25525,7 +25525,7 @@
         <v>137</v>
       </c>
       <c r="C259" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -25536,7 +25536,7 @@
         <v>418</v>
       </c>
       <c r="C260" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -25547,7 +25547,7 @@
         <v>419</v>
       </c>
       <c r="C261" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -25558,7 +25558,7 @@
         <v>420</v>
       </c>
       <c r="C262" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -25569,7 +25569,7 @@
         <v>421</v>
       </c>
       <c r="C263" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
@@ -25580,7 +25580,7 @@
         <v>417</v>
       </c>
       <c r="C264" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -25591,7 +25591,7 @@
         <v>145</v>
       </c>
       <c r="C265" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -25602,7 +25602,7 @@
         <v>349</v>
       </c>
       <c r="C266" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -25613,7 +25613,7 @@
         <v>351</v>
       </c>
       <c r="C267" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -25624,7 +25624,7 @@
         <v>352</v>
       </c>
       <c r="C268" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -25635,7 +25635,7 @@
         <v>350</v>
       </c>
       <c r="C269" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
@@ -25646,7 +25646,7 @@
         <v>408</v>
       </c>
       <c r="C270" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -25657,7 +25657,7 @@
         <v>143</v>
       </c>
       <c r="C271" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -25701,7 +25701,7 @@
         <v>353</v>
       </c>
       <c r="C275" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -25747,7 +25747,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="B3">
         <v>5235</v>
@@ -25767,13 +25767,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="B4">
         <v>3621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D4">
         <v>1230</v>
@@ -25787,7 +25787,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="B5">
         <v>3412</v>
@@ -25802,7 +25802,7 @@
         <v>1977</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
   </sheetData>
@@ -25839,84 +25839,84 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B2" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C2" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B4" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C4" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B5" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C5" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C7" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B8" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C8" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B9" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clock: Repeating Tick Sound (script-18)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="653">
   <si>
     <t>Purpose</t>
   </si>
@@ -1991,6 +1991,9 @@
   </si>
   <si>
     <t>Telescope: Alien shown</t>
+  </si>
+  <si>
+    <t>Clock Tick</t>
   </si>
 </sst>
 </file>
@@ -3300,7 +3303,7 @@
   <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21499,8 +21502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F87" sqref="F87"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22553,10 +22556,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22698,6 +22701,14 @@
       </c>
       <c r="B17" t="s">
         <v>645</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>652</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Phone: Disconnect if Kid walks too far away (script-28)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="733">
   <si>
     <t>Purpose</t>
   </si>
@@ -2222,6 +2222,18 @@
   </si>
   <si>
     <t>Gravy Stain</t>
+  </si>
+  <si>
+    <t>Library Phone Ring</t>
+  </si>
+  <si>
+    <t>Ednas Phone Ring</t>
+  </si>
+  <si>
+    <t>Library Phone Busy</t>
+  </si>
+  <si>
+    <t>08 = On Hook</t>
   </si>
 </sst>
 </file>
@@ -2777,8 +2789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3540,7 +3552,7 @@
   <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21737,10 +21749,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21754,7 +21766,7 @@
     <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -21774,1021 +21786,1029 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
+        <v>338</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>69</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F4" t="s">
+        <v>294</v>
+      </c>
+      <c r="G4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H4" t="s">
+        <v>291</v>
+      </c>
+      <c r="I4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>70</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="C5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
+      </c>
+      <c r="F5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>71</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>513</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>72</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>624</v>
+      </c>
+      <c r="F7" t="s">
+        <v>625</v>
+      </c>
+      <c r="G7" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>81</v>
-      </c>
-      <c r="B8" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>330</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>127</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="C10" t="s">
+        <v>640</v>
+      </c>
+      <c r="E10" t="s">
+        <v>641</v>
+      </c>
+      <c r="F10" t="s">
+        <v>642</v>
+      </c>
+      <c r="G10" t="s">
+        <v>643</v>
+      </c>
+      <c r="H10" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>22</v>
       </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>73</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F10" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
       <c r="C11" t="s">
-        <v>75</v>
-      </c>
-      <c r="D11" t="s">
-        <v>73</v>
+        <v>247</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>239</v>
       </c>
       <c r="F11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>667</v>
+      </c>
+      <c r="G11" t="s">
+        <v>251</v>
+      </c>
+      <c r="H11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>103</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>76</v>
+        <v>277</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="F12" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>514</v>
+        <v>249</v>
       </c>
       <c r="E13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F13" t="s">
+        <v>667</v>
+      </c>
+      <c r="G13" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>645</v>
+      </c>
+      <c r="E14" t="s">
         <v>227</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="E15" t="s">
+        <v>239</v>
+      </c>
+      <c r="F15" t="s">
+        <v>667</v>
+      </c>
+      <c r="G15" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>513</v>
-      </c>
-      <c r="D16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>630</v>
+      </c>
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+      <c r="F16" t="s">
+        <v>631</v>
+      </c>
+      <c r="G16" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>91</v>
-      </c>
-      <c r="D18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>90</v>
-      </c>
-      <c r="D19" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>97</v>
+        <v>35</v>
       </c>
       <c r="C20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="C22" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="C23" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>92</v>
-      </c>
-      <c r="B24" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>90</v>
-      </c>
-      <c r="B26" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="C26" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>20</v>
-      </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="C27" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>37</v>
-      </c>
-      <c r="C33" t="s">
-        <v>155</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>156</v>
+        <v>124</v>
+      </c>
+      <c r="D34" t="s">
+        <v>647</v>
+      </c>
+      <c r="E34" t="s">
+        <v>125</v>
+      </c>
+      <c r="F34" t="s">
+        <v>128</v>
+      </c>
+      <c r="G34" t="s">
+        <v>127</v>
+      </c>
+      <c r="H34" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>39</v>
+        <v>54</v>
+      </c>
+      <c r="B35" t="s">
+        <v>7</v>
       </c>
       <c r="C35" t="s">
-        <v>157</v>
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>281</v>
+        <v>312</v>
+      </c>
+      <c r="E36" t="s">
+        <v>313</v>
+      </c>
+      <c r="F36" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>282</v>
+        <v>181</v>
+      </c>
+      <c r="E37" t="s">
+        <v>182</v>
+      </c>
+      <c r="F37" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" t="s">
+        <v>184</v>
+      </c>
+      <c r="H37" t="s">
+        <v>185</v>
+      </c>
+      <c r="I37" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>283</v>
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>43</v>
+        <v>59</v>
       </c>
       <c r="C39" t="s">
-        <v>284</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C40" t="s">
-        <v>181</v>
-      </c>
-      <c r="E40" t="s">
-        <v>182</v>
-      </c>
-      <c r="F40" t="s">
-        <v>183</v>
-      </c>
-      <c r="G40" t="s">
-        <v>184</v>
-      </c>
-      <c r="H40" t="s">
-        <v>185</v>
-      </c>
-      <c r="I40" t="s">
-        <v>186</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>59</v>
-      </c>
-      <c r="C42" t="s">
-        <v>166</v>
+      <c r="A42" s="2">
+        <v>62</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>259</v>
+      </c>
+      <c r="E43" t="s">
+        <v>239</v>
+      </c>
+      <c r="F43" t="s">
+        <v>260</v>
+      </c>
+      <c r="G43" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>252</v>
+      </c>
+      <c r="E44" t="s">
+        <v>227</v>
+      </c>
+      <c r="F44" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="C45" t="s">
-        <v>124</v>
-      </c>
-      <c r="D45" t="s">
-        <v>647</v>
+        <v>212</v>
       </c>
       <c r="E45" t="s">
-        <v>125</v>
+        <v>239</v>
       </c>
       <c r="F45" t="s">
-        <v>128</v>
+        <v>429</v>
       </c>
       <c r="G45" t="s">
-        <v>127</v>
+        <v>240</v>
       </c>
       <c r="H45" t="s">
-        <v>126</v>
+        <v>241</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>106</v>
-      </c>
-      <c r="B46" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
-      </c>
-      <c r="E46" t="s">
-        <v>131</v>
+        <v>582</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>105</v>
+        <v>68</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
+        <v>25</v>
+      </c>
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>16</v>
+        <v>69</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
-      </c>
-      <c r="C48" t="s">
-        <v>140</v>
-      </c>
-      <c r="E48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F48" t="s">
-        <v>142</v>
-      </c>
-      <c r="G48" t="s">
-        <v>143</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>44</v>
-      </c>
-      <c r="C49" t="s">
-        <v>158</v>
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>45</v>
-      </c>
-      <c r="C50" t="s">
-        <v>161</v>
+        <v>71</v>
+      </c>
+      <c r="B50" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>46</v>
-      </c>
-      <c r="C51" t="s">
-        <v>160</v>
+        <v>72</v>
+      </c>
+      <c r="B51" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>47</v>
+        <v>73</v>
+      </c>
+      <c r="B52" t="s">
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>159</v>
+        <v>66</v>
+      </c>
+      <c r="E52" t="s">
+        <v>67</v>
+      </c>
+      <c r="F52" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>486</v>
       </c>
       <c r="E53" t="s">
-        <v>213</v>
-      </c>
-      <c r="F53" t="s">
-        <v>214</v>
-      </c>
-      <c r="G53" t="s">
-        <v>215</v>
-      </c>
-      <c r="H53" t="s">
-        <v>299</v>
-      </c>
-      <c r="I53" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C54" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E54" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F54" t="s">
-        <v>221</v>
+        <v>214</v>
+      </c>
+      <c r="G54" t="s">
+        <v>215</v>
+      </c>
+      <c r="H54" t="s">
+        <v>299</v>
+      </c>
+      <c r="I54" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="C55" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="E55" t="s">
+        <v>220</v>
+      </c>
+      <c r="F55" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>79</v>
+      </c>
+      <c r="C56" t="s">
+        <v>347</v>
+      </c>
+      <c r="E56" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>80</v>
+      </c>
+      <c r="C57" t="s">
+        <v>349</v>
+      </c>
+      <c r="E57" t="s">
         <v>227</v>
       </c>
-      <c r="F55" t="s">
+      <c r="F57" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>66</v>
-      </c>
-      <c r="C56" t="s">
-        <v>212</v>
-      </c>
-      <c r="E56" t="s">
-        <v>239</v>
-      </c>
-      <c r="F56" t="s">
-        <v>429</v>
-      </c>
-      <c r="G56" t="s">
-        <v>240</v>
-      </c>
-      <c r="H56" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>11</v>
-      </c>
-      <c r="C57" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>27</v>
+        <v>81</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>257</v>
+        <v>59</v>
       </c>
       <c r="E58" t="s">
-        <v>239</v>
-      </c>
-      <c r="F58" t="s">
-        <v>667</v>
-      </c>
-      <c r="G58" t="s">
-        <v>251</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>22</v>
+        <v>82</v>
       </c>
       <c r="C59" t="s">
-        <v>247</v>
+        <v>581</v>
       </c>
       <c r="E59" t="s">
-        <v>239</v>
+        <v>302</v>
       </c>
       <c r="F59" t="s">
-        <v>667</v>
+        <v>300</v>
       </c>
       <c r="G59" t="s">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="H59" t="s">
-        <v>460</v>
+        <v>602</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>24</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
-        <v>249</v>
-      </c>
-      <c r="E60" t="s">
-        <v>239</v>
-      </c>
-      <c r="F60" t="s">
-        <v>667</v>
-      </c>
-      <c r="G60" t="s">
-        <v>251</v>
+        <v>583</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>64</v>
+        <v>84</v>
       </c>
       <c r="C61" t="s">
-        <v>252</v>
+        <v>413</v>
       </c>
       <c r="E61" t="s">
         <v>227</v>
       </c>
       <c r="F61" t="s">
-        <v>228</v>
+        <v>414</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>12</v>
-      </c>
-      <c r="C62" t="s">
-        <v>338</v>
-      </c>
-      <c r="E62" t="s">
-        <v>255</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>63</v>
-      </c>
-      <c r="C63" t="s">
-        <v>259</v>
-      </c>
-      <c r="E63" t="s">
-        <v>239</v>
-      </c>
-      <c r="F63" t="s">
-        <v>260</v>
-      </c>
-      <c r="G63" t="s">
-        <v>261</v>
+        <v>90</v>
+      </c>
+      <c r="D63" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>23</v>
+        <v>90</v>
+      </c>
+      <c r="B64" t="s">
+        <v>7</v>
       </c>
       <c r="C64" t="s">
-        <v>277</v>
-      </c>
-      <c r="E64" t="s">
-        <v>276</v>
-      </c>
-      <c r="F64" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>13</v>
-      </c>
-      <c r="C65" t="s">
-        <v>288</v>
-      </c>
-      <c r="E65" t="s">
-        <v>289</v>
-      </c>
-      <c r="F65" t="s">
-        <v>294</v>
-      </c>
-      <c r="G65" t="s">
-        <v>290</v>
-      </c>
-      <c r="H65" t="s">
-        <v>291</v>
-      </c>
-      <c r="I65" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="D65" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>82</v>
+        <v>91</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>581</v>
-      </c>
-      <c r="E66" t="s">
-        <v>302</v>
-      </c>
-      <c r="F66" t="s">
-        <v>300</v>
-      </c>
-      <c r="G66" t="s">
-        <v>301</v>
-      </c>
-      <c r="H66" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D66" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>56</v>
+        <v>92</v>
+      </c>
+      <c r="B67" t="s">
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>312</v>
-      </c>
-      <c r="E67" t="s">
-        <v>313</v>
-      </c>
-      <c r="F67" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D67" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="C68" t="s">
-        <v>624</v>
+        <v>226</v>
+      </c>
+      <c r="E68" t="s">
+        <v>227</v>
       </c>
       <c r="F68" t="s">
-        <v>625</v>
-      </c>
-      <c r="G68" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="C69" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>67</v>
+        <v>98</v>
       </c>
       <c r="C70" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
+        <v>99</v>
+      </c>
+      <c r="C71" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>103</v>
+      </c>
+      <c r="B72" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" t="s">
+        <v>77</v>
+      </c>
+      <c r="D72" t="s">
+        <v>76</v>
+      </c>
+      <c r="E72" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>105</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>106</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>132</v>
+      </c>
+      <c r="E74" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>108</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C75" t="s">
         <v>326</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E75" t="s">
         <v>322</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F75" t="s">
         <v>323</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G75" t="s">
         <v>324</v>
       </c>
-      <c r="H71" t="s">
+      <c r="H75" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>19</v>
-      </c>
-      <c r="C74" t="s">
-        <v>330</v>
-      </c>
-      <c r="E74" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>79</v>
-      </c>
-      <c r="C75" t="s">
-        <v>347</v>
-      </c>
-      <c r="E75" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>80</v>
-      </c>
-      <c r="C76" t="s">
-        <v>349</v>
-      </c>
-      <c r="E76" t="s">
-        <v>227</v>
-      </c>
-      <c r="F76" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>413</v>
+        <v>514</v>
       </c>
       <c r="E77" t="s">
         <v>227</v>
       </c>
       <c r="F77" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>122</v>
+      </c>
+      <c r="B81" t="s">
+        <v>6</v>
+      </c>
+      <c r="C81" t="s">
         <v>75</v>
       </c>
-      <c r="C78" t="s">
-        <v>486</v>
-      </c>
-      <c r="E78" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>83</v>
-      </c>
-      <c r="C79" t="s">
-        <v>583</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>137</v>
-      </c>
-      <c r="C80" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81">
-        <v>136</v>
-      </c>
-      <c r="C81" t="s">
-        <v>623</v>
+      <c r="D81" t="s">
+        <v>73</v>
       </c>
       <c r="E81" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F81" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>126</v>
       </c>
-      <c r="C82" t="s">
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>126</v>
+      </c>
+      <c r="C83" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83">
-        <v>31</v>
-      </c>
-      <c r="C83" t="s">
-        <v>630</v>
-      </c>
-      <c r="E83" t="s">
-        <v>227</v>
-      </c>
-      <c r="F83" t="s">
-        <v>631</v>
-      </c>
-      <c r="G83" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
+        <v>127</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
+      </c>
+      <c r="C84" t="s">
+        <v>20</v>
+      </c>
+      <c r="D84" t="s">
+        <v>22</v>
+      </c>
+      <c r="E84" t="s">
+        <v>21</v>
+      </c>
+      <c r="F84" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>135</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C85" t="s">
         <v>636</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85">
-        <v>20</v>
-      </c>
-      <c r="C85" t="s">
-        <v>640</v>
-      </c>
-      <c r="E85" t="s">
-        <v>641</v>
-      </c>
-      <c r="F85" t="s">
-        <v>642</v>
-      </c>
-      <c r="G85" t="s">
-        <v>643</v>
-      </c>
-      <c r="H85" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>25</v>
+        <v>136</v>
       </c>
       <c r="C86" t="s">
-        <v>645</v>
+        <v>623</v>
       </c>
       <c r="E86" t="s">
-        <v>227</v>
-      </c>
-      <c r="F86" t="s">
         <v>228</v>
       </c>
     </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>137</v>
+      </c>
+      <c r="C87" t="s">
+        <v>593</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A2:I86">
+    <sortCondition ref="A2:A86"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -22796,15 +22816,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -22817,82 +22837,82 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>594</v>
+        <v>605</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>598</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>597</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>601</v>
+        <v>639</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>605</v>
+        <v>648</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>606</v>
+        <v>634</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -22905,61 +22925,88 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>618</v>
+        <v>577</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>62</v>
+        <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>594</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>577</v>
+        <v>596</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>634</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>639</v>
+        <v>603</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>28</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
-        <v>648</v>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>731</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B19">
+    <sortCondition ref="A2:A19"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22968,8 +23015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" workbookViewId="0">
-      <selection activeCell="C194" sqref="C194"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23540,7 +23587,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>4</v>
       </c>
@@ -23551,7 +23598,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>4</v>
       </c>
@@ -23562,7 +23609,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>4</v>
       </c>
@@ -23573,7 +23620,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>4</v>
       </c>
@@ -23584,7 +23631,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>4</v>
       </c>
@@ -23595,7 +23642,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>4</v>
       </c>
@@ -23606,7 +23653,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>5</v>
       </c>
@@ -23617,7 +23664,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>5</v>
       </c>
@@ -23628,7 +23675,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>5</v>
       </c>
@@ -23641,8 +23688,11 @@
       <c r="D57" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>5</v>
       </c>
@@ -23653,7 +23703,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>5</v>
       </c>
@@ -23664,7 +23714,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>5</v>
       </c>
@@ -23675,7 +23725,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>5</v>
       </c>
@@ -23686,7 +23736,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>5</v>
       </c>
@@ -23697,7 +23747,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>5</v>
       </c>
@@ -23708,7 +23758,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>5</v>
       </c>
@@ -27936,7 +27986,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cutscene: Edna: Prank Phone Call (script-29)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="5"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1234" uniqueCount="733">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="738">
   <si>
     <t>Purpose</t>
   </si>
@@ -2234,6 +2234,21 @@
   </si>
   <si>
     <t>08 = On Hook</t>
+  </si>
+  <si>
+    <t>1 = Disabled</t>
+  </si>
+  <si>
+    <t>0 = Enabled</t>
+  </si>
+  <si>
+    <t>08 = Off Hook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 = </t>
+  </si>
+  <si>
+    <t>Nurse Edna Called on Phone</t>
   </si>
 </sst>
 </file>
@@ -2565,7 +2580,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,7 +3567,7 @@
   <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21749,10 +21764,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21861,6 +21876,12 @@
       <c r="D6" t="s">
         <v>84</v>
       </c>
+      <c r="E6" t="s">
+        <v>734</v>
+      </c>
+      <c r="F6" t="s">
+        <v>733</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -22186,184 +22207,190 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>312</v>
+        <v>737</v>
       </c>
       <c r="E36" t="s">
-        <v>313</v>
+        <v>227</v>
       </c>
       <c r="F36" t="s">
-        <v>314</v>
+        <v>228</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>312</v>
       </c>
       <c r="E37" t="s">
-        <v>182</v>
+        <v>313</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
-      </c>
-      <c r="G37" t="s">
-        <v>184</v>
-      </c>
-      <c r="H37" t="s">
-        <v>185</v>
-      </c>
-      <c r="I37" t="s">
-        <v>186</v>
+        <v>314</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>181</v>
+      </c>
+      <c r="E38" t="s">
+        <v>182</v>
+      </c>
+      <c r="F38" t="s">
+        <v>183</v>
+      </c>
+      <c r="G38" t="s">
+        <v>184</v>
+      </c>
+      <c r="H38" t="s">
+        <v>185</v>
+      </c>
+      <c r="I38" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42">
         <v>61</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>62</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D42" s="1"/>
-      <c r="E42" t="s">
+      <c r="D43" s="1"/>
+      <c r="E43" t="s">
         <v>61</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F43" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G43" s="2" t="s">
         <v>258</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>63</v>
-      </c>
-      <c r="C43" t="s">
-        <v>259</v>
-      </c>
-      <c r="E43" t="s">
-        <v>239</v>
-      </c>
-      <c r="F43" t="s">
-        <v>260</v>
-      </c>
-      <c r="G43" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="E44" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="F44" t="s">
-        <v>228</v>
+        <v>260</v>
+      </c>
+      <c r="G44" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
-        <v>212</v>
+        <v>252</v>
       </c>
       <c r="E45" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="F45" t="s">
-        <v>429</v>
-      </c>
-      <c r="G45" t="s">
-        <v>240</v>
-      </c>
-      <c r="H45" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
-        <v>582</v>
+        <v>212</v>
+      </c>
+      <c r="E46" t="s">
+        <v>239</v>
+      </c>
+      <c r="F46" t="s">
+        <v>429</v>
+      </c>
+      <c r="G46" t="s">
+        <v>240</v>
+      </c>
+      <c r="H46" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>68</v>
-      </c>
-      <c r="B47" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
-      </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" t="s">
-        <v>27</v>
+        <v>582</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D48" t="s">
+        <v>22</v>
+      </c>
+      <c r="E48" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
@@ -22371,7 +22398,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -22379,7 +22406,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -22387,160 +22414,160 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
       </c>
-      <c r="C52" t="s">
-        <v>66</v>
-      </c>
-      <c r="E52" t="s">
-        <v>67</v>
-      </c>
-      <c r="F52" t="s">
-        <v>271</v>
-      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>75</v>
+        <v>73</v>
+      </c>
+      <c r="B53" t="s">
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>486</v>
+        <v>66</v>
       </c>
       <c r="E53" t="s">
-        <v>294</v>
+        <v>67</v>
+      </c>
+      <c r="F53" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>486</v>
       </c>
       <c r="E54" t="s">
-        <v>213</v>
-      </c>
-      <c r="F54" t="s">
-        <v>214</v>
-      </c>
-      <c r="G54" t="s">
-        <v>215</v>
-      </c>
-      <c r="H54" t="s">
-        <v>299</v>
-      </c>
-      <c r="I54" t="s">
-        <v>216</v>
+        <v>294</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C55" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E55" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F55" t="s">
-        <v>221</v>
+        <v>214</v>
+      </c>
+      <c r="G55" t="s">
+        <v>215</v>
+      </c>
+      <c r="H55" t="s">
+        <v>299</v>
+      </c>
+      <c r="I55" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
+        <v>78</v>
+      </c>
+      <c r="C56" t="s">
+        <v>219</v>
+      </c>
+      <c r="E56" t="s">
+        <v>220</v>
+      </c>
+      <c r="F56" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57">
         <v>79</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>347</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E57" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57">
+    <row r="58" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>80</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>349</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>227</v>
       </c>
-      <c r="F57" t="s">
+      <c r="F58" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>81</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58" t="s">
-        <v>59</v>
-      </c>
-      <c r="E58" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>581</v>
+        <v>59</v>
       </c>
       <c r="E59" t="s">
-        <v>302</v>
-      </c>
-      <c r="F59" t="s">
-        <v>300</v>
-      </c>
-      <c r="G59" t="s">
-        <v>301</v>
-      </c>
-      <c r="H59" t="s">
-        <v>602</v>
+        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>583</v>
+        <v>581</v>
+      </c>
+      <c r="E60" t="s">
+        <v>302</v>
+      </c>
+      <c r="F60" t="s">
+        <v>300</v>
+      </c>
+      <c r="G60" t="s">
+        <v>301</v>
+      </c>
+      <c r="H60" t="s">
+        <v>602</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>413</v>
-      </c>
-      <c r="E61" t="s">
-        <v>227</v>
-      </c>
-      <c r="F61" t="s">
-        <v>414</v>
+        <v>583</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="C62" t="s">
+        <v>413</v>
+      </c>
+      <c r="E62" t="s">
+        <v>227</v>
+      </c>
+      <c r="F62" t="s">
+        <v>414</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>90</v>
-      </c>
-      <c r="D63" t="s">
         <v>89</v>
       </c>
     </row>
@@ -22548,44 +22575,38 @@
       <c r="A64">
         <v>90</v>
       </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
-        <v>106</v>
+      <c r="D64" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>91</v>
-      </c>
-      <c r="D65" t="s">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>91</v>
       </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66" t="s">
-        <v>105</v>
-      </c>
       <c r="D66" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
         <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D67" t="s">
         <v>92</v>
@@ -22593,215 +22614,229 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="B68" t="s">
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>226</v>
-      </c>
-      <c r="E68" t="s">
-        <v>227</v>
-      </c>
-      <c r="F68" t="s">
-        <v>228</v>
+        <v>107</v>
+      </c>
+      <c r="D68" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C69" t="s">
-        <v>109</v>
+        <v>226</v>
+      </c>
+      <c r="E69" t="s">
+        <v>227</v>
+      </c>
+      <c r="F69" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C70" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>103</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6</v>
+        <v>99</v>
       </c>
       <c r="C72" t="s">
-        <v>77</v>
-      </c>
-      <c r="D72" t="s">
-        <v>76</v>
-      </c>
-      <c r="E72" t="s">
-        <v>78</v>
+        <v>111</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>133</v>
+        <v>77</v>
+      </c>
+      <c r="D73" t="s">
+        <v>76</v>
+      </c>
+      <c r="E73" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>132</v>
-      </c>
-      <c r="E74" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>326</v>
+        <v>132</v>
       </c>
       <c r="E75" t="s">
-        <v>322</v>
-      </c>
-      <c r="F75" t="s">
-        <v>323</v>
-      </c>
-      <c r="G75" t="s">
-        <v>324</v>
-      </c>
-      <c r="H75" t="s">
-        <v>325</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C76" t="s">
+        <v>326</v>
+      </c>
+      <c r="E76" t="s">
+        <v>322</v>
+      </c>
+      <c r="F76" t="s">
+        <v>323</v>
+      </c>
+      <c r="G76" t="s">
+        <v>324</v>
+      </c>
+      <c r="H76" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>110</v>
-      </c>
-      <c r="C77" t="s">
-        <v>514</v>
-      </c>
-      <c r="E77" t="s">
-        <v>227</v>
-      </c>
-      <c r="F77" t="s">
-        <v>228</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C78" t="s">
+        <v>514</v>
+      </c>
+      <c r="E78" t="s">
+        <v>227</v>
+      </c>
+      <c r="F78" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>122</v>
-      </c>
-      <c r="B81" t="s">
-        <v>6</v>
-      </c>
-      <c r="C81" t="s">
-        <v>75</v>
-      </c>
-      <c r="D81" t="s">
-        <v>73</v>
-      </c>
-      <c r="E81" t="s">
-        <v>71</v>
-      </c>
-      <c r="F81" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B82" t="s">
+        <v>6</v>
+      </c>
+      <c r="C82" t="s">
+        <v>75</v>
+      </c>
+      <c r="D82" t="s">
+        <v>73</v>
+      </c>
+      <c r="E82" t="s">
+        <v>71</v>
+      </c>
+      <c r="F82" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>126</v>
       </c>
-      <c r="C83" t="s">
-        <v>629</v>
-      </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>127</v>
-      </c>
-      <c r="B84" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" t="s">
-        <v>22</v>
-      </c>
-      <c r="E84" t="s">
-        <v>21</v>
-      </c>
-      <c r="F84" t="s">
-        <v>26</v>
+        <v>629</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="B85" t="s">
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>636</v>
+        <v>20</v>
+      </c>
+      <c r="D85" t="s">
+        <v>22</v>
+      </c>
+      <c r="E85" t="s">
+        <v>21</v>
+      </c>
+      <c r="F85" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>623</v>
-      </c>
-      <c r="E86" t="s">
-        <v>228</v>
+        <v>636</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
+        <v>136</v>
+      </c>
+      <c r="C87" t="s">
+        <v>623</v>
+      </c>
+      <c r="E87" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88">
         <v>137</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C88" t="s">
         <v>593</v>
       </c>
     </row>
@@ -23015,8 +23050,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView topLeftCell="A201" workbookViewId="0">
+      <selection activeCell="D216" sqref="D216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25371,7 +25406,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>18</v>
       </c>
@@ -25382,7 +25417,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>18</v>
       </c>
@@ -25393,7 +25428,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>18</v>
       </c>
@@ -25404,7 +25439,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>18</v>
       </c>
@@ -25415,7 +25450,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>18</v>
       </c>
@@ -25426,7 +25461,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>18</v>
       </c>
@@ -25437,7 +25472,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>19</v>
       </c>
@@ -25448,7 +25483,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>19</v>
       </c>
@@ -25458,8 +25493,14 @@
       <c r="C216" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D216" t="s">
+        <v>736</v>
+      </c>
+      <c r="E216" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>19</v>
       </c>
@@ -25470,7 +25511,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>19</v>
       </c>
@@ -25481,7 +25522,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>19</v>
       </c>
@@ -25492,7 +25533,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>19</v>
       </c>
@@ -25503,7 +25544,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>19</v>
       </c>
@@ -25514,7 +25555,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>19</v>
       </c>
@@ -25525,7 +25566,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>19</v>
       </c>
@@ -25536,7 +25577,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Nurse Edna: Check for close actors (script-30)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="740">
   <si>
     <t>Purpose</t>
   </si>
@@ -2249,6 +2249,12 @@
   </si>
   <si>
     <t>Nurse Edna Called on Phone</t>
+  </si>
+  <si>
+    <t>2 = Returning To Room</t>
+  </si>
+  <si>
+    <t>1 = In Room</t>
   </si>
 </sst>
 </file>
@@ -2805,7 +2811,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3566,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21766,8 +21772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22679,6 +22685,12 @@
       </c>
       <c r="E73" t="s">
         <v>78</v>
+      </c>
+      <c r="F73" t="s">
+        <v>739</v>
+      </c>
+      <c r="G73" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pin: Entry - Radio (Meteor Police) (script-35)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="740">
   <si>
     <t>Purpose</t>
   </si>
@@ -3573,7 +3573,7 @@
   <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21772,8 +21772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22172,6 +22172,9 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>48</v>
+      </c>
+      <c r="C33" t="s">
+        <v>574</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cutscene: Meteor Police (script-36)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -967,9 +967,6 @@
     <t>Talk Show:  Talking to Meteor</t>
   </si>
   <si>
-    <t>Meteor Police Called</t>
-  </si>
-  <si>
     <t>0 = Not Called</t>
   </si>
   <si>
@@ -2255,6 +2252,9 @@
   </si>
   <si>
     <t>Nurse Edna: Waiting</t>
+  </si>
+  <si>
+    <t>Meteor Police Called Count</t>
   </si>
 </sst>
 </file>
@@ -2586,7 +2586,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2811,7 +2811,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2828,10 +2828,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>520</v>
+      </c>
+      <c r="D1" t="s">
         <v>521</v>
-      </c>
-      <c r="D1" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2839,7 +2839,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2853,7 +2853,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2867,7 +2867,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2881,7 +2881,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2895,13 +2895,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,7 +2909,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -2923,7 +2923,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -2937,7 +2937,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -2951,7 +2951,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -2965,7 +2965,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -2979,7 +2979,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -2993,7 +2993,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -3007,7 +3007,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -3021,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -3035,7 +3035,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -3049,7 +3049,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -3063,7 +3063,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -3077,7 +3077,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -3091,7 +3091,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -3105,7 +3105,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -3133,7 +3133,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -3147,7 +3147,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -3161,7 +3161,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -3175,7 +3175,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -3189,7 +3189,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -3203,7 +3203,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -3217,7 +3217,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -3231,7 +3231,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3245,7 +3245,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -3259,7 +3259,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -3273,7 +3273,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3287,7 +3287,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3301,7 +3301,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3315,7 +3315,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3329,7 +3329,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -3343,7 +3343,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -3357,7 +3357,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -3371,7 +3371,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3385,7 +3385,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -3399,7 +3399,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3413,7 +3413,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3427,7 +3427,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -3441,7 +3441,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3455,7 +3455,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3469,7 +3469,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3483,7 +3483,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3497,7 +3497,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3511,7 +3511,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -3525,7 +3525,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3539,7 +3539,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3553,7 +3553,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -3572,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D130" sqref="D130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3625,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3647,7 +3647,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3658,7 +3658,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3669,7 +3669,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3680,7 +3680,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3691,7 +3691,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3724,7 +3724,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3735,7 +3735,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3746,7 +3746,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3757,7 +3757,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3768,7 +3768,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3878,7 +3878,7 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3889,7 +3889,7 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3900,7 +3900,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3911,7 +3911,7 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3961,7 +3961,7 @@
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -3975,7 +3975,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3986,7 +3986,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="E35" t="s">
         <v>89</v>
@@ -4105,7 +4105,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4168,7 +4168,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4179,7 +4179,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4190,7 +4190,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="56" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4224,7 +4224,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -20805,7 +20805,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -20907,10 +20907,10 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
+        <v>407</v>
+      </c>
+      <c r="F83" t="s">
         <v>408</v>
-      </c>
-      <c r="F83" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -21092,7 +21092,7 @@
         <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -21103,7 +21103,7 @@
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F100" t="s">
         <v>285</v>
@@ -21150,7 +21150,7 @@
         <v>18</v>
       </c>
       <c r="D104" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -21161,7 +21161,7 @@
         <v>18</v>
       </c>
       <c r="D105" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -21183,7 +21183,7 @@
         <v>18</v>
       </c>
       <c r="D107" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -21266,7 +21266,7 @@
         <v>2</v>
       </c>
       <c r="D114" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="E114" t="s">
         <v>90</v>
@@ -21280,7 +21280,7 @@
         <v>18</v>
       </c>
       <c r="D115" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -21291,7 +21291,7 @@
         <v>18</v>
       </c>
       <c r="D116" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -21324,7 +21324,7 @@
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -21335,7 +21335,7 @@
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -21346,7 +21346,7 @@
         <v>18</v>
       </c>
       <c r="D121" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -21357,7 +21357,7 @@
         <v>18</v>
       </c>
       <c r="D122" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -21368,7 +21368,7 @@
         <v>18</v>
       </c>
       <c r="D123" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -21379,7 +21379,7 @@
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -21404,7 +21404,7 @@
         <v>18</v>
       </c>
       <c r="D126" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -21415,7 +21415,7 @@
         <v>18</v>
       </c>
       <c r="D127" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -21426,7 +21426,7 @@
         <v>18</v>
       </c>
       <c r="D128" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -21451,7 +21451,7 @@
         <v>18</v>
       </c>
       <c r="D130" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
@@ -21462,7 +21462,7 @@
         <v>18</v>
       </c>
       <c r="D131" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
@@ -21473,10 +21473,10 @@
         <v>18</v>
       </c>
       <c r="D132" t="s">
+        <v>623</v>
+      </c>
+      <c r="F132" t="s">
         <v>624</v>
-      </c>
-      <c r="F132" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
@@ -21487,7 +21487,7 @@
         <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -21509,7 +21509,7 @@
         <v>18</v>
       </c>
       <c r="D135" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
@@ -21520,7 +21520,7 @@
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
@@ -21531,7 +21531,7 @@
         <v>18</v>
       </c>
       <c r="D137" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
@@ -21542,7 +21542,7 @@
         <v>18</v>
       </c>
       <c r="D138" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
@@ -21553,7 +21553,7 @@
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -21564,10 +21564,10 @@
         <v>18</v>
       </c>
       <c r="D140" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F140" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
@@ -21578,7 +21578,7 @@
         <v>18</v>
       </c>
       <c r="D141" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.25">
@@ -21603,7 +21603,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -21611,7 +21611,7 @@
         <v>145</v>
       </c>
       <c r="D144" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -21636,7 +21636,7 @@
         <v>18</v>
       </c>
       <c r="D146" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E146" t="s">
         <v>80</v>
@@ -21664,7 +21664,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -21675,10 +21675,10 @@
         <v>2</v>
       </c>
       <c r="D149" t="s">
+        <v>338</v>
+      </c>
+      <c r="E149" t="s">
         <v>339</v>
-      </c>
-      <c r="E149" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -21689,7 +21689,7 @@
         <v>18</v>
       </c>
       <c r="D150" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -21700,7 +21700,7 @@
         <v>2</v>
       </c>
       <c r="D151" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -21711,7 +21711,7 @@
         <v>18</v>
       </c>
       <c r="D152" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -21722,7 +21722,7 @@
         <v>18</v>
       </c>
       <c r="D153" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -21733,7 +21733,7 @@
         <v>18</v>
       </c>
       <c r="D154" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -21744,10 +21744,10 @@
         <v>18</v>
       </c>
       <c r="D155" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E155" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -21772,8 +21772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21820,7 +21820,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E3" t="s">
         <v>253</v>
@@ -21877,16 +21877,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D6" t="s">
         <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F6" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -21894,13 +21894,13 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>620</v>
+      </c>
+      <c r="F7" t="s">
         <v>621</v>
       </c>
-      <c r="F7" t="s">
-        <v>622</v>
-      </c>
       <c r="G7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -21908,10 +21908,10 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E8" t="s">
         <v>328</v>
-      </c>
-      <c r="E8" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -21927,19 +21927,19 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>636</v>
+      </c>
+      <c r="E10" t="s">
         <v>637</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>638</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>639</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>640</v>
-      </c>
-      <c r="H10" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -21953,13 +21953,13 @@
         <v>237</v>
       </c>
       <c r="F11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G11" t="s">
         <v>249</v>
       </c>
       <c r="H11" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -21987,7 +21987,7 @@
         <v>237</v>
       </c>
       <c r="F13" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G13" t="s">
         <v>249</v>
@@ -21998,7 +21998,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E14" t="s">
         <v>225</v>
@@ -22018,7 +22018,7 @@
         <v>237</v>
       </c>
       <c r="F15" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G15" t="s">
         <v>249</v>
@@ -22029,16 +22029,16 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E16" t="s">
         <v>225</v>
       </c>
       <c r="F16" t="s">
+        <v>627</v>
+      </c>
+      <c r="G16" t="s">
         <v>628</v>
-      </c>
-      <c r="G16" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -22174,7 +22174,7 @@
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -22185,7 +22185,7 @@
         <v>122</v>
       </c>
       <c r="D34" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E34" t="s">
         <v>123</v>
@@ -22219,7 +22219,7 @@
         <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E36" t="s">
         <v>225</v>
@@ -22233,13 +22233,13 @@
         <v>56</v>
       </c>
       <c r="C37" t="s">
+        <v>739</v>
+      </c>
+      <c r="E37" t="s">
         <v>310</v>
       </c>
-      <c r="E37" t="s">
+      <c r="F37" t="s">
         <v>311</v>
-      </c>
-      <c r="F37" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -22360,7 +22360,7 @@
         <v>237</v>
       </c>
       <c r="F46" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="G46" t="s">
         <v>238</v>
@@ -22374,7 +22374,7 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -22451,7 +22451,7 @@
         <v>75</v>
       </c>
       <c r="C54" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E54" t="s">
         <v>292</v>
@@ -22499,10 +22499,10 @@
         <v>79</v>
       </c>
       <c r="C57" t="s">
+        <v>344</v>
+      </c>
+      <c r="E57" t="s">
         <v>345</v>
-      </c>
-      <c r="E57" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -22510,7 +22510,7 @@
         <v>80</v>
       </c>
       <c r="C58" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E58" t="s">
         <v>225</v>
@@ -22538,7 +22538,7 @@
         <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E60" t="s">
         <v>300</v>
@@ -22550,7 +22550,7 @@
         <v>299</v>
       </c>
       <c r="H60" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -22558,7 +22558,7 @@
         <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -22566,13 +22566,13 @@
         <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E62" t="s">
         <v>225</v>
       </c>
       <c r="F62" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -22678,7 +22678,7 @@
         <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D73" t="s">
         <v>76</v>
@@ -22687,10 +22687,10 @@
         <v>77</v>
       </c>
       <c r="F73" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G73" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -22723,19 +22723,19 @@
         <v>108</v>
       </c>
       <c r="C76" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E76" t="s">
+        <v>319</v>
+      </c>
+      <c r="F76" t="s">
         <v>320</v>
       </c>
-      <c r="F76" t="s">
+      <c r="G76" t="s">
         <v>321</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>322</v>
-      </c>
-      <c r="H76" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -22748,7 +22748,7 @@
         <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E78" t="s">
         <v>225</v>
@@ -22802,7 +22802,7 @@
         <v>126</v>
       </c>
       <c r="C84" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -22830,7 +22830,7 @@
         <v>135</v>
       </c>
       <c r="C86" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -22838,7 +22838,7 @@
         <v>136</v>
       </c>
       <c r="C87" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E87" t="s">
         <v>226</v>
@@ -22849,7 +22849,7 @@
         <v>137</v>
       </c>
       <c r="C88" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
   </sheetData>
@@ -22879,7 +22879,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -22887,7 +22887,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -22895,7 +22895,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -22903,7 +22903,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -22911,7 +22911,7 @@
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -22927,7 +22927,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -22935,7 +22935,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -22943,7 +22943,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -22951,7 +22951,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -22959,7 +22959,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -22967,7 +22967,7 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -22975,7 +22975,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -22983,7 +22983,7 @@
         <v>39</v>
       </c>
       <c r="B14" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -22991,7 +22991,7 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -22999,7 +22999,7 @@
         <v>54</v>
       </c>
       <c r="B16" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -23007,7 +23007,7 @@
         <v>56</v>
       </c>
       <c r="B17" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -23015,7 +23015,7 @@
         <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -23031,7 +23031,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -23039,7 +23039,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -23047,7 +23047,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -23084,13 +23084,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>53</v>
@@ -23334,7 +23334,7 @@
         <v>108</v>
       </c>
       <c r="C21" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -23356,7 +23356,7 @@
         <v>134</v>
       </c>
       <c r="C23" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -23367,7 +23367,7 @@
         <v>138</v>
       </c>
       <c r="C24" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -23378,7 +23378,7 @@
         <v>275</v>
       </c>
       <c r="C25" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -23389,7 +23389,7 @@
         <v>326</v>
       </c>
       <c r="C26" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -23400,7 +23400,7 @@
         <v>327</v>
       </c>
       <c r="C27" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -23411,7 +23411,7 @@
         <v>328</v>
       </c>
       <c r="C28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -23422,7 +23422,7 @@
         <v>329</v>
       </c>
       <c r="C29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -23466,7 +23466,7 @@
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -23477,7 +23477,7 @@
         <v>43</v>
       </c>
       <c r="C34" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -23488,7 +23488,7 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -23510,7 +23510,7 @@
         <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -23543,7 +23543,7 @@
         <v>273</v>
       </c>
       <c r="C40" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -23554,7 +23554,7 @@
         <v>47</v>
       </c>
       <c r="C41" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -23565,7 +23565,7 @@
         <v>207</v>
       </c>
       <c r="C42" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -23576,7 +23576,7 @@
         <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -23587,7 +23587,7 @@
         <v>446</v>
       </c>
       <c r="C44" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -23609,7 +23609,7 @@
         <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -23620,7 +23620,7 @@
         <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -23631,7 +23631,7 @@
         <v>129</v>
       </c>
       <c r="C48" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -23642,7 +23642,7 @@
         <v>127</v>
       </c>
       <c r="C49" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -23653,7 +23653,7 @@
         <v>193</v>
       </c>
       <c r="C50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -23664,7 +23664,7 @@
         <v>340</v>
       </c>
       <c r="C51" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -23675,7 +23675,7 @@
         <v>341</v>
       </c>
       <c r="C52" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -23686,7 +23686,7 @@
         <v>343</v>
       </c>
       <c r="C53" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -23697,7 +23697,7 @@
         <v>345</v>
       </c>
       <c r="C54" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -23730,13 +23730,13 @@
         <v>103</v>
       </c>
       <c r="C57" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D57" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E57" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -23747,7 +23747,7 @@
         <v>156</v>
       </c>
       <c r="C58" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -23758,7 +23758,7 @@
         <v>235</v>
       </c>
       <c r="C59" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -23769,7 +23769,7 @@
         <v>315</v>
       </c>
       <c r="C60" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -23780,7 +23780,7 @@
         <v>316</v>
       </c>
       <c r="C61" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -23791,7 +23791,7 @@
         <v>319</v>
       </c>
       <c r="C62" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -23802,7 +23802,7 @@
         <v>318</v>
       </c>
       <c r="C63" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -23813,7 +23813,7 @@
         <v>320</v>
       </c>
       <c r="C64" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -23835,7 +23835,7 @@
         <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -23846,7 +23846,7 @@
         <v>139</v>
       </c>
       <c r="C67" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -23857,7 +23857,7 @@
         <v>272</v>
       </c>
       <c r="C68" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -23879,7 +23879,7 @@
         <v>323</v>
       </c>
       <c r="C70" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -23890,10 +23890,10 @@
         <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D71" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -23904,7 +23904,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -23937,7 +23937,7 @@
         <v>51</v>
       </c>
       <c r="C75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -23948,7 +23948,7 @@
         <v>280</v>
       </c>
       <c r="C76" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -23970,7 +23970,7 @@
         <v>54</v>
       </c>
       <c r="C78" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -23981,7 +23981,7 @@
         <v>50</v>
       </c>
       <c r="C79" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -23992,7 +23992,7 @@
         <v>234</v>
       </c>
       <c r="C80" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -24003,7 +24003,7 @@
         <v>52</v>
       </c>
       <c r="C81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -24014,7 +24014,7 @@
         <v>55</v>
       </c>
       <c r="C82" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -24025,7 +24025,7 @@
         <v>100</v>
       </c>
       <c r="C83" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -24036,7 +24036,7 @@
         <v>57</v>
       </c>
       <c r="C84" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -24047,7 +24047,7 @@
         <v>58</v>
       </c>
       <c r="C85" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -24058,7 +24058,7 @@
         <v>59</v>
       </c>
       <c r="C86" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -24069,7 +24069,7 @@
         <v>60</v>
       </c>
       <c r="C87" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -24080,7 +24080,7 @@
         <v>56</v>
       </c>
       <c r="C88" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -24091,7 +24091,7 @@
         <v>61</v>
       </c>
       <c r="C89" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -24113,7 +24113,7 @@
         <v>277</v>
       </c>
       <c r="C91" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -24124,7 +24124,7 @@
         <v>279</v>
       </c>
       <c r="C92" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -24135,10 +24135,10 @@
         <v>124</v>
       </c>
       <c r="C93" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D93" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -24149,7 +24149,7 @@
         <v>123</v>
       </c>
       <c r="C94" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -24160,7 +24160,7 @@
         <v>121</v>
       </c>
       <c r="C95" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -24171,7 +24171,7 @@
         <v>325</v>
       </c>
       <c r="C96" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -24193,7 +24193,7 @@
         <v>125</v>
       </c>
       <c r="C98" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -24204,7 +24204,7 @@
         <v>337</v>
       </c>
       <c r="C99" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -24215,7 +24215,7 @@
         <v>338</v>
       </c>
       <c r="C100" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -24226,7 +24226,7 @@
         <v>339</v>
       </c>
       <c r="C101" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -24237,7 +24237,7 @@
         <v>196</v>
       </c>
       <c r="C102" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -24248,7 +24248,7 @@
         <v>201</v>
       </c>
       <c r="C103" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -24259,7 +24259,7 @@
         <v>414</v>
       </c>
       <c r="C104" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -24270,7 +24270,7 @@
         <v>198</v>
       </c>
       <c r="C105" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -24281,7 +24281,7 @@
         <v>197</v>
       </c>
       <c r="C106" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -24292,7 +24292,7 @@
         <v>293</v>
       </c>
       <c r="C107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -24303,7 +24303,7 @@
         <v>200</v>
       </c>
       <c r="C108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -24325,7 +24325,7 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -24336,7 +24336,7 @@
         <v>36</v>
       </c>
       <c r="C111" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -24358,7 +24358,7 @@
         <v>209</v>
       </c>
       <c r="C113" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -24369,7 +24369,7 @@
         <v>269</v>
       </c>
       <c r="C114" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -24380,7 +24380,7 @@
         <v>270</v>
       </c>
       <c r="C115" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -24391,7 +24391,7 @@
         <v>271</v>
       </c>
       <c r="C116" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -24413,7 +24413,7 @@
         <v>342</v>
       </c>
       <c r="C118" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -24424,7 +24424,7 @@
         <v>344</v>
       </c>
       <c r="C119" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -24435,7 +24435,7 @@
         <v>146</v>
       </c>
       <c r="C120" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
@@ -24479,7 +24479,7 @@
         <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -24490,7 +24490,7 @@
         <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24501,7 +24501,7 @@
         <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24512,7 +24512,7 @@
         <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24523,7 +24523,7 @@
         <v>179</v>
       </c>
       <c r="C128" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -24534,13 +24534,13 @@
         <v>180</v>
       </c>
       <c r="C129" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G129" t="s">
         <v>55</v>
       </c>
       <c r="H129" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -24562,7 +24562,7 @@
         <v>378</v>
       </c>
       <c r="C131" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -24606,7 +24606,7 @@
         <v>361</v>
       </c>
       <c r="C135" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -24617,7 +24617,7 @@
         <v>350</v>
       </c>
       <c r="C136" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -24639,7 +24639,7 @@
         <v>161</v>
       </c>
       <c r="C138" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -24683,7 +24683,7 @@
         <v>165</v>
       </c>
       <c r="C142" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -24694,7 +24694,7 @@
         <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -24705,7 +24705,7 @@
         <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -24716,7 +24716,7 @@
         <v>362</v>
       </c>
       <c r="C145" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -24727,7 +24727,7 @@
         <v>363</v>
       </c>
       <c r="C146" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -24738,7 +24738,7 @@
         <v>364</v>
       </c>
       <c r="C147" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -24749,7 +24749,7 @@
         <v>365</v>
       </c>
       <c r="C148" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -24760,7 +24760,7 @@
         <v>366</v>
       </c>
       <c r="C149" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -24771,7 +24771,7 @@
         <v>202</v>
       </c>
       <c r="C150" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -24782,10 +24782,10 @@
         <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D151" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -24796,7 +24796,7 @@
         <v>399</v>
       </c>
       <c r="C152" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -24807,7 +24807,7 @@
         <v>401</v>
       </c>
       <c r="C153" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -24818,7 +24818,7 @@
         <v>415</v>
       </c>
       <c r="C154" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -24829,7 +24829,7 @@
         <v>110</v>
       </c>
       <c r="C155" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -24840,7 +24840,7 @@
         <v>111</v>
       </c>
       <c r="C156" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -24851,7 +24851,7 @@
         <v>112</v>
       </c>
       <c r="C157" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -24862,7 +24862,7 @@
         <v>113</v>
       </c>
       <c r="C158" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -24873,7 +24873,7 @@
         <v>114</v>
       </c>
       <c r="C159" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -24884,7 +24884,7 @@
         <v>115</v>
       </c>
       <c r="C160" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -24895,7 +24895,7 @@
         <v>116</v>
       </c>
       <c r="C161" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -24906,7 +24906,7 @@
         <v>117</v>
       </c>
       <c r="C162" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -24928,7 +24928,7 @@
         <v>119</v>
       </c>
       <c r="C164" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -24950,7 +24950,7 @@
         <v>334</v>
       </c>
       <c r="C166" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -24961,7 +24961,7 @@
         <v>268</v>
       </c>
       <c r="C167" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -24972,7 +24972,7 @@
         <v>118</v>
       </c>
       <c r="C168" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -24983,7 +24983,7 @@
         <v>101</v>
       </c>
       <c r="C169" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -24994,7 +24994,7 @@
         <v>153</v>
       </c>
       <c r="C170" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -25005,7 +25005,7 @@
         <v>331</v>
       </c>
       <c r="C171" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -25016,7 +25016,7 @@
         <v>332</v>
       </c>
       <c r="C172" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -25027,7 +25027,7 @@
         <v>330</v>
       </c>
       <c r="C173" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -25038,7 +25038,7 @@
         <v>26</v>
       </c>
       <c r="C174" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
@@ -25049,7 +25049,7 @@
         <v>120</v>
       </c>
       <c r="C175" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -25060,7 +25060,7 @@
         <v>335</v>
       </c>
       <c r="C176" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -25082,7 +25082,7 @@
         <v>154</v>
       </c>
       <c r="C178" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -25093,7 +25093,7 @@
         <v>357</v>
       </c>
       <c r="C179" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -25104,7 +25104,7 @@
         <v>159</v>
       </c>
       <c r="C180" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -25115,10 +25115,10 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D181" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -25129,7 +25129,7 @@
         <v>231</v>
       </c>
       <c r="C182" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -25140,7 +25140,7 @@
         <v>358</v>
       </c>
       <c r="C183" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -25151,7 +25151,7 @@
         <v>155</v>
       </c>
       <c r="C184" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -25162,7 +25162,7 @@
         <v>359</v>
       </c>
       <c r="C185" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -25173,7 +25173,7 @@
         <v>157</v>
       </c>
       <c r="C186" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -25184,7 +25184,7 @@
         <v>356</v>
       </c>
       <c r="C187" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -25206,7 +25206,7 @@
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -25217,7 +25217,7 @@
         <v>170</v>
       </c>
       <c r="C190" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -25228,7 +25228,7 @@
         <v>171</v>
       </c>
       <c r="C191" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -25239,7 +25239,7 @@
         <v>172</v>
       </c>
       <c r="C192" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -25250,7 +25250,7 @@
         <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -25261,7 +25261,7 @@
         <v>174</v>
       </c>
       <c r="C194" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -25272,7 +25272,7 @@
         <v>367</v>
       </c>
       <c r="C195" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -25283,7 +25283,7 @@
         <v>368</v>
       </c>
       <c r="C196" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -25294,7 +25294,7 @@
         <v>221</v>
       </c>
       <c r="C197" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -25305,7 +25305,7 @@
         <v>222</v>
       </c>
       <c r="C198" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -25316,7 +25316,7 @@
         <v>223</v>
       </c>
       <c r="C199" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -25327,7 +25327,7 @@
         <v>224</v>
       </c>
       <c r="C200" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -25338,7 +25338,7 @@
         <v>225</v>
       </c>
       <c r="C201" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -25349,7 +25349,7 @@
         <v>226</v>
       </c>
       <c r="C202" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -25360,7 +25360,7 @@
         <v>215</v>
       </c>
       <c r="C203" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -25371,7 +25371,7 @@
         <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -25382,7 +25382,7 @@
         <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -25393,7 +25393,7 @@
         <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -25404,7 +25404,7 @@
         <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -25415,7 +25415,7 @@
         <v>220</v>
       </c>
       <c r="C208" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -25426,7 +25426,7 @@
         <v>431</v>
       </c>
       <c r="C209" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -25437,7 +25437,7 @@
         <v>432</v>
       </c>
       <c r="C210" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -25448,7 +25448,7 @@
         <v>433</v>
       </c>
       <c r="C211" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -25459,7 +25459,7 @@
         <v>434</v>
       </c>
       <c r="C212" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -25470,7 +25470,7 @@
         <v>435</v>
       </c>
       <c r="C213" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -25481,7 +25481,7 @@
         <v>436</v>
       </c>
       <c r="C214" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -25503,13 +25503,13 @@
         <v>72</v>
       </c>
       <c r="C216" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D216" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E216" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -25520,7 +25520,7 @@
         <v>74</v>
       </c>
       <c r="C217" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -25531,7 +25531,7 @@
         <v>210</v>
       </c>
       <c r="C218" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -25542,7 +25542,7 @@
         <v>294</v>
       </c>
       <c r="C219" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -25553,7 +25553,7 @@
         <v>295</v>
       </c>
       <c r="C220" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -25564,7 +25564,7 @@
         <v>296</v>
       </c>
       <c r="C221" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -25575,7 +25575,7 @@
         <v>297</v>
       </c>
       <c r="C222" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -25597,7 +25597,7 @@
         <v>299</v>
       </c>
       <c r="C224" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -25608,7 +25608,7 @@
         <v>301</v>
       </c>
       <c r="C225" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -25630,7 +25630,7 @@
         <v>437</v>
       </c>
       <c r="C227" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -25641,7 +25641,7 @@
         <v>438</v>
       </c>
       <c r="C228" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -25652,7 +25652,7 @@
         <v>195</v>
       </c>
       <c r="C229" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -25663,7 +25663,7 @@
         <v>131</v>
       </c>
       <c r="C230" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -25674,7 +25674,7 @@
         <v>235</v>
       </c>
       <c r="C231" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -25685,7 +25685,7 @@
         <v>192</v>
       </c>
       <c r="C232" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -25696,7 +25696,7 @@
         <v>439</v>
       </c>
       <c r="C233" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -25707,7 +25707,7 @@
         <v>194</v>
       </c>
       <c r="C234" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -25718,7 +25718,7 @@
         <v>393</v>
       </c>
       <c r="C235" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -25729,7 +25729,7 @@
         <v>394</v>
       </c>
       <c r="C236" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -25740,7 +25740,7 @@
         <v>396</v>
       </c>
       <c r="C237" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -25751,7 +25751,7 @@
         <v>397</v>
       </c>
       <c r="C238" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -25762,7 +25762,7 @@
         <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -25817,7 +25817,7 @@
         <v>214</v>
       </c>
       <c r="C244" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
@@ -25894,7 +25894,7 @@
         <v>177</v>
       </c>
       <c r="C251" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -25905,7 +25905,7 @@
         <v>176</v>
       </c>
       <c r="C252" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -25916,7 +25916,7 @@
         <v>372</v>
       </c>
       <c r="C253" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -25927,7 +25927,7 @@
         <v>376</v>
       </c>
       <c r="C254" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -25938,7 +25938,7 @@
         <v>412</v>
       </c>
       <c r="C255" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -25949,7 +25949,7 @@
         <v>369</v>
       </c>
       <c r="C256" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -25960,7 +25960,7 @@
         <v>370</v>
       </c>
       <c r="C257" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -25971,7 +25971,7 @@
         <v>371</v>
       </c>
       <c r="C258" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -25982,7 +25982,7 @@
         <v>373</v>
       </c>
       <c r="C259" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -25993,7 +25993,7 @@
         <v>374</v>
       </c>
       <c r="C260" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -26004,7 +26004,7 @@
         <v>375</v>
       </c>
       <c r="C261" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -26015,7 +26015,7 @@
         <v>377</v>
       </c>
       <c r="C262" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -26037,7 +26037,7 @@
         <v>382</v>
       </c>
       <c r="C264" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -26048,7 +26048,7 @@
         <v>383</v>
       </c>
       <c r="C265" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -26059,7 +26059,7 @@
         <v>384</v>
       </c>
       <c r="C266" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -26070,7 +26070,7 @@
         <v>385</v>
       </c>
       <c r="C267" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -26081,7 +26081,7 @@
         <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -26103,7 +26103,7 @@
         <v>312</v>
       </c>
       <c r="C270" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -26114,7 +26114,7 @@
         <v>81</v>
       </c>
       <c r="C271" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -26125,7 +26125,7 @@
         <v>311</v>
       </c>
       <c r="C272" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -26136,7 +26136,7 @@
         <v>85</v>
       </c>
       <c r="C273" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -26147,7 +26147,7 @@
         <v>266</v>
       </c>
       <c r="C274" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -26158,7 +26158,7 @@
         <v>82</v>
       </c>
       <c r="C275" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -26169,7 +26169,7 @@
         <v>83</v>
       </c>
       <c r="C276" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -26180,7 +26180,7 @@
         <v>84</v>
       </c>
       <c r="C277" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -26191,7 +26191,7 @@
         <v>212</v>
       </c>
       <c r="C278" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -26202,7 +26202,7 @@
         <v>239</v>
       </c>
       <c r="C279" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
@@ -26213,7 +26213,7 @@
         <v>86</v>
       </c>
       <c r="C280" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -26224,7 +26224,7 @@
         <v>87</v>
       </c>
       <c r="C281" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -26235,7 +26235,7 @@
         <v>88</v>
       </c>
       <c r="C282" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -26246,7 +26246,7 @@
         <v>89</v>
       </c>
       <c r="C283" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -26268,7 +26268,7 @@
         <v>309</v>
       </c>
       <c r="C285" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -26279,7 +26279,7 @@
         <v>233</v>
       </c>
       <c r="C286" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -26312,7 +26312,7 @@
         <v>305</v>
       </c>
       <c r="C289" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -26323,7 +26323,7 @@
         <v>78</v>
       </c>
       <c r="C290" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -26345,7 +26345,7 @@
         <v>306</v>
       </c>
       <c r="C292" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -26356,7 +26356,7 @@
         <v>307</v>
       </c>
       <c r="C293" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -26367,7 +26367,7 @@
         <v>308</v>
       </c>
       <c r="C294" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -26378,7 +26378,7 @@
         <v>77</v>
       </c>
       <c r="C295" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -26458,7 +26458,7 @@
         <v>31</v>
       </c>
       <c r="E302" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -26546,7 +26546,7 @@
         <v>68</v>
       </c>
       <c r="C310" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -26568,7 +26568,7 @@
         <v>292</v>
       </c>
       <c r="C312" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -26579,7 +26579,7 @@
         <v>211</v>
       </c>
       <c r="C313" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -26590,7 +26590,7 @@
         <v>67</v>
       </c>
       <c r="C314" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -26601,7 +26601,7 @@
         <v>290</v>
       </c>
       <c r="C315" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -26612,7 +26612,7 @@
         <v>291</v>
       </c>
       <c r="C316" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -26623,7 +26623,7 @@
         <v>410</v>
       </c>
       <c r="C317" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -26634,7 +26634,7 @@
         <v>409</v>
       </c>
       <c r="C318" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -26656,7 +26656,7 @@
         <v>232</v>
       </c>
       <c r="C320" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -26667,7 +26667,7 @@
         <v>402</v>
       </c>
       <c r="C321" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -26678,7 +26678,7 @@
         <v>407</v>
       </c>
       <c r="C322" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -26689,7 +26689,7 @@
         <v>404</v>
       </c>
       <c r="C323" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -26700,7 +26700,7 @@
         <v>405</v>
       </c>
       <c r="C324" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -26711,7 +26711,7 @@
         <v>403</v>
       </c>
       <c r="C325" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
@@ -26722,7 +26722,7 @@
         <v>406</v>
       </c>
       <c r="C326" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -26733,7 +26733,7 @@
         <v>32</v>
       </c>
       <c r="C327" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -26744,7 +26744,7 @@
         <v>33</v>
       </c>
       <c r="C328" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -26755,7 +26755,7 @@
         <v>213</v>
       </c>
       <c r="C329" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -26766,7 +26766,7 @@
         <v>267</v>
       </c>
       <c r="C330" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -26810,7 +26810,7 @@
         <v>137</v>
       </c>
       <c r="C334" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
@@ -26821,7 +26821,7 @@
         <v>418</v>
       </c>
       <c r="C335" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
@@ -26832,7 +26832,7 @@
         <v>419</v>
       </c>
       <c r="C336" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -26843,7 +26843,7 @@
         <v>420</v>
       </c>
       <c r="C337" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -26854,7 +26854,7 @@
         <v>421</v>
       </c>
       <c r="C338" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -26865,7 +26865,7 @@
         <v>417</v>
       </c>
       <c r="C339" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -26876,7 +26876,7 @@
         <v>145</v>
       </c>
       <c r="C340" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -26887,7 +26887,7 @@
         <v>349</v>
       </c>
       <c r="C341" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -26898,7 +26898,7 @@
         <v>351</v>
       </c>
       <c r="C342" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -26909,7 +26909,7 @@
         <v>352</v>
       </c>
       <c r="C343" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -26920,7 +26920,7 @@
         <v>350</v>
       </c>
       <c r="C344" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -26931,7 +26931,7 @@
         <v>408</v>
       </c>
       <c r="C345" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -26964,7 +26964,7 @@
         <v>347</v>
       </c>
       <c r="C348" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -26975,7 +26975,7 @@
         <v>348</v>
       </c>
       <c r="C349" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -26986,7 +26986,7 @@
         <v>416</v>
       </c>
       <c r="C350" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -26997,7 +26997,7 @@
         <v>203</v>
       </c>
       <c r="C351" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -27008,10 +27008,10 @@
         <v>7</v>
       </c>
       <c r="C352" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D352" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -27022,10 +27022,10 @@
         <v>8</v>
       </c>
       <c r="C353" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D353" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -27036,10 +27036,10 @@
         <v>9</v>
       </c>
       <c r="C354" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D354" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -27050,10 +27050,10 @@
         <v>10</v>
       </c>
       <c r="C355" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D355" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -27064,10 +27064,10 @@
         <v>11</v>
       </c>
       <c r="C356" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D356" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -27078,7 +27078,7 @@
         <v>73</v>
       </c>
       <c r="C357" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -27089,7 +27089,7 @@
         <v>140</v>
       </c>
       <c r="C358" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -27100,7 +27100,7 @@
         <v>141</v>
       </c>
       <c r="C359" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -27111,7 +27111,7 @@
         <v>142</v>
       </c>
       <c r="C360" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -27122,7 +27122,7 @@
         <v>199</v>
       </c>
       <c r="C361" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -27133,7 +27133,7 @@
         <v>205</v>
       </c>
       <c r="C362" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -27144,7 +27144,7 @@
         <v>206</v>
       </c>
       <c r="C363" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -27188,7 +27188,7 @@
         <v>94</v>
       </c>
       <c r="C367" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -27199,7 +27199,7 @@
         <v>95</v>
       </c>
       <c r="C368" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -27210,7 +27210,7 @@
         <v>96</v>
       </c>
       <c r="C369" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -27221,7 +27221,7 @@
         <v>97</v>
       </c>
       <c r="C370" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -27232,7 +27232,7 @@
         <v>314</v>
       </c>
       <c r="C371" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -27243,7 +27243,7 @@
         <v>98</v>
       </c>
       <c r="C372" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -27265,7 +27265,7 @@
         <v>63</v>
       </c>
       <c r="C374" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -27276,7 +27276,7 @@
         <v>64</v>
       </c>
       <c r="C375" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -27298,7 +27298,7 @@
         <v>281</v>
       </c>
       <c r="C377" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -27309,7 +27309,7 @@
         <v>282</v>
       </c>
       <c r="C378" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -27320,7 +27320,7 @@
         <v>283</v>
       </c>
       <c r="C379" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -27331,7 +27331,7 @@
         <v>284</v>
       </c>
       <c r="C380" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -27342,7 +27342,7 @@
         <v>285</v>
       </c>
       <c r="C381" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -27353,7 +27353,7 @@
         <v>286</v>
       </c>
       <c r="C382" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -27364,7 +27364,7 @@
         <v>441</v>
       </c>
       <c r="C383" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -27375,7 +27375,7 @@
         <v>184</v>
       </c>
       <c r="C384" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -27386,7 +27386,7 @@
         <v>185</v>
       </c>
       <c r="C385" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -27397,7 +27397,7 @@
         <v>186</v>
       </c>
       <c r="C386" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -27408,7 +27408,7 @@
         <v>187</v>
       </c>
       <c r="C387" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -27419,7 +27419,7 @@
         <v>188</v>
       </c>
       <c r="C388" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -27430,7 +27430,7 @@
         <v>208</v>
       </c>
       <c r="C389" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
@@ -27474,7 +27474,7 @@
         <v>227</v>
       </c>
       <c r="C393" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -27485,7 +27485,7 @@
         <v>228</v>
       </c>
       <c r="C394" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -27496,7 +27496,7 @@
         <v>229</v>
       </c>
       <c r="C395" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -27507,7 +27507,7 @@
         <v>230</v>
       </c>
       <c r="C396" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -27518,7 +27518,7 @@
         <v>249</v>
       </c>
       <c r="C397" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -27529,7 +27529,7 @@
         <v>242</v>
       </c>
       <c r="C398" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -27540,7 +27540,7 @@
         <v>274</v>
       </c>
       <c r="C399" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -27779,7 +27779,7 @@
         <v>16</v>
       </c>
       <c r="C424" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -27790,7 +27790,7 @@
         <v>15</v>
       </c>
       <c r="C425" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
@@ -27801,7 +27801,7 @@
         <v>14</v>
       </c>
       <c r="C426" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -27812,7 +27812,7 @@
         <v>13</v>
       </c>
       <c r="C427" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -27833,7 +27833,7 @@
         <v>442</v>
       </c>
       <c r="C430" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -27844,7 +27844,7 @@
         <v>443</v>
       </c>
       <c r="C431" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -27855,7 +27855,7 @@
         <v>444</v>
       </c>
       <c r="C432" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -27866,7 +27866,7 @@
         <v>143</v>
       </c>
       <c r="C433" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -27910,7 +27910,7 @@
         <v>353</v>
       </c>
       <c r="C437" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -27921,7 +27921,7 @@
         <v>75</v>
       </c>
       <c r="C438" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -27970,7 +27970,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B3">
         <v>5235</v>
@@ -27990,13 +27990,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B4">
         <v>3621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D4">
         <v>1230</v>
@@ -28010,7 +28010,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="B5">
         <v>3412</v>
@@ -28025,7 +28025,7 @@
         <v>1977</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
   </sheetData>
@@ -28062,84 +28062,84 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C8" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B9" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Room9: Wallsafe Input (script-39) Lab Entry Keypad Input (script-40) Door: Open (scrpit-4)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -3572,8 +3572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21770,10 +21770,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22769,86 +22769,91 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>122</v>
-      </c>
-      <c r="B82" t="s">
-        <v>6</v>
-      </c>
-      <c r="C82" t="s">
-        <v>75</v>
-      </c>
-      <c r="D82" t="s">
-        <v>73</v>
-      </c>
-      <c r="E82" t="s">
-        <v>71</v>
-      </c>
-      <c r="F82" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B83" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" t="s">
+        <v>73</v>
+      </c>
+      <c r="E83" t="s">
+        <v>71</v>
+      </c>
+      <c r="F83" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>126</v>
       </c>
-      <c r="C84" t="s">
-        <v>624</v>
-      </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>127</v>
-      </c>
-      <c r="B85" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C85" t="s">
-        <v>20</v>
-      </c>
-      <c r="D85" t="s">
-        <v>22</v>
-      </c>
-      <c r="E85" t="s">
-        <v>21</v>
-      </c>
-      <c r="F85" t="s">
-        <v>26</v>
+        <v>624</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="B86" t="s">
+        <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>631</v>
+        <v>20</v>
+      </c>
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" t="s">
+        <v>21</v>
+      </c>
+      <c r="F86" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C87" t="s">
-        <v>618</v>
-      </c>
-      <c r="E87" t="s">
-        <v>226</v>
+        <v>631</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
+        <v>136</v>
+      </c>
+      <c r="C88" t="s">
+        <v>618</v>
+      </c>
+      <c r="E88" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89">
         <v>137</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C89" t="s">
         <v>588</v>
       </c>
     </row>
@@ -23062,8 +23067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="C436" sqref="C436"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Cutscene: Purple Tentacle in Basement (script-42)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="743">
   <si>
     <t>Purpose</t>
   </si>
@@ -3581,8 +3581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21781,8 +21781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22883,10 +22883,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23076,6 +23076,14 @@
       </c>
       <c r="B23" t="s">
         <v>738</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -23090,8 +23098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A248" workbookViewId="0">
+      <selection activeCell="B256" sqref="B256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Purple Tentacle: Check for close actors (script-43)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1247" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="744">
   <si>
     <t>Purpose</t>
   </si>
@@ -2264,6 +2264,9 @@
   </si>
   <si>
     <t>3 = Again</t>
+  </si>
+  <si>
+    <t>Weird Ed: Should storm lab</t>
   </si>
 </sst>
 </file>
@@ -3581,8 +3584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21779,10 +21782,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I89"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22457,188 +22460,185 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C54" t="s">
-        <v>481</v>
+        <v>743</v>
       </c>
       <c r="E54" t="s">
-        <v>290</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>213</v>
+        <v>481</v>
       </c>
       <c r="E55" t="s">
-        <v>209</v>
-      </c>
-      <c r="F55" t="s">
-        <v>210</v>
-      </c>
-      <c r="G55" t="s">
-        <v>211</v>
-      </c>
-      <c r="H55" t="s">
-        <v>295</v>
-      </c>
-      <c r="I55" t="s">
-        <v>212</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="E56" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="F56" t="s">
-        <v>217</v>
+        <v>210</v>
+      </c>
+      <c r="G56" t="s">
+        <v>211</v>
+      </c>
+      <c r="H56" t="s">
+        <v>295</v>
+      </c>
+      <c r="I56" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
+        <v>78</v>
+      </c>
+      <c r="C57" t="s">
+        <v>215</v>
+      </c>
+      <c r="E57" t="s">
+        <v>216</v>
+      </c>
+      <c r="F57" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58">
         <v>79</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>342</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E58" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="59" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59">
         <v>80</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>344</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E59" t="s">
         <v>223</v>
       </c>
-      <c r="F58" t="s">
+      <c r="F59" t="s">
         <v>224</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>81</v>
-      </c>
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" t="s">
-        <v>59</v>
-      </c>
-      <c r="E59" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B60" t="s">
+        <v>7</v>
       </c>
       <c r="C60" t="s">
-        <v>574</v>
+        <v>59</v>
       </c>
       <c r="E60" t="s">
-        <v>298</v>
-      </c>
-      <c r="F60" t="s">
-        <v>296</v>
-      </c>
-      <c r="G60" t="s">
-        <v>297</v>
-      </c>
-      <c r="H60" t="s">
-        <v>595</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
-        <v>576</v>
+        <v>574</v>
+      </c>
+      <c r="E61" t="s">
+        <v>298</v>
+      </c>
+      <c r="F61" t="s">
+        <v>296</v>
+      </c>
+      <c r="G61" t="s">
+        <v>297</v>
+      </c>
+      <c r="H61" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C62" t="s">
-        <v>408</v>
-      </c>
-      <c r="E62" t="s">
-        <v>223</v>
-      </c>
-      <c r="F62" t="s">
-        <v>409</v>
+        <v>576</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>89</v>
+        <v>84</v>
+      </c>
+      <c r="C63" t="s">
+        <v>408</v>
+      </c>
+      <c r="E63" t="s">
+        <v>223</v>
+      </c>
+      <c r="F63" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>90</v>
-      </c>
-      <c r="D64" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>90</v>
       </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>104</v>
+      <c r="D65" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>91</v>
-      </c>
-      <c r="D66" t="s">
-        <v>87</v>
+        <v>90</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>91</v>
       </c>
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67" t="s">
-        <v>103</v>
-      </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D68" t="s">
         <v>90</v>
@@ -22646,229 +22646,243 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>96</v>
+        <v>92</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
-      </c>
-      <c r="E69" t="s">
-        <v>223</v>
-      </c>
-      <c r="F69" t="s">
-        <v>224</v>
+        <v>105</v>
+      </c>
+      <c r="D69" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>222</v>
+      </c>
+      <c r="E70" t="s">
+        <v>223</v>
+      </c>
+      <c r="F70" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C73" t="s">
-        <v>735</v>
-      </c>
-      <c r="D73" t="s">
-        <v>76</v>
-      </c>
-      <c r="E73" t="s">
-        <v>77</v>
-      </c>
-      <c r="F73" t="s">
-        <v>732</v>
-      </c>
-      <c r="G73" t="s">
-        <v>731</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>105</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C74" t="s">
-        <v>130</v>
+        <v>735</v>
+      </c>
+      <c r="D74" t="s">
+        <v>76</v>
+      </c>
+      <c r="E74" t="s">
+        <v>77</v>
+      </c>
+      <c r="F74" t="s">
+        <v>732</v>
+      </c>
+      <c r="G74" t="s">
+        <v>731</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>740</v>
-      </c>
-      <c r="D75" t="s">
-        <v>741</v>
-      </c>
-      <c r="E75" t="s">
-        <v>129</v>
-      </c>
-      <c r="F75" t="s">
-        <v>742</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B76" t="s">
+        <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>321</v>
+        <v>740</v>
+      </c>
+      <c r="D76" t="s">
+        <v>741</v>
       </c>
       <c r="E76" t="s">
-        <v>317</v>
+        <v>129</v>
       </c>
       <c r="F76" t="s">
-        <v>318</v>
-      </c>
-      <c r="G76" t="s">
-        <v>319</v>
-      </c>
-      <c r="H76" t="s">
-        <v>320</v>
+        <v>742</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C77" t="s">
+        <v>321</v>
+      </c>
+      <c r="E77" t="s">
+        <v>317</v>
+      </c>
+      <c r="F77" t="s">
+        <v>318</v>
+      </c>
+      <c r="G77" t="s">
+        <v>319</v>
+      </c>
+      <c r="H77" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>110</v>
-      </c>
-      <c r="C78" t="s">
-        <v>509</v>
-      </c>
-      <c r="E78" t="s">
-        <v>223</v>
-      </c>
-      <c r="F78" t="s">
-        <v>224</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C79" t="s">
+        <v>509</v>
+      </c>
+      <c r="E79" t="s">
+        <v>223</v>
+      </c>
+      <c r="F79" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>122</v>
-      </c>
-      <c r="B83" t="s">
-        <v>6</v>
-      </c>
-      <c r="C83" t="s">
-        <v>75</v>
-      </c>
-      <c r="D83" t="s">
-        <v>73</v>
-      </c>
-      <c r="E83" t="s">
-        <v>71</v>
-      </c>
-      <c r="F83" t="s">
-        <v>72</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" t="s">
+        <v>73</v>
+      </c>
+      <c r="E84" t="s">
+        <v>71</v>
+      </c>
+      <c r="F84" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>126</v>
       </c>
-      <c r="C85" t="s">
-        <v>622</v>
-      </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>127</v>
-      </c>
-      <c r="B86" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C86" t="s">
-        <v>20</v>
-      </c>
-      <c r="D86" t="s">
-        <v>22</v>
-      </c>
-      <c r="E86" t="s">
-        <v>21</v>
-      </c>
-      <c r="F86" t="s">
-        <v>26</v>
+        <v>622</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="B87" t="s">
+        <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>629</v>
+        <v>20</v>
+      </c>
+      <c r="D87" t="s">
+        <v>22</v>
+      </c>
+      <c r="E87" t="s">
+        <v>21</v>
+      </c>
+      <c r="F87" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C88" t="s">
-        <v>616</v>
-      </c>
-      <c r="E88" t="s">
-        <v>224</v>
+        <v>629</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
+        <v>136</v>
+      </c>
+      <c r="C89" t="s">
+        <v>616</v>
+      </c>
+      <c r="E89" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90">
         <v>137</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C90" t="s">
         <v>586</v>
       </c>
     </row>
@@ -23098,8 +23112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A248" workbookViewId="0">
-      <selection activeCell="B256" sqref="B256"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Door: Close (script-5) Room Lights: Check for flashlight / room light status (script-50) Dungeon: Close Entry Door (script-51) Repeat Outside Sound (script-52) Microwave (script-53)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1255" uniqueCount="749">
   <si>
     <t>Purpose</t>
   </si>
@@ -1930,9 +1930,6 @@
     <t>Green Tentacle: Block player passing</t>
   </si>
   <si>
-    <t>Telescope Rotate</t>
-  </si>
-  <si>
     <t>Telescope: Current Room</t>
   </si>
   <si>
@@ -2279,6 +2276,12 @@
   </si>
   <si>
     <t>255 = Dead</t>
+  </si>
+  <si>
+    <t>Steel Door</t>
+  </si>
+  <si>
+    <t>Rotate</t>
   </si>
 </sst>
 </file>
@@ -2834,7 +2837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -3269,7 +3272,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -3395,7 +3398,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3596,8 +3599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3649,7 +3652,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3985,7 +3988,7 @@
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E33" t="s">
         <v>85</v>
@@ -4010,7 +4013,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="E35" t="s">
         <v>89</v>
@@ -4079,7 +4082,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4151,7 +4154,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -20829,7 +20832,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -21796,8 +21799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21907,10 +21910,10 @@
         <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F6" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -21951,19 +21954,19 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>631</v>
+      </c>
+      <c r="E10" t="s">
         <v>632</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>633</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>634</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>635</v>
-      </c>
-      <c r="H10" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -21977,7 +21980,7 @@
         <v>234</v>
       </c>
       <c r="F11" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G11" t="s">
         <v>246</v>
@@ -22011,7 +22014,7 @@
         <v>234</v>
       </c>
       <c r="F13" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G13" t="s">
         <v>246</v>
@@ -22022,7 +22025,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E14" t="s">
         <v>222</v>
@@ -22042,7 +22045,7 @@
         <v>234</v>
       </c>
       <c r="F15" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G15" t="s">
         <v>246</v>
@@ -22053,19 +22056,19 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>742</v>
+      </c>
+      <c r="E16" t="s">
         <v>743</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>744</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>745</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>746</v>
-      </c>
-      <c r="H16" t="s">
-        <v>747</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -22229,7 +22232,7 @@
         <v>122</v>
       </c>
       <c r="D35" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="E35" t="s">
         <v>123</v>
@@ -22263,7 +22266,7 @@
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="E37" t="s">
         <v>222</v>
@@ -22277,7 +22280,7 @@
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="E38" t="s">
         <v>307</v>
@@ -22495,7 +22498,7 @@
         <v>74</v>
       </c>
       <c r="C55" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="E55" t="s">
         <v>223</v>
@@ -22733,7 +22736,7 @@
         <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D75" t="s">
         <v>76</v>
@@ -22742,10 +22745,10 @@
         <v>77</v>
       </c>
       <c r="F75" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G75" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -22767,16 +22770,16 @@
         <v>7</v>
       </c>
       <c r="C77" t="s">
+        <v>738</v>
+      </c>
+      <c r="D77" t="s">
         <v>739</v>
-      </c>
-      <c r="D77" t="s">
-        <v>740</v>
       </c>
       <c r="E77" t="s">
         <v>129</v>
       </c>
       <c r="F77" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -22929,10 +22932,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22993,7 +22996,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>631</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -23009,7 +23012,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -23025,7 +23028,7 @@
         <v>28</v>
       </c>
       <c r="B11" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -23081,7 +23084,7 @@
         <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -23097,7 +23100,7 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -23105,7 +23108,7 @@
         <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -23113,7 +23116,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -23121,7 +23124,7 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -23130,6 +23133,14 @@
       </c>
       <c r="B24" t="s">
         <v>381</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -23144,8 +23155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A298" workbookViewId="0">
-      <selection activeCell="C313" sqref="C313"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="C93" sqref="C93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23172,7 +23183,7 @@
         <v>402</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>53</v>
@@ -23818,7 +23829,7 @@
         <v>476</v>
       </c>
       <c r="E57" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -23972,10 +23983,10 @@
         <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D71" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -23986,7 +23997,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -24220,7 +24231,7 @@
         <v>378</v>
       </c>
       <c r="D93" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -24561,7 +24572,7 @@
         <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -24572,7 +24583,7 @@
         <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24583,7 +24594,7 @@
         <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24594,7 +24605,7 @@
         <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24688,7 +24699,7 @@
         <v>361</v>
       </c>
       <c r="C135" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -24699,7 +24710,7 @@
         <v>350</v>
       </c>
       <c r="C136" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -24765,7 +24776,7 @@
         <v>165</v>
       </c>
       <c r="C142" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -24776,7 +24787,7 @@
         <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -24787,7 +24798,7 @@
         <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -24798,7 +24809,7 @@
         <v>362</v>
       </c>
       <c r="C145" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -24809,7 +24820,7 @@
         <v>363</v>
       </c>
       <c r="C146" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -24820,7 +24831,7 @@
         <v>364</v>
       </c>
       <c r="C147" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -24831,7 +24842,7 @@
         <v>365</v>
       </c>
       <c r="C148" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -24842,7 +24853,7 @@
         <v>366</v>
       </c>
       <c r="C149" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -24864,7 +24875,7 @@
         <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D151" t="s">
         <v>592</v>
@@ -24878,7 +24889,7 @@
         <v>399</v>
       </c>
       <c r="C152" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -24900,7 +24911,7 @@
         <v>415</v>
       </c>
       <c r="C154" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -25288,7 +25299,7 @@
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -25299,7 +25310,7 @@
         <v>170</v>
       </c>
       <c r="C190" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -25310,7 +25321,7 @@
         <v>171</v>
       </c>
       <c r="C191" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -25321,7 +25332,7 @@
         <v>172</v>
       </c>
       <c r="C192" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -25332,7 +25343,7 @@
         <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -25343,7 +25354,7 @@
         <v>174</v>
       </c>
       <c r="C194" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -25354,7 +25365,7 @@
         <v>367</v>
       </c>
       <c r="C195" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -25365,7 +25376,7 @@
         <v>368</v>
       </c>
       <c r="C196" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -25442,7 +25453,7 @@
         <v>215</v>
       </c>
       <c r="C203" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -25453,7 +25464,7 @@
         <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -25464,7 +25475,7 @@
         <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -25475,7 +25486,7 @@
         <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -25486,7 +25497,7 @@
         <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -25497,7 +25508,7 @@
         <v>220</v>
       </c>
       <c r="C208" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -25508,7 +25519,7 @@
         <v>431</v>
       </c>
       <c r="C209" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -25519,7 +25530,7 @@
         <v>432</v>
       </c>
       <c r="C210" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -25530,7 +25541,7 @@
         <v>433</v>
       </c>
       <c r="C211" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -25541,7 +25552,7 @@
         <v>434</v>
       </c>
       <c r="C212" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -25552,7 +25563,7 @@
         <v>435</v>
       </c>
       <c r="C213" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -25563,7 +25574,7 @@
         <v>436</v>
       </c>
       <c r="C214" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -25588,10 +25599,10 @@
         <v>470</v>
       </c>
       <c r="D216" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="E216" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -25976,7 +25987,7 @@
         <v>177</v>
       </c>
       <c r="C251" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -26009,7 +26020,7 @@
         <v>376</v>
       </c>
       <c r="C254" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -26020,7 +26031,7 @@
         <v>412</v>
       </c>
       <c r="C255" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -26031,7 +26042,7 @@
         <v>369</v>
       </c>
       <c r="C256" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -26042,7 +26053,7 @@
         <v>370</v>
       </c>
       <c r="C257" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -26053,7 +26064,7 @@
         <v>371</v>
       </c>
       <c r="C258" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -26064,7 +26075,7 @@
         <v>373</v>
       </c>
       <c r="C259" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -26075,7 +26086,7 @@
         <v>374</v>
       </c>
       <c r="C260" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -26086,7 +26097,7 @@
         <v>375</v>
       </c>
       <c r="C261" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -26097,7 +26108,7 @@
         <v>377</v>
       </c>
       <c r="C262" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -26119,7 +26130,7 @@
         <v>382</v>
       </c>
       <c r="C264" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -26130,7 +26141,7 @@
         <v>383</v>
       </c>
       <c r="C265" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -26152,7 +26163,7 @@
         <v>385</v>
       </c>
       <c r="C267" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -26163,7 +26174,7 @@
         <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -26405,7 +26416,7 @@
         <v>78</v>
       </c>
       <c r="C290" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -26427,7 +26438,7 @@
         <v>306</v>
       </c>
       <c r="C292" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -26449,7 +26460,7 @@
         <v>308</v>
       </c>
       <c r="C294" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -26460,7 +26471,7 @@
         <v>77</v>
       </c>
       <c r="C295" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -26628,7 +26639,7 @@
         <v>68</v>
       </c>
       <c r="C310" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -26650,7 +26661,7 @@
         <v>292</v>
       </c>
       <c r="C312" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -26661,7 +26672,7 @@
         <v>211</v>
       </c>
       <c r="C313" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -26672,7 +26683,7 @@
         <v>67</v>
       </c>
       <c r="C314" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -26683,7 +26694,7 @@
         <v>290</v>
       </c>
       <c r="C315" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -26694,7 +26705,7 @@
         <v>291</v>
       </c>
       <c r="C316" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -26738,7 +26749,7 @@
         <v>232</v>
       </c>
       <c r="C320" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
@@ -26749,7 +26760,7 @@
         <v>402</v>
       </c>
       <c r="C321" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
@@ -26760,7 +26771,7 @@
         <v>407</v>
       </c>
       <c r="C322" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
@@ -26771,7 +26782,7 @@
         <v>404</v>
       </c>
       <c r="C323" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
@@ -26782,7 +26793,7 @@
         <v>405</v>
       </c>
       <c r="C324" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
@@ -26804,7 +26815,7 @@
         <v>406</v>
       </c>
       <c r="C326" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
@@ -26815,7 +26826,7 @@
         <v>32</v>
       </c>
       <c r="C327" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
@@ -26826,7 +26837,7 @@
         <v>33</v>
       </c>
       <c r="C328" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
@@ -26837,7 +26848,7 @@
         <v>213</v>
       </c>
       <c r="C329" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
@@ -26848,7 +26859,7 @@
         <v>267</v>
       </c>
       <c r="C330" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
@@ -27079,7 +27090,7 @@
         <v>203</v>
       </c>
       <c r="C351" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -27270,7 +27281,7 @@
         <v>94</v>
       </c>
       <c r="C367" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -27281,7 +27292,7 @@
         <v>95</v>
       </c>
       <c r="C368" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -27292,7 +27303,7 @@
         <v>96</v>
       </c>
       <c r="C369" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -27303,7 +27314,7 @@
         <v>97</v>
       </c>
       <c r="C370" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -27314,7 +27325,7 @@
         <v>314</v>
       </c>
       <c r="C371" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -27325,7 +27336,7 @@
         <v>98</v>
       </c>
       <c r="C372" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -27347,7 +27358,7 @@
         <v>63</v>
       </c>
       <c r="C374" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -27358,7 +27369,7 @@
         <v>64</v>
       </c>
       <c r="C375" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -27402,7 +27413,7 @@
         <v>283</v>
       </c>
       <c r="C379" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -27413,7 +27424,7 @@
         <v>284</v>
       </c>
       <c r="C380" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -27424,7 +27435,7 @@
         <v>285</v>
       </c>
       <c r="C381" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -27446,7 +27457,7 @@
         <v>441</v>
       </c>
       <c r="C383" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -27915,7 +27926,7 @@
         <v>442</v>
       </c>
       <c r="C430" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -27926,7 +27937,7 @@
         <v>443</v>
       </c>
       <c r="C431" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -27937,7 +27948,7 @@
         <v>444</v>
       </c>
       <c r="C432" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Pool is Empty (script-6) Microwave: (script-69) Pool Water Valve (script-70)
script-67: Contains fragments of surrounding scripts, as well as content not seen elsewhere
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="751">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="756">
   <si>
     <t>Purpose</t>
   </si>
@@ -2288,6 +2288,21 @@
   </si>
   <si>
     <t>Explosion</t>
+  </si>
+  <si>
+    <t>Alarm 1</t>
+  </si>
+  <si>
+    <t>Alarm 2</t>
+  </si>
+  <si>
+    <t>Water Drain</t>
+  </si>
+  <si>
+    <t>0x80 = Valve Open</t>
+  </si>
+  <si>
+    <t>02 = Untouchable</t>
   </si>
 </sst>
 </file>
@@ -2844,7 +2859,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,7 +3621,7 @@
   <dimension ref="A1:XFD156"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D59" sqref="D59"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21806,7 +21821,7 @@
   <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22943,10 +22958,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23168,6 +23183,30 @@
       </c>
       <c r="B27" t="s">
         <v>750</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>32</v>
+      </c>
+      <c r="B28" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>33</v>
+      </c>
+      <c r="B29" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -23182,8 +23221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A412" workbookViewId="0">
-      <selection activeCell="B427" sqref="B427"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23968,6 +24007,9 @@
       <c r="C67" t="s">
         <v>385</v>
       </c>
+      <c r="D67" t="s">
+        <v>755</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68">
@@ -26779,7 +26821,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>28</v>
       </c>
@@ -26790,7 +26832,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="322" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>28</v>
       </c>
@@ -26801,7 +26843,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="323" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>28</v>
       </c>
@@ -26812,7 +26854,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="324" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>28</v>
       </c>
@@ -26823,7 +26865,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="325" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>28</v>
       </c>
@@ -26834,7 +26876,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="326" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>28</v>
       </c>
@@ -26845,7 +26887,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="327" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>29</v>
       </c>
@@ -26856,7 +26898,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="328" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>29</v>
       </c>
@@ -26866,8 +26908,11 @@
       <c r="C328" t="s">
         <v>710</v>
       </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D328" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>29</v>
       </c>
@@ -26878,7 +26923,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="330" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>29</v>
       </c>
@@ -26889,7 +26934,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="331" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>30</v>
       </c>
@@ -26900,7 +26945,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="332" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>30</v>
       </c>
@@ -26911,7 +26956,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="333" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>30</v>
       </c>
@@ -26922,7 +26967,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="334" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>30</v>
       </c>
@@ -26933,7 +26978,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="335" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>30</v>
       </c>
@@ -26944,7 +26989,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="336" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Weird Ed: Check Front Door (script-90) Weird Ed: Help Find Plans (script-91) Weird Ed: Respond to Door Bell (script-92) Weird Ed: Walk Hallway (script-93)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="772">
   <si>
     <t>Purpose</t>
   </si>
@@ -2339,6 +2339,18 @@
   </si>
   <si>
     <t>Give Hamster</t>
+  </si>
+  <si>
+    <t>08 = Not Available</t>
+  </si>
+  <si>
+    <t>2 = Ed has package</t>
+  </si>
+  <si>
+    <t>Weird Ed: Looking for plans</t>
+  </si>
+  <si>
+    <t>Glass Jar has content</t>
   </si>
 </sst>
 </file>
@@ -2670,7 +2682,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2894,8 +2906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3656,8 +3668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21876,10 +21888,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22621,6 +22633,9 @@
       <c r="F55" t="s">
         <v>260</v>
       </c>
+      <c r="G55" t="s">
+        <v>769</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -22764,59 +22779,53 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C66" t="s">
+        <v>770</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>90</v>
-      </c>
-      <c r="D67" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>90</v>
       </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68" t="s">
-        <v>103</v>
+      <c r="D68" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>91</v>
-      </c>
-      <c r="D69" t="s">
-        <v>86</v>
+        <v>90</v>
+      </c>
+      <c r="B69" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>91</v>
       </c>
-      <c r="B70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70" t="s">
-        <v>102</v>
-      </c>
       <c r="D70" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D71" t="s">
         <v>89</v>
@@ -22824,253 +22833,275 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="B72" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" t="s">
+        <v>104</v>
+      </c>
+      <c r="D72" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>96</v>
-      </c>
-      <c r="C73" t="s">
-        <v>218</v>
-      </c>
-      <c r="E73" t="s">
-        <v>219</v>
-      </c>
-      <c r="F73" t="s">
-        <v>220</v>
+        <v>94</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C74" t="s">
-        <v>106</v>
+        <v>218</v>
+      </c>
+      <c r="E74" t="s">
+        <v>219</v>
+      </c>
+      <c r="F74" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C75" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C76" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C77" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>102</v>
-      </c>
-      <c r="C78" t="s">
-        <v>762</v>
-      </c>
-      <c r="E78" t="s">
-        <v>219</v>
-      </c>
-      <c r="F78" t="s">
-        <v>220</v>
+        <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C79" t="s">
-        <v>725</v>
-      </c>
-      <c r="D79" t="s">
-        <v>75</v>
+        <v>762</v>
       </c>
       <c r="E79" t="s">
-        <v>76</v>
+        <v>219</v>
       </c>
       <c r="F79" t="s">
-        <v>722</v>
-      </c>
-      <c r="G79" t="s">
-        <v>721</v>
+        <v>220</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>105</v>
-      </c>
-      <c r="B80" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>129</v>
+        <v>725</v>
+      </c>
+      <c r="D80" t="s">
+        <v>75</v>
+      </c>
+      <c r="E80" t="s">
+        <v>76</v>
+      </c>
+      <c r="F80" t="s">
+        <v>722</v>
+      </c>
+      <c r="G80" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
       </c>
       <c r="C81" t="s">
-        <v>730</v>
-      </c>
-      <c r="E81" t="s">
-        <v>731</v>
-      </c>
-      <c r="F81" t="s">
-        <v>128</v>
-      </c>
-      <c r="G81" t="s">
-        <v>732</v>
+        <v>129</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B82" t="s">
+        <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>312</v>
+        <v>730</v>
       </c>
       <c r="E82" t="s">
-        <v>308</v>
+        <v>731</v>
       </c>
       <c r="F82" t="s">
-        <v>309</v>
+        <v>128</v>
       </c>
       <c r="G82" t="s">
-        <v>310</v>
-      </c>
-      <c r="H82" t="s">
-        <v>311</v>
+        <v>732</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C83" t="s">
+        <v>312</v>
+      </c>
+      <c r="E83" t="s">
+        <v>308</v>
+      </c>
+      <c r="F83" t="s">
+        <v>309</v>
+      </c>
+      <c r="G83" t="s">
+        <v>310</v>
+      </c>
+      <c r="H83" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>110</v>
-      </c>
-      <c r="C84" t="s">
-        <v>500</v>
-      </c>
-      <c r="E84" t="s">
-        <v>219</v>
-      </c>
-      <c r="F84" t="s">
-        <v>220</v>
+        <v>109</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C85" t="s">
+        <v>500</v>
+      </c>
+      <c r="E85" t="s">
+        <v>219</v>
+      </c>
+      <c r="F85" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>122</v>
-      </c>
-      <c r="B89" t="s">
-        <v>6</v>
-      </c>
-      <c r="C89" t="s">
-        <v>74</v>
-      </c>
-      <c r="D89" t="s">
-        <v>72</v>
-      </c>
-      <c r="E89" t="s">
-        <v>70</v>
-      </c>
-      <c r="F89" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B90" t="s">
+        <v>6</v>
+      </c>
+      <c r="C90" t="s">
+        <v>74</v>
+      </c>
+      <c r="D90" t="s">
+        <v>72</v>
+      </c>
+      <c r="E90" t="s">
+        <v>70</v>
+      </c>
+      <c r="F90" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>126</v>
       </c>
-      <c r="C91" t="s">
-        <v>613</v>
-      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>127</v>
-      </c>
-      <c r="B92" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C92" t="s">
-        <v>20</v>
-      </c>
-      <c r="D92" t="s">
-        <v>22</v>
-      </c>
-      <c r="E92" t="s">
-        <v>21</v>
-      </c>
-      <c r="F92" t="s">
-        <v>26</v>
+        <v>613</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="B93" t="s">
+        <v>7</v>
       </c>
       <c r="C93" t="s">
-        <v>620</v>
+        <v>20</v>
+      </c>
+      <c r="D93" t="s">
+        <v>22</v>
+      </c>
+      <c r="E93" t="s">
+        <v>21</v>
+      </c>
+      <c r="F93" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C94" t="s">
-        <v>607</v>
-      </c>
-      <c r="E94" t="s">
-        <v>220</v>
+        <v>771</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
+        <v>135</v>
+      </c>
+      <c r="C95" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>136</v>
+      </c>
+      <c r="C96" t="s">
+        <v>607</v>
+      </c>
+      <c r="E96" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97">
         <v>137</v>
       </c>
-      <c r="C95" t="s">
+      <c r="C97" t="s">
         <v>577</v>
       </c>
     </row>
@@ -23087,7 +23118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -23364,8 +23395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView topLeftCell="A371" workbookViewId="0">
+      <selection activeCell="C386" sqref="C386"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23471,6 +23502,9 @@
       </c>
       <c r="C7" t="s">
         <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Weird Ed: Storm Dr. Freds Lab (script-94) Play Piano (script-95) Dr Fred: Play Meteor Mess (script-96) The Lab: Set Pin (script-97) Give: Accept Item Check (script-98) Give: Accept Item Check 2 (script-99)
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22695" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="772">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1551" uniqueCount="778">
   <si>
     <t>Purpose</t>
   </si>
@@ -1486,9 +1486,6 @@
     <t>Piano Bench</t>
   </si>
   <si>
-    <t>08 = ?</t>
-  </si>
-  <si>
     <t>Record: Tentacle Mating Call</t>
   </si>
   <si>
@@ -1897,9 +1894,6 @@
     <t>Cassette: Play, Break Windows/Free Key</t>
   </si>
   <si>
-    <t>script-154</t>
-  </si>
-  <si>
     <t>Weird Ed: Walk around the Lab Entry</t>
   </si>
   <si>
@@ -2351,6 +2345,30 @@
   </si>
   <si>
     <t>Glass Jar has content</t>
+  </si>
+  <si>
+    <t>Weird Ed: Is Storming Lab</t>
+  </si>
+  <si>
+    <t>Purple chased out of lab</t>
+  </si>
+  <si>
+    <t>08 = On</t>
+  </si>
+  <si>
+    <t>Highscore: Pin1</t>
+  </si>
+  <si>
+    <t>Highscore: Pin2</t>
+  </si>
+  <si>
+    <t>Highscore: Pin3</t>
+  </si>
+  <si>
+    <t>Highscore: Pin4</t>
+  </si>
+  <si>
+    <t>Give Script: Object-ID</t>
   </si>
 </sst>
 </file>
@@ -2924,10 +2942,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" t="s">
         <v>509</v>
-      </c>
-      <c r="D1" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,7 +2953,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2949,7 +2967,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2963,7 +2981,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2977,7 +2995,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -2991,13 +3009,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3005,7 +3023,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3019,7 +3037,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -3033,7 +3051,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -3047,7 +3065,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -3061,7 +3079,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -3075,7 +3093,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -3089,7 +3107,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -3103,7 +3121,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -3117,7 +3135,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -3131,7 +3149,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -3145,7 +3163,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -3159,7 +3177,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -3173,7 +3191,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -3187,7 +3205,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -3201,7 +3219,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -3229,7 +3247,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -3243,7 +3261,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -3257,7 +3275,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -3271,7 +3289,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -3285,7 +3303,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -3299,7 +3317,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -3313,7 +3331,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -3327,7 +3345,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3341,7 +3359,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -3355,7 +3373,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -3369,7 +3387,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3383,7 +3401,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3397,7 +3415,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3411,7 +3429,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3425,7 +3443,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -3439,7 +3457,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -3453,7 +3471,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -3467,7 +3485,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3481,7 +3499,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -3495,7 +3513,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3509,7 +3527,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3523,7 +3541,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -3537,7 +3555,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3551,7 +3569,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3565,7 +3583,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3579,7 +3597,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3593,7 +3611,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3607,7 +3625,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -3621,7 +3639,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3635,7 +3653,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3649,7 +3667,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -3668,8 +3686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="D98" sqref="D98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3721,7 +3739,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3853,7 +3871,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3864,7 +3882,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -4057,7 +4075,7 @@
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E33" t="s">
         <v>84</v>
@@ -4071,7 +4089,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4082,7 +4100,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E35" t="s">
         <v>88</v>
@@ -4151,7 +4169,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4223,7 +4241,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4275,7 +4293,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4286,7 +4304,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
@@ -20711,7 +20729,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="F57" t="s">
         <v>286</v>
@@ -20882,7 +20900,7 @@
         <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -20904,7 +20922,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -20981,7 +20999,7 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -20992,7 +21010,7 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F82" t="s">
         <v>254</v>
@@ -21075,7 +21093,7 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -21083,7 +21101,7 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -21268,7 +21286,7 @@
         <v>18</v>
       </c>
       <c r="D106" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -21279,7 +21297,7 @@
         <v>18</v>
       </c>
       <c r="D107" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -21301,7 +21319,7 @@
         <v>18</v>
       </c>
       <c r="D109" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -21334,7 +21352,7 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -21384,7 +21402,7 @@
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E116" t="s">
         <v>89</v>
@@ -21453,7 +21471,7 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -21591,10 +21609,10 @@
         <v>18</v>
       </c>
       <c r="D134" t="s">
+        <v>610</v>
+      </c>
+      <c r="F134" t="s">
         <v>611</v>
-      </c>
-      <c r="F134" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -21696,7 +21714,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -21721,7 +21739,7 @@
         <v>18</v>
       </c>
       <c r="D145" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -21754,7 +21772,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E148" t="s">
         <v>79</v>
@@ -21840,7 +21858,7 @@
         <v>18</v>
       </c>
       <c r="D155" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -21851,7 +21869,7 @@
         <v>18</v>
       </c>
       <c r="D156" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -21862,7 +21880,7 @@
         <v>18</v>
       </c>
       <c r="D157" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="E157" t="s">
         <v>332</v>
@@ -21888,10 +21906,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21939,10 +21957,10 @@
         <v>220</v>
       </c>
       <c r="G2" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="H2" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -22007,16 +22025,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D6" t="s">
         <v>81</v>
       </c>
       <c r="E6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F6" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -22024,10 +22042,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
+        <v>607</v>
+      </c>
+      <c r="F7" t="s">
         <v>608</v>
-      </c>
-      <c r="F7" t="s">
-        <v>609</v>
       </c>
       <c r="G7" t="s">
         <v>302</v>
@@ -22057,19 +22075,19 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>621</v>
+      </c>
+      <c r="E10" t="s">
+        <v>622</v>
+      </c>
+      <c r="F10" t="s">
         <v>623</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>624</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>625</v>
-      </c>
-      <c r="G10" t="s">
-        <v>626</v>
-      </c>
-      <c r="H10" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -22083,7 +22101,7 @@
         <v>231</v>
       </c>
       <c r="F11" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G11" t="s">
         <v>242</v>
@@ -22117,7 +22135,7 @@
         <v>231</v>
       </c>
       <c r="F13" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G13" t="s">
         <v>242</v>
@@ -22131,7 +22149,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="E14" t="s">
         <v>219</v>
@@ -22151,7 +22169,7 @@
         <v>231</v>
       </c>
       <c r="F15" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G15" t="s">
         <v>242</v>
@@ -22165,19 +22183,19 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>732</v>
+      </c>
+      <c r="E16" t="s">
+        <v>733</v>
+      </c>
+      <c r="F16" t="s">
         <v>734</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>735</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>736</v>
-      </c>
-      <c r="G16" t="s">
-        <v>737</v>
-      </c>
-      <c r="H16" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -22185,16 +22203,16 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="E17" t="s">
         <v>219</v>
       </c>
       <c r="F17" t="s">
+        <v>614</v>
+      </c>
+      <c r="G17" t="s">
         <v>615</v>
-      </c>
-      <c r="G17" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -22330,7 +22348,7 @@
         <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -22341,7 +22359,7 @@
         <v>121</v>
       </c>
       <c r="D35" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E35" t="s">
         <v>122</v>
@@ -22375,7 +22393,7 @@
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="E37" t="s">
         <v>219</v>
@@ -22389,7 +22407,7 @@
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E38" t="s">
         <v>299</v>
@@ -22510,7 +22528,7 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="E47" t="s">
         <v>219</v>
@@ -22544,7 +22562,7 @@
         <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -22575,10 +22593,10 @@
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="E51" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -22589,10 +22607,10 @@
         <v>7</v>
       </c>
       <c r="C52" t="s">
+        <v>757</v>
+      </c>
+      <c r="E52" t="s">
         <v>759</v>
-      </c>
-      <c r="E52" t="s">
-        <v>761</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -22603,7 +22621,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -22614,7 +22632,7 @@
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -22634,7 +22652,7 @@
         <v>260</v>
       </c>
       <c r="G55" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -22642,7 +22660,7 @@
         <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E56" t="s">
         <v>220</v>
@@ -22670,7 +22688,7 @@
         <v>207</v>
       </c>
       <c r="F58" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="G58" t="s">
         <v>208</v>
@@ -22687,7 +22705,7 @@
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E59" t="s">
         <v>212</v>
@@ -22740,7 +22758,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="E63" t="s">
         <v>290</v>
@@ -22752,7 +22770,7 @@
         <v>289</v>
       </c>
       <c r="H63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -22760,7 +22778,7 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -22782,7 +22800,7 @@
         <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -22898,7 +22916,7 @@
         <v>102</v>
       </c>
       <c r="C79" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E79" t="s">
         <v>219</v>
@@ -22912,7 +22930,7 @@
         <v>103</v>
       </c>
       <c r="C80" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D80" t="s">
         <v>75</v>
@@ -22921,188 +22939,216 @@
         <v>76</v>
       </c>
       <c r="F80" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G80" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>105</v>
-      </c>
-      <c r="B81" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C81" t="s">
-        <v>129</v>
+        <v>770</v>
+      </c>
+      <c r="E81" t="s">
+        <v>219</v>
+      </c>
+      <c r="F81" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B82" t="s">
         <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>730</v>
-      </c>
-      <c r="E82" t="s">
-        <v>731</v>
-      </c>
-      <c r="F82" t="s">
-        <v>128</v>
-      </c>
-      <c r="G82" t="s">
-        <v>732</v>
+        <v>129</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="B83" t="s">
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>312</v>
+        <v>728</v>
       </c>
       <c r="E83" t="s">
-        <v>308</v>
+        <v>729</v>
       </c>
       <c r="F83" t="s">
-        <v>309</v>
+        <v>128</v>
       </c>
       <c r="G83" t="s">
-        <v>310</v>
-      </c>
-      <c r="H83" t="s">
-        <v>311</v>
+        <v>730</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="C84" t="s">
+        <v>777</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C85" t="s">
-        <v>500</v>
+        <v>312</v>
       </c>
       <c r="E85" t="s">
-        <v>219</v>
+        <v>308</v>
       </c>
       <c r="F85" t="s">
-        <v>220</v>
+        <v>309</v>
+      </c>
+      <c r="G85" t="s">
+        <v>310</v>
+      </c>
+      <c r="H85" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C87" t="s">
+        <v>499</v>
+      </c>
+      <c r="E87" t="s">
+        <v>219</v>
+      </c>
+      <c r="F87" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>122</v>
-      </c>
-      <c r="B90" t="s">
-        <v>6</v>
-      </c>
-      <c r="C90" t="s">
-        <v>74</v>
-      </c>
-      <c r="D90" t="s">
-        <v>72</v>
-      </c>
-      <c r="E90" t="s">
-        <v>70</v>
-      </c>
-      <c r="F90" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B92" t="s">
+        <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>613</v>
+        <v>74</v>
+      </c>
+      <c r="D92" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" t="s">
+        <v>70</v>
+      </c>
+      <c r="F92" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>127</v>
-      </c>
-      <c r="B93" t="s">
-        <v>7</v>
-      </c>
-      <c r="C93" t="s">
-        <v>20</v>
-      </c>
-      <c r="D93" t="s">
-        <v>22</v>
-      </c>
-      <c r="E93" t="s">
-        <v>21</v>
-      </c>
-      <c r="F93" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C94" t="s">
-        <v>771</v>
+        <v>612</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>135</v>
+        <v>127</v>
+      </c>
+      <c r="B95" t="s">
+        <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>620</v>
+        <v>20</v>
+      </c>
+      <c r="D95" t="s">
+        <v>22</v>
+      </c>
+      <c r="E95" t="s">
+        <v>21</v>
+      </c>
+      <c r="F95" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
+        <v>134</v>
+      </c>
+      <c r="C96" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>135</v>
+      </c>
+      <c r="C97" t="s">
+        <v>771</v>
+      </c>
+      <c r="E97" t="s">
+        <v>219</v>
+      </c>
+      <c r="F97" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98">
         <v>136</v>
       </c>
-      <c r="C96" t="s">
-        <v>607</v>
-      </c>
-      <c r="E96" t="s">
+      <c r="C98" t="s">
+        <v>606</v>
+      </c>
+      <c r="E98" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99">
         <v>137</v>
       </c>
-      <c r="C97" t="s">
-        <v>577</v>
+      <c r="C99" t="s">
+        <v>576</v>
       </c>
     </row>
   </sheetData>
@@ -23118,8 +23164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23132,7 +23178,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -23140,7 +23186,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -23148,7 +23194,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -23156,60 +23202,60 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>582</v>
+        <v>373</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>726</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>740</v>
+        <v>581</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>581</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>631</v>
+        <v>738</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>618</v>
+        <v>580</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>629</v>
@@ -23217,175 +23263,175 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>441</v>
+        <v>712</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>561</v>
+        <v>711</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>578</v>
+        <v>710</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>580</v>
+        <v>617</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>602</v>
+        <v>627</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>587</v>
+        <v>744</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>632</v>
+        <v>745</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>441</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>712</v>
+        <v>560</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>713</v>
+        <v>577</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>714</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>728</v>
+        <v>751</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>373</v>
+        <v>737</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>739</v>
+        <v>746</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>744</v>
+        <v>579</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>745</v>
+        <v>601</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>747</v>
+        <v>586</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>748</v>
+        <v>630</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>753</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>414</v>
+        <v>743</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B19">
-    <sortCondition ref="A2:A19"/>
+  <sortState ref="A2:B32">
+    <sortCondition ref="A2:A32"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -23395,8 +23441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="C386" sqref="C386"/>
+    <sheetView topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C142" sqref="C142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23423,7 +23469,7 @@
         <v>394</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>52</v>
@@ -23504,7 +23550,7 @@
         <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -23772,7 +23818,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -23786,7 +23832,7 @@
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -23921,7 +23967,7 @@
         <v>392</v>
       </c>
       <c r="D43" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -23946,7 +23992,7 @@
         <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -23960,7 +24006,7 @@
         <v>362</v>
       </c>
       <c r="D46" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -23996,7 +24042,7 @@
         <v>365</v>
       </c>
       <c r="D49" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -24076,7 +24122,7 @@
         <v>10</v>
       </c>
       <c r="D56" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -24093,7 +24139,7 @@
         <v>468</v>
       </c>
       <c r="E57" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -24184,7 +24230,7 @@
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -24209,7 +24255,7 @@
         <v>380</v>
       </c>
       <c r="D67" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -24253,10 +24299,10 @@
         <v>106</v>
       </c>
       <c r="C71" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="D71" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -24267,7 +24313,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -24281,7 +24327,7 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -24295,7 +24341,7 @@
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -24507,7 +24553,7 @@
         <v>370</v>
       </c>
       <c r="D93" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -24694,7 +24740,7 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -24705,7 +24751,7 @@
         <v>36</v>
       </c>
       <c r="C111" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -24738,7 +24784,7 @@
         <v>269</v>
       </c>
       <c r="C114" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -24782,7 +24828,7 @@
         <v>342</v>
       </c>
       <c r="C118" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -24793,7 +24839,7 @@
         <v>344</v>
       </c>
       <c r="C119" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -24848,7 +24894,7 @@
         <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -24859,7 +24905,7 @@
         <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24870,7 +24916,7 @@
         <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24881,7 +24927,7 @@
         <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24975,7 +25021,7 @@
         <v>361</v>
       </c>
       <c r="C135" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
@@ -24986,7 +25032,7 @@
         <v>350</v>
       </c>
       <c r="C136" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -25052,7 +25098,7 @@
         <v>165</v>
       </c>
       <c r="C142" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -25063,7 +25109,7 @@
         <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -25074,7 +25120,7 @@
         <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -25085,7 +25131,7 @@
         <v>362</v>
       </c>
       <c r="C145" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -25096,7 +25142,7 @@
         <v>363</v>
       </c>
       <c r="C146" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -25107,7 +25153,7 @@
         <v>364</v>
       </c>
       <c r="C147" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -25118,7 +25164,7 @@
         <v>365</v>
       </c>
       <c r="C148" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -25129,7 +25175,7 @@
         <v>366</v>
       </c>
       <c r="C149" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -25151,10 +25197,10 @@
         <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="D151" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -25165,7 +25211,7 @@
         <v>399</v>
       </c>
       <c r="C152" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -25176,7 +25222,7 @@
         <v>401</v>
       </c>
       <c r="C153" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -25187,7 +25233,7 @@
         <v>415</v>
       </c>
       <c r="C154" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -25487,7 +25533,7 @@
         <v>476</v>
       </c>
       <c r="D181" t="s">
-        <v>483</v>
+        <v>772</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -25575,7 +25621,7 @@
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -25586,7 +25632,7 @@
         <v>170</v>
       </c>
       <c r="C190" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -25597,7 +25643,7 @@
         <v>171</v>
       </c>
       <c r="C191" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -25608,7 +25654,7 @@
         <v>172</v>
       </c>
       <c r="C192" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -25619,7 +25665,7 @@
         <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -25630,7 +25676,7 @@
         <v>174</v>
       </c>
       <c r="C194" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -25641,7 +25687,7 @@
         <v>367</v>
       </c>
       <c r="C195" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -25652,7 +25698,7 @@
         <v>368</v>
       </c>
       <c r="C196" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -25729,7 +25775,7 @@
         <v>215</v>
       </c>
       <c r="C203" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -25740,7 +25786,7 @@
         <v>216</v>
       </c>
       <c r="C204" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -25751,7 +25797,7 @@
         <v>217</v>
       </c>
       <c r="C205" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -25762,7 +25808,7 @@
         <v>218</v>
       </c>
       <c r="C206" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -25773,7 +25819,7 @@
         <v>219</v>
       </c>
       <c r="C207" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -25784,7 +25830,7 @@
         <v>220</v>
       </c>
       <c r="C208" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -25795,7 +25841,7 @@
         <v>431</v>
       </c>
       <c r="C209" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -25806,7 +25852,7 @@
         <v>432</v>
       </c>
       <c r="C210" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -25817,7 +25863,7 @@
         <v>433</v>
       </c>
       <c r="C211" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -25828,7 +25874,7 @@
         <v>434</v>
       </c>
       <c r="C212" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -25839,7 +25885,7 @@
         <v>435</v>
       </c>
       <c r="C213" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -25850,7 +25896,7 @@
         <v>436</v>
       </c>
       <c r="C214" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -25875,10 +25921,10 @@
         <v>462</v>
       </c>
       <c r="D216" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="E216" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -25889,7 +25935,7 @@
         <v>74</v>
       </c>
       <c r="C217" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -25911,7 +25957,7 @@
         <v>294</v>
       </c>
       <c r="C219" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -25933,7 +25979,7 @@
         <v>296</v>
       </c>
       <c r="C221" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -25944,7 +25990,7 @@
         <v>297</v>
       </c>
       <c r="C222" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -25966,7 +26012,7 @@
         <v>299</v>
       </c>
       <c r="C224" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -25977,7 +26023,7 @@
         <v>301</v>
       </c>
       <c r="C225" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -25999,7 +26045,7 @@
         <v>437</v>
       </c>
       <c r="C227" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -26010,7 +26056,7 @@
         <v>438</v>
       </c>
       <c r="C228" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -26032,7 +26078,7 @@
         <v>131</v>
       </c>
       <c r="C230" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -26065,7 +26111,7 @@
         <v>439</v>
       </c>
       <c r="C233" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -26076,7 +26122,7 @@
         <v>194</v>
       </c>
       <c r="C234" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -26087,7 +26133,7 @@
         <v>393</v>
       </c>
       <c r="C235" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -26098,7 +26144,7 @@
         <v>394</v>
       </c>
       <c r="C236" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -26109,7 +26155,7 @@
         <v>396</v>
       </c>
       <c r="C237" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -26120,7 +26166,7 @@
         <v>397</v>
       </c>
       <c r="C238" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -26131,7 +26177,7 @@
         <v>238</v>
       </c>
       <c r="C239" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
@@ -26263,7 +26309,7 @@
         <v>177</v>
       </c>
       <c r="C251" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -26274,7 +26320,7 @@
         <v>176</v>
       </c>
       <c r="C252" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -26285,7 +26331,7 @@
         <v>372</v>
       </c>
       <c r="C253" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -26296,7 +26342,7 @@
         <v>376</v>
       </c>
       <c r="C254" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -26307,7 +26353,7 @@
         <v>412</v>
       </c>
       <c r="C255" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -26318,7 +26364,7 @@
         <v>369</v>
       </c>
       <c r="C256" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -26329,7 +26375,7 @@
         <v>370</v>
       </c>
       <c r="C257" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -26340,7 +26386,7 @@
         <v>371</v>
       </c>
       <c r="C258" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -26351,7 +26397,7 @@
         <v>373</v>
       </c>
       <c r="C259" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -26362,7 +26408,7 @@
         <v>374</v>
       </c>
       <c r="C260" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -26373,7 +26419,7 @@
         <v>375</v>
       </c>
       <c r="C261" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -26384,7 +26430,7 @@
         <v>377</v>
       </c>
       <c r="C262" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -26406,7 +26452,7 @@
         <v>382</v>
       </c>
       <c r="C264" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -26417,7 +26463,7 @@
         <v>383</v>
       </c>
       <c r="C265" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -26428,7 +26474,7 @@
         <v>384</v>
       </c>
       <c r="C266" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -26439,7 +26485,7 @@
         <v>385</v>
       </c>
       <c r="C267" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -26450,7 +26496,7 @@
         <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -26681,7 +26727,7 @@
         <v>305</v>
       </c>
       <c r="C289" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -26692,7 +26738,7 @@
         <v>78</v>
       </c>
       <c r="C290" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -26714,7 +26760,7 @@
         <v>306</v>
       </c>
       <c r="C292" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -26725,7 +26771,7 @@
         <v>307</v>
       </c>
       <c r="C293" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -26736,7 +26782,7 @@
         <v>308</v>
       </c>
       <c r="C294" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -26747,7 +26793,7 @@
         <v>77</v>
       </c>
       <c r="C295" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -26827,7 +26873,7 @@
         <v>30</v>
       </c>
       <c r="E302" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="303" spans="1:5" x14ac:dyDescent="0.25">
@@ -26915,7 +26961,7 @@
         <v>68</v>
       </c>
       <c r="C310" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -26937,7 +26983,7 @@
         <v>292</v>
       </c>
       <c r="C312" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
@@ -26948,7 +26994,7 @@
         <v>211</v>
       </c>
       <c r="C313" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -26959,7 +27005,7 @@
         <v>67</v>
       </c>
       <c r="C314" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -26970,7 +27016,7 @@
         <v>290</v>
       </c>
       <c r="C315" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -26981,7 +27027,7 @@
         <v>291</v>
       </c>
       <c r="C316" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -26992,7 +27038,7 @@
         <v>410</v>
       </c>
       <c r="C317" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -27003,7 +27049,7 @@
         <v>409</v>
       </c>
       <c r="C318" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -27025,7 +27071,7 @@
         <v>232</v>
       </c>
       <c r="C320" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -27036,7 +27082,7 @@
         <v>402</v>
       </c>
       <c r="C321" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -27047,7 +27093,7 @@
         <v>407</v>
       </c>
       <c r="C322" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -27058,7 +27104,7 @@
         <v>404</v>
       </c>
       <c r="C323" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -27069,7 +27115,7 @@
         <v>405</v>
       </c>
       <c r="C324" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -27091,7 +27137,7 @@
         <v>406</v>
       </c>
       <c r="C326" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -27102,7 +27148,7 @@
         <v>32</v>
       </c>
       <c r="C327" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -27113,10 +27159,10 @@
         <v>33</v>
       </c>
       <c r="C328" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D328" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -27127,7 +27173,7 @@
         <v>213</v>
       </c>
       <c r="C329" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -27138,7 +27184,7 @@
         <v>267</v>
       </c>
       <c r="C330" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -27182,7 +27228,7 @@
         <v>137</v>
       </c>
       <c r="C334" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="335" spans="1:4" x14ac:dyDescent="0.25">
@@ -27193,7 +27239,7 @@
         <v>418</v>
       </c>
       <c r="C335" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="336" spans="1:4" x14ac:dyDescent="0.25">
@@ -27204,7 +27250,7 @@
         <v>419</v>
       </c>
       <c r="C336" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -27215,7 +27261,7 @@
         <v>420</v>
       </c>
       <c r="C337" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -27226,7 +27272,7 @@
         <v>421</v>
       </c>
       <c r="C338" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -27248,7 +27294,7 @@
         <v>145</v>
       </c>
       <c r="C340" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -27259,7 +27305,7 @@
         <v>349</v>
       </c>
       <c r="C341" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -27270,7 +27316,7 @@
         <v>351</v>
       </c>
       <c r="C342" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -27281,7 +27327,7 @@
         <v>352</v>
       </c>
       <c r="C343" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -27292,7 +27338,7 @@
         <v>350</v>
       </c>
       <c r="C344" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -27303,7 +27349,7 @@
         <v>408</v>
       </c>
       <c r="C345" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -27369,7 +27415,7 @@
         <v>203</v>
       </c>
       <c r="C351" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -27380,10 +27426,10 @@
         <v>7</v>
       </c>
       <c r="C352" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D352" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -27394,10 +27440,10 @@
         <v>8</v>
       </c>
       <c r="C353" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D353" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -27408,10 +27454,10 @@
         <v>9</v>
       </c>
       <c r="C354" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D354" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -27422,10 +27468,10 @@
         <v>10</v>
       </c>
       <c r="C355" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D355" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -27436,10 +27482,10 @@
         <v>11</v>
       </c>
       <c r="C356" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D356" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -27450,7 +27496,7 @@
         <v>73</v>
       </c>
       <c r="C357" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -27461,7 +27507,7 @@
         <v>140</v>
       </c>
       <c r="C358" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -27472,7 +27518,7 @@
         <v>141</v>
       </c>
       <c r="C359" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -27483,7 +27529,7 @@
         <v>142</v>
       </c>
       <c r="C360" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -27494,7 +27540,7 @@
         <v>199</v>
       </c>
       <c r="C361" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -27505,7 +27551,7 @@
         <v>205</v>
       </c>
       <c r="C362" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -27516,7 +27562,7 @@
         <v>206</v>
       </c>
       <c r="C363" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -27560,7 +27606,7 @@
         <v>94</v>
       </c>
       <c r="C367" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -27571,7 +27617,7 @@
         <v>95</v>
       </c>
       <c r="C368" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -27582,7 +27628,7 @@
         <v>96</v>
       </c>
       <c r="C369" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -27593,7 +27639,7 @@
         <v>97</v>
       </c>
       <c r="C370" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -27604,7 +27650,7 @@
         <v>314</v>
       </c>
       <c r="C371" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
@@ -27615,7 +27661,7 @@
         <v>98</v>
       </c>
       <c r="C372" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -27637,7 +27683,7 @@
         <v>63</v>
       </c>
       <c r="C374" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -27648,7 +27694,7 @@
         <v>64</v>
       </c>
       <c r="C375" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -27692,7 +27738,7 @@
         <v>283</v>
       </c>
       <c r="C379" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -27703,7 +27749,7 @@
         <v>284</v>
       </c>
       <c r="C380" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -27714,7 +27760,7 @@
         <v>285</v>
       </c>
       <c r="C381" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -27725,7 +27771,7 @@
         <v>286</v>
       </c>
       <c r="C382" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -27736,7 +27782,7 @@
         <v>441</v>
       </c>
       <c r="C383" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -27747,7 +27793,7 @@
         <v>184</v>
       </c>
       <c r="C384" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -27758,7 +27804,7 @@
         <v>185</v>
       </c>
       <c r="C385" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -27769,7 +27815,7 @@
         <v>186</v>
       </c>
       <c r="C386" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -27780,7 +27826,7 @@
         <v>187</v>
       </c>
       <c r="C387" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -27791,7 +27837,7 @@
         <v>188</v>
       </c>
       <c r="C388" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -27846,7 +27892,7 @@
         <v>227</v>
       </c>
       <c r="C393" t="s">
-        <v>564</v>
+        <v>773</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -27857,7 +27903,7 @@
         <v>228</v>
       </c>
       <c r="C394" t="s">
-        <v>564</v>
+        <v>774</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -27868,7 +27914,7 @@
         <v>229</v>
       </c>
       <c r="C395" t="s">
-        <v>564</v>
+        <v>775</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -27879,7 +27925,7 @@
         <v>230</v>
       </c>
       <c r="C396" t="s">
-        <v>564</v>
+        <v>776</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -27890,7 +27936,7 @@
         <v>249</v>
       </c>
       <c r="C397" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -27901,7 +27947,7 @@
         <v>242</v>
       </c>
       <c r="C398" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -27912,7 +27958,7 @@
         <v>274</v>
       </c>
       <c r="C399" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -28151,7 +28197,7 @@
         <v>16</v>
       </c>
       <c r="C424" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -28162,7 +28208,7 @@
         <v>15</v>
       </c>
       <c r="C425" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
@@ -28173,7 +28219,7 @@
         <v>14</v>
       </c>
       <c r="C426" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -28184,7 +28230,7 @@
         <v>13</v>
       </c>
       <c r="C427" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -28205,7 +28251,7 @@
         <v>442</v>
       </c>
       <c r="C430" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -28216,7 +28262,7 @@
         <v>443</v>
       </c>
       <c r="C431" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -28227,7 +28273,7 @@
         <v>444</v>
       </c>
       <c r="C432" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -28238,7 +28284,7 @@
         <v>143</v>
       </c>
       <c r="C433" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -28282,7 +28328,7 @@
         <v>353</v>
       </c>
       <c r="C437" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -28309,7 +28355,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28342,7 +28388,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="B3">
         <v>5235</v>
@@ -28362,13 +28408,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B4">
         <v>3621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D4">
         <v>1230</v>
@@ -28382,7 +28428,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="B5">
         <v>3412</v>
@@ -28397,7 +28443,7 @@
         <v>1977</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Room 2 andd 3 objects named
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22110" windowHeight="10260" activeTab="5"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22110" windowHeight="10260" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Scripts!$A$1:$F$149</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="781">
   <si>
     <t>Purpose</t>
   </si>
@@ -1183,18 +1184,9 @@
     <t>Exposed cooling rods</t>
   </si>
   <si>
-    <t>Old Fashion</t>
-  </si>
-  <si>
     <t>Old Rusty Key</t>
   </si>
   <si>
-    <t>Broken Chandelleer</t>
-  </si>
-  <si>
-    <t>Glass Chandeleer</t>
-  </si>
-  <si>
     <t>Couch</t>
   </si>
   <si>
@@ -2369,6 +2361,24 @@
   </si>
   <si>
     <t>08 = Flag Raised</t>
+  </si>
+  <si>
+    <t>08 = Moved</t>
+  </si>
+  <si>
+    <t>Envelope: Addressed</t>
+  </si>
+  <si>
+    <t>04 = Locked</t>
+  </si>
+  <si>
+    <t>Old Fashion Radio</t>
+  </si>
+  <si>
+    <t>Broken Chandelier</t>
+  </si>
+  <si>
+    <t>Glass Chandelier</t>
   </si>
 </sst>
 </file>
@@ -2700,7 +2710,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2924,8 +2934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2942,10 +2952,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2953,7 +2963,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -2967,7 +2977,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
@@ -2981,7 +2991,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>
@@ -2995,7 +3005,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="C5" t="s">
         <v>18</v>
@@ -3009,13 +3019,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3023,7 +3033,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -3037,7 +3047,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="C8" t="s">
         <v>18</v>
@@ -3051,7 +3061,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -3065,7 +3075,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="C10" t="s">
         <v>18</v>
@@ -3079,7 +3089,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="C11" t="s">
         <v>18</v>
@@ -3093,7 +3103,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
@@ -3107,7 +3117,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="C13" t="s">
         <v>18</v>
@@ -3121,7 +3131,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -3135,7 +3145,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -3149,7 +3159,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -3163,7 +3173,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C17" t="s">
         <v>2</v>
@@ -3177,7 +3187,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -3191,7 +3201,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -3205,7 +3215,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -3219,7 +3229,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -3247,7 +3257,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -3261,7 +3271,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -3275,7 +3285,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -3289,7 +3299,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -3303,7 +3313,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -3317,7 +3327,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -3331,7 +3341,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -3345,7 +3355,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="C30" t="s">
         <v>2</v>
@@ -3359,7 +3369,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -3373,7 +3383,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -3387,7 +3397,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="C33" t="s">
         <v>2</v>
@@ -3401,7 +3411,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C34" t="s">
         <v>2</v>
@@ -3415,7 +3425,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C35" t="s">
         <v>2</v>
@@ -3429,7 +3439,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C36" t="s">
         <v>2</v>
@@ -3443,7 +3453,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -3457,7 +3467,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C38" t="s">
         <v>18</v>
@@ -3471,7 +3481,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="C39" t="s">
         <v>18</v>
@@ -3485,7 +3495,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C40" t="s">
         <v>18</v>
@@ -3499,7 +3509,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C41" t="s">
         <v>2</v>
@@ -3513,7 +3523,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="C42" t="s">
         <v>2</v>
@@ -3527,7 +3537,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="C43" t="s">
         <v>2</v>
@@ -3541,7 +3551,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="C44" t="s">
         <v>18</v>
@@ -3555,7 +3565,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="C45" t="s">
         <v>2</v>
@@ -3569,7 +3579,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -3583,7 +3593,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C47" t="s">
         <v>2</v>
@@ -3597,7 +3607,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C48" t="s">
         <v>2</v>
@@ -3611,7 +3621,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C49" t="s">
         <v>2</v>
@@ -3625,7 +3635,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C50" t="s">
         <v>2</v>
@@ -3639,7 +3649,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
@@ -3653,7 +3663,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C52" t="s">
         <v>18</v>
@@ -3667,7 +3677,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
@@ -3686,8 +3696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3739,7 +3749,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3761,7 +3771,7 @@
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3772,7 +3782,7 @@
         <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3783,7 +3793,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3794,7 +3804,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3805,7 +3815,7 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3838,7 +3848,7 @@
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3849,7 +3859,7 @@
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -3860,7 +3870,7 @@
         <v>18</v>
       </c>
       <c r="D14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -3871,7 +3881,7 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3882,7 +3892,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3992,7 +4002,7 @@
         <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -4003,7 +4013,7 @@
         <v>18</v>
       </c>
       <c r="D27" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -4014,7 +4024,7 @@
         <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -4025,7 +4035,7 @@
         <v>18</v>
       </c>
       <c r="D29" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -4075,7 +4085,7 @@
         <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="E33" t="s">
         <v>83</v>
@@ -4089,7 +4099,7 @@
         <v>18</v>
       </c>
       <c r="D34" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -4100,7 +4110,7 @@
         <v>18</v>
       </c>
       <c r="D35" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="E35" t="s">
         <v>87</v>
@@ -4169,7 +4179,7 @@
         <v>2</v>
       </c>
       <c r="D41" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4219,7 +4229,7 @@
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -4241,7 +4251,7 @@
         <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4282,7 +4292,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="52" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4293,7 +4303,7 @@
         <v>18</v>
       </c>
       <c r="D52" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="53" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4304,7 +4314,7 @@
         <v>18</v>
       </c>
       <c r="D53" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="54" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4326,7 +4336,7 @@
         <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="56" spans="1:16384" x14ac:dyDescent="0.25">
@@ -4338,7 +4348,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -20729,7 +20739,7 @@
         <v>2</v>
       </c>
       <c r="D57" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="F57" t="s">
         <v>283</v>
@@ -20900,7 +20910,7 @@
         <v>18</v>
       </c>
       <c r="D72" t="s">
-        <v>745</v>
+        <v>742</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -20922,7 +20932,7 @@
         <v>18</v>
       </c>
       <c r="D74" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -20999,7 +21009,7 @@
         <v>18</v>
       </c>
       <c r="D81" t="s">
-        <v>750</v>
+        <v>747</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -21010,7 +21020,7 @@
         <v>18</v>
       </c>
       <c r="D82" t="s">
-        <v>751</v>
+        <v>748</v>
       </c>
       <c r="F82" t="s">
         <v>251</v>
@@ -21024,10 +21034,10 @@
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="F83" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -21093,7 +21103,7 @@
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -21101,7 +21111,7 @@
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>760</v>
+        <v>757</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -21228,7 +21238,7 @@
         <v>18</v>
       </c>
       <c r="D101" t="s">
-        <v>773</v>
+        <v>770</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -21239,7 +21249,7 @@
         <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="F102" t="s">
         <v>273</v>
@@ -21286,7 +21296,7 @@
         <v>18</v>
       </c>
       <c r="D106" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -21297,7 +21307,7 @@
         <v>18</v>
       </c>
       <c r="D107" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -21319,7 +21329,7 @@
         <v>18</v>
       </c>
       <c r="D109" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -21352,7 +21362,7 @@
         <v>18</v>
       </c>
       <c r="D112" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -21402,7 +21412,7 @@
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="E116" t="s">
         <v>88</v>
@@ -21471,7 +21481,7 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -21609,10 +21619,10 @@
         <v>18</v>
       </c>
       <c r="D134" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="F134" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
@@ -21667,7 +21677,7 @@
         <v>18</v>
       </c>
       <c r="D139" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
@@ -21700,10 +21710,10 @@
         <v>18</v>
       </c>
       <c r="D142" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="F142" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
@@ -21714,7 +21724,7 @@
         <v>18</v>
       </c>
       <c r="D143" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
@@ -21739,7 +21749,7 @@
         <v>18</v>
       </c>
       <c r="D145" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -21772,7 +21782,7 @@
         <v>18</v>
       </c>
       <c r="D148" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="E148" t="s">
         <v>78</v>
@@ -21858,7 +21868,7 @@
         <v>18</v>
       </c>
       <c r="D155" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -21869,7 +21879,7 @@
         <v>18</v>
       </c>
       <c r="D156" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -21880,7 +21890,7 @@
         <v>18</v>
       </c>
       <c r="D157" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="E157" t="s">
         <v>329</v>
@@ -21906,10 +21916,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21957,10 +21967,10 @@
         <v>219</v>
       </c>
       <c r="G2" t="s">
-        <v>748</v>
+        <v>745</v>
       </c>
       <c r="H2" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -22025,16 +22035,16 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D6" t="s">
         <v>80</v>
       </c>
       <c r="E6" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="F6" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -22042,10 +22052,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="F7" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="G7" t="s">
         <v>299</v>
@@ -22075,19 +22085,19 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
+        <v>614</v>
+      </c>
+      <c r="E10" t="s">
+        <v>615</v>
+      </c>
+      <c r="F10" t="s">
+        <v>616</v>
+      </c>
+      <c r="G10" t="s">
         <v>617</v>
       </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>618</v>
-      </c>
-      <c r="F10" t="s">
-        <v>619</v>
-      </c>
-      <c r="G10" t="s">
-        <v>620</v>
-      </c>
-      <c r="H10" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -22101,13 +22111,13 @@
         <v>230</v>
       </c>
       <c r="F11" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G11" t="s">
         <v>241</v>
       </c>
       <c r="H11" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -22135,13 +22145,13 @@
         <v>230</v>
       </c>
       <c r="F13" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G13" t="s">
         <v>241</v>
       </c>
       <c r="H13" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -22149,7 +22159,7 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="E14" t="s">
         <v>218</v>
@@ -22169,13 +22179,13 @@
         <v>230</v>
       </c>
       <c r="F15" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="G15" t="s">
         <v>241</v>
       </c>
       <c r="H15" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -22183,19 +22193,19 @@
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>725</v>
+      </c>
+      <c r="E16" t="s">
+        <v>726</v>
+      </c>
+      <c r="F16" t="s">
+        <v>727</v>
+      </c>
+      <c r="G16" t="s">
         <v>728</v>
       </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>729</v>
-      </c>
-      <c r="F16" t="s">
-        <v>730</v>
-      </c>
-      <c r="G16" t="s">
-        <v>731</v>
-      </c>
-      <c r="H16" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -22203,16 +22213,16 @@
         <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="E17" t="s">
         <v>218</v>
       </c>
       <c r="F17" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="G17" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -22348,7 +22358,7 @@
         <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -22359,7 +22369,7 @@
         <v>120</v>
       </c>
       <c r="D35" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="E35" t="s">
         <v>121</v>
@@ -22393,7 +22403,7 @@
         <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="E37" t="s">
         <v>218</v>
@@ -22407,7 +22417,7 @@
         <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="E38" t="s">
         <v>296</v>
@@ -22497,7 +22507,7 @@
         <v>63</v>
       </c>
       <c r="C45" t="s">
-        <v>776</v>
+        <v>773</v>
       </c>
       <c r="E45" t="s">
         <v>230</v>
@@ -22514,7 +22524,7 @@
         <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>774</v>
+        <v>771</v>
       </c>
       <c r="E46" t="s">
         <v>218</v>
@@ -22528,7 +22538,7 @@
         <v>65</v>
       </c>
       <c r="C47" t="s">
-        <v>775</v>
+        <v>772</v>
       </c>
       <c r="E47" t="s">
         <v>218</v>
@@ -22548,7 +22558,7 @@
         <v>230</v>
       </c>
       <c r="F48" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="G48" t="s">
         <v>231</v>
@@ -22562,7 +22572,7 @@
         <v>67</v>
       </c>
       <c r="C49" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -22593,10 +22603,10 @@
         <v>7</v>
       </c>
       <c r="C51" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E51" t="s">
-        <v>753</v>
+        <v>750</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -22607,10 +22617,10 @@
         <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>752</v>
+        <v>749</v>
       </c>
       <c r="E52" t="s">
-        <v>754</v>
+        <v>751</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -22621,7 +22631,7 @@
         <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>756</v>
+        <v>753</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -22632,7 +22642,7 @@
         <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>757</v>
+        <v>754</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -22652,7 +22662,7 @@
         <v>257</v>
       </c>
       <c r="G55" t="s">
-        <v>762</v>
+        <v>759</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -22660,7 +22670,7 @@
         <v>74</v>
       </c>
       <c r="C56" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="E56" t="s">
         <v>219</v>
@@ -22671,7 +22681,7 @@
         <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="E57" t="s">
         <v>280</v>
@@ -22688,7 +22698,7 @@
         <v>206</v>
       </c>
       <c r="F58" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="G58" t="s">
         <v>207</v>
@@ -22705,7 +22715,7 @@
         <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="E59" t="s">
         <v>211</v>
@@ -22758,7 +22768,7 @@
         <v>82</v>
       </c>
       <c r="C63" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="E63" t="s">
         <v>287</v>
@@ -22770,7 +22780,7 @@
         <v>286</v>
       </c>
       <c r="H63" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -22778,377 +22788,391 @@
         <v>83</v>
       </c>
       <c r="C64" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>84</v>
       </c>
       <c r="C65" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E65" t="s">
         <v>218</v>
       </c>
       <c r="F65" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
+        <v>85</v>
+      </c>
+      <c r="C66" t="s">
+        <v>776</v>
+      </c>
+      <c r="E66" t="s">
+        <v>218</v>
+      </c>
+      <c r="F66" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67">
         <v>87</v>
       </c>
-      <c r="C66" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="C67" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68">
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>90</v>
-      </c>
-      <c r="D68" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>90</v>
       </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>90</v>
+      </c>
+      <c r="B70" t="s">
         <v>7</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>91</v>
-      </c>
-      <c r="D70" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>91</v>
       </c>
-      <c r="B71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71" t="s">
-        <v>101</v>
-      </c>
       <c r="D71" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D72" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
+        <v>92</v>
+      </c>
+      <c r="B73" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74">
         <v>94</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75">
         <v>96</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>217</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E75" t="s">
         <v>218</v>
       </c>
-      <c r="F74" t="s">
+      <c r="F75" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76">
         <v>97</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C76" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77">
         <v>98</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C77" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78">
         <v>99</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79">
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80">
         <v>102</v>
       </c>
-      <c r="C79" t="s">
-        <v>755</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="C80" t="s">
+        <v>752</v>
+      </c>
+      <c r="E80" t="s">
         <v>218</v>
       </c>
-      <c r="F79" t="s">
+      <c r="F80" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>103</v>
-      </c>
-      <c r="C80" t="s">
-        <v>719</v>
-      </c>
-      <c r="D80" t="s">
-        <v>74</v>
-      </c>
-      <c r="E80" t="s">
-        <v>75</v>
-      </c>
-      <c r="F80" t="s">
-        <v>716</v>
-      </c>
-      <c r="G80" t="s">
-        <v>715</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C81" t="s">
-        <v>765</v>
+        <v>716</v>
+      </c>
+      <c r="D81" t="s">
+        <v>74</v>
       </c>
       <c r="E81" t="s">
-        <v>218</v>
+        <v>75</v>
       </c>
       <c r="F81" t="s">
-        <v>219</v>
+        <v>713</v>
+      </c>
+      <c r="G81" t="s">
+        <v>712</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>105</v>
-      </c>
-      <c r="B82" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C82" t="s">
-        <v>128</v>
+        <v>762</v>
+      </c>
+      <c r="E82" t="s">
+        <v>218</v>
+      </c>
+      <c r="F82" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B83" t="s">
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>724</v>
-      </c>
-      <c r="E83" t="s">
-        <v>725</v>
-      </c>
-      <c r="F83" t="s">
-        <v>127</v>
-      </c>
-      <c r="G83" t="s">
-        <v>726</v>
+        <v>128</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B84" t="s">
+        <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>772</v>
+        <v>721</v>
+      </c>
+      <c r="E84" t="s">
+        <v>722</v>
+      </c>
+      <c r="F84" t="s">
+        <v>127</v>
+      </c>
+      <c r="G84" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C85" t="s">
-        <v>309</v>
-      </c>
-      <c r="E85" t="s">
-        <v>305</v>
-      </c>
-      <c r="F85" t="s">
-        <v>306</v>
-      </c>
-      <c r="G85" t="s">
-        <v>307</v>
-      </c>
-      <c r="H85" t="s">
-        <v>308</v>
+        <v>769</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C86" t="s">
+        <v>309</v>
+      </c>
+      <c r="E86" t="s">
+        <v>305</v>
+      </c>
+      <c r="F86" t="s">
+        <v>306</v>
+      </c>
+      <c r="G86" t="s">
+        <v>307</v>
+      </c>
+      <c r="H86" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>110</v>
-      </c>
-      <c r="C87" t="s">
-        <v>495</v>
-      </c>
-      <c r="E87" t="s">
-        <v>218</v>
-      </c>
-      <c r="F87" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C88" t="s">
+        <v>492</v>
+      </c>
+      <c r="E88" t="s">
+        <v>218</v>
+      </c>
+      <c r="F88" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>122</v>
-      </c>
-      <c r="B92" t="s">
-        <v>6</v>
-      </c>
-      <c r="C92" t="s">
-        <v>73</v>
-      </c>
-      <c r="D92" t="s">
-        <v>71</v>
-      </c>
-      <c r="E92" t="s">
-        <v>69</v>
-      </c>
-      <c r="F92" t="s">
-        <v>70</v>
+        <v>117</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B93" t="s">
+        <v>6</v>
+      </c>
+      <c r="C93" t="s">
+        <v>73</v>
+      </c>
+      <c r="D93" t="s">
+        <v>71</v>
+      </c>
+      <c r="E93" t="s">
+        <v>69</v>
+      </c>
+      <c r="F93" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>126</v>
       </c>
-      <c r="C94" t="s">
-        <v>608</v>
-      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>127</v>
-      </c>
-      <c r="B95" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C95" t="s">
-        <v>20</v>
-      </c>
-      <c r="D95" t="s">
-        <v>22</v>
-      </c>
-      <c r="E95" t="s">
-        <v>21</v>
-      </c>
-      <c r="F95" t="s">
-        <v>26</v>
+        <v>605</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>134</v>
+        <v>127</v>
+      </c>
+      <c r="B96" t="s">
+        <v>7</v>
       </c>
       <c r="C96" t="s">
-        <v>764</v>
+        <v>20</v>
+      </c>
+      <c r="D96" t="s">
+        <v>22</v>
+      </c>
+      <c r="E96" t="s">
+        <v>21</v>
+      </c>
+      <c r="F96" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C97" t="s">
-        <v>766</v>
-      </c>
-      <c r="E97" t="s">
-        <v>218</v>
-      </c>
-      <c r="F97" t="s">
-        <v>219</v>
+        <v>761</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C98" t="s">
-        <v>602</v>
+        <v>763</v>
       </c>
       <c r="E98" t="s">
+        <v>218</v>
+      </c>
+      <c r="F98" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
+        <v>136</v>
+      </c>
+      <c r="C99" t="s">
+        <v>599</v>
+      </c>
+      <c r="E99" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100">
         <v>137</v>
       </c>
-      <c r="C99" t="s">
-        <v>572</v>
+      <c r="C100" t="s">
+        <v>569</v>
       </c>
     </row>
   </sheetData>
@@ -23178,7 +23202,7 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -23186,7 +23210,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -23194,7 +23218,7 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -23202,7 +23226,7 @@
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -23218,7 +23242,7 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -23226,7 +23250,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -23242,7 +23266,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -23250,7 +23274,7 @@
         <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -23258,7 +23282,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -23266,7 +23290,7 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -23274,7 +23298,7 @@
         <v>23</v>
       </c>
       <c r="B13" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -23282,7 +23306,7 @@
         <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -23290,7 +23314,7 @@
         <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -23298,7 +23322,7 @@
         <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -23306,7 +23330,7 @@
         <v>32</v>
       </c>
       <c r="B17" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -23314,7 +23338,7 @@
         <v>33</v>
       </c>
       <c r="B18" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -23322,7 +23346,7 @@
         <v>34</v>
       </c>
       <c r="B19" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -23330,7 +23354,7 @@
         <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -23338,7 +23362,7 @@
         <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -23346,7 +23370,7 @@
         <v>40</v>
       </c>
       <c r="B22" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -23354,7 +23378,7 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>747</v>
+        <v>744</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -23362,7 +23386,7 @@
         <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -23370,7 +23394,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -23378,7 +23402,7 @@
         <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -23386,7 +23410,7 @@
         <v>54</v>
       </c>
       <c r="B27" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -23394,7 +23418,7 @@
         <v>55</v>
       </c>
       <c r="B28" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -23402,7 +23426,7 @@
         <v>56</v>
       </c>
       <c r="B29" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -23410,7 +23434,7 @@
         <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -23426,7 +23450,7 @@
         <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -23441,8 +23465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23463,13 +23487,13 @@
         <v>9</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>51</v>
@@ -23485,6 +23509,9 @@
       <c r="C2" t="s">
         <v>45</v>
       </c>
+      <c r="D2" t="s">
+        <v>743</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -23497,7 +23524,7 @@
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>777</v>
+        <v>774</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -23538,6 +23565,9 @@
       <c r="C6" t="s">
         <v>39</v>
       </c>
+      <c r="D6" t="s">
+        <v>775</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -23549,6 +23579,9 @@
       <c r="C7" t="s">
         <v>66</v>
       </c>
+      <c r="D7" t="s">
+        <v>777</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -23572,7 +23605,7 @@
         <v>41</v>
       </c>
       <c r="D9" t="s">
-        <v>761</v>
+        <v>758</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -23821,7 +23854,7 @@
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -23832,7 +23865,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>382</v>
+        <v>778</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -23854,7 +23887,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>385</v>
+        <v>780</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -23865,7 +23898,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>384</v>
+        <v>779</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -23876,7 +23909,7 @@
         <v>43</v>
       </c>
       <c r="C35" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -23887,10 +23920,10 @@
         <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="D36" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -23923,7 +23956,7 @@
         <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -23937,7 +23970,7 @@
         <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -23948,7 +23981,7 @@
         <v>207</v>
       </c>
       <c r="C41" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -23959,7 +23992,7 @@
         <v>273</v>
       </c>
       <c r="C42" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -23984,7 +24017,7 @@
         <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -23998,7 +24031,7 @@
         <v>362</v>
       </c>
       <c r="D45" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -24034,7 +24067,7 @@
         <v>359</v>
       </c>
       <c r="D48" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -24114,7 +24147,7 @@
         <v>10</v>
       </c>
       <c r="D55" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -24125,13 +24158,13 @@
         <v>103</v>
       </c>
       <c r="C56" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D56" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="E56" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -24142,7 +24175,7 @@
         <v>156</v>
       </c>
       <c r="C57" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -24153,7 +24186,7 @@
         <v>235</v>
       </c>
       <c r="C58" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -24164,7 +24197,7 @@
         <v>315</v>
       </c>
       <c r="C59" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -24175,7 +24208,7 @@
         <v>316</v>
       </c>
       <c r="C60" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -24186,7 +24219,7 @@
         <v>318</v>
       </c>
       <c r="C61" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -24197,7 +24230,7 @@
         <v>319</v>
       </c>
       <c r="C62" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -24208,7 +24241,7 @@
         <v>320</v>
       </c>
       <c r="C63" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -24233,7 +24266,7 @@
         <v>10</v>
       </c>
       <c r="D65" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -24244,7 +24277,7 @@
         <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -24255,10 +24288,10 @@
         <v>106</v>
       </c>
       <c r="C67" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="D67" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -24283,7 +24316,7 @@
         <v>377</v>
       </c>
       <c r="D69" t="s">
-        <v>744</v>
+        <v>741</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -24316,7 +24349,7 @@
         <v>324</v>
       </c>
       <c r="C72" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -24330,7 +24363,7 @@
         <v>10</v>
       </c>
       <c r="D73" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -24344,7 +24377,7 @@
         <v>10</v>
       </c>
       <c r="D74" t="s">
-        <v>746</v>
+        <v>743</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -24355,7 +24388,7 @@
         <v>50</v>
       </c>
       <c r="C75" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -24377,7 +24410,7 @@
         <v>52</v>
       </c>
       <c r="C77" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -24399,7 +24432,7 @@
         <v>54</v>
       </c>
       <c r="C79" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -24410,7 +24443,7 @@
         <v>55</v>
       </c>
       <c r="C80" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -24421,7 +24454,10 @@
         <v>56</v>
       </c>
       <c r="C81" t="s">
-        <v>429</v>
+        <v>426</v>
+      </c>
+      <c r="D81" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -24432,7 +24468,7 @@
         <v>57</v>
       </c>
       <c r="C82" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -24443,7 +24479,7 @@
         <v>58</v>
       </c>
       <c r="C83" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -24454,7 +24490,7 @@
         <v>59</v>
       </c>
       <c r="C84" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -24465,7 +24501,7 @@
         <v>60</v>
       </c>
       <c r="C85" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -24476,7 +24512,7 @@
         <v>61</v>
       </c>
       <c r="C86" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -24487,7 +24523,7 @@
         <v>100</v>
       </c>
       <c r="C87" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -24498,7 +24534,7 @@
         <v>234</v>
       </c>
       <c r="C88" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -24520,7 +24556,7 @@
         <v>277</v>
       </c>
       <c r="C90" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -24531,7 +24567,7 @@
         <v>279</v>
       </c>
       <c r="C91" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -24542,7 +24578,7 @@
         <v>280</v>
       </c>
       <c r="C92" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -24589,7 +24625,7 @@
         <v>367</v>
       </c>
       <c r="D96" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -24655,7 +24691,7 @@
         <v>196</v>
       </c>
       <c r="C102" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -24666,7 +24702,7 @@
         <v>197</v>
       </c>
       <c r="C103" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -24677,7 +24713,7 @@
         <v>198</v>
       </c>
       <c r="C104" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -24688,7 +24724,7 @@
         <v>200</v>
       </c>
       <c r="C105" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -24699,7 +24735,7 @@
         <v>201</v>
       </c>
       <c r="C106" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -24721,7 +24757,7 @@
         <v>414</v>
       </c>
       <c r="C108" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -24743,7 +24779,7 @@
         <v>35</v>
       </c>
       <c r="C110" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -24754,7 +24790,7 @@
         <v>36</v>
       </c>
       <c r="C111" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -24787,7 +24823,7 @@
         <v>269</v>
       </c>
       <c r="C114" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -24798,7 +24834,7 @@
         <v>270</v>
       </c>
       <c r="C115" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -24809,7 +24845,7 @@
         <v>271</v>
       </c>
       <c r="C116" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -24831,7 +24867,7 @@
         <v>342</v>
       </c>
       <c r="C118" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
@@ -24842,7 +24878,7 @@
         <v>344</v>
       </c>
       <c r="C119" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
@@ -24897,7 +24933,7 @@
         <v>150</v>
       </c>
       <c r="C124" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
@@ -24908,7 +24944,7 @@
         <v>151</v>
       </c>
       <c r="C125" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -24919,7 +24955,7 @@
         <v>354</v>
       </c>
       <c r="C126" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
@@ -24930,7 +24966,7 @@
         <v>355</v>
       </c>
       <c r="C127" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
@@ -24958,7 +24994,7 @@
         <v>53</v>
       </c>
       <c r="H129" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -24980,7 +25016,7 @@
         <v>378</v>
       </c>
       <c r="C131" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -25068,7 +25104,7 @@
         <v>350</v>
       </c>
       <c r="C139" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
@@ -25079,7 +25115,7 @@
         <v>361</v>
       </c>
       <c r="C140" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -25101,7 +25137,7 @@
         <v>165</v>
       </c>
       <c r="C142" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -25112,7 +25148,7 @@
         <v>166</v>
       </c>
       <c r="C143" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -25123,7 +25159,7 @@
         <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -25134,7 +25170,7 @@
         <v>362</v>
       </c>
       <c r="C145" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -25145,7 +25181,7 @@
         <v>363</v>
       </c>
       <c r="C146" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -25156,7 +25192,7 @@
         <v>364</v>
       </c>
       <c r="C147" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -25167,7 +25203,7 @@
         <v>365</v>
       </c>
       <c r="C148" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -25178,7 +25214,7 @@
         <v>366</v>
       </c>
       <c r="C149" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -25189,7 +25225,7 @@
         <v>202</v>
       </c>
       <c r="C150" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -25200,10 +25236,10 @@
         <v>204</v>
       </c>
       <c r="C151" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="D151" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -25214,7 +25250,7 @@
         <v>399</v>
       </c>
       <c r="C152" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -25225,7 +25261,7 @@
         <v>401</v>
       </c>
       <c r="C153" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -25236,7 +25272,7 @@
         <v>415</v>
       </c>
       <c r="C154" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -25258,7 +25294,7 @@
         <v>26</v>
       </c>
       <c r="C156" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -25269,7 +25305,7 @@
         <v>101</v>
       </c>
       <c r="C157" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -25280,7 +25316,7 @@
         <v>110</v>
       </c>
       <c r="C158" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -25291,7 +25327,7 @@
         <v>111</v>
       </c>
       <c r="C159" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -25302,7 +25338,7 @@
         <v>112</v>
       </c>
       <c r="C160" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
@@ -25313,7 +25349,7 @@
         <v>113</v>
       </c>
       <c r="C161" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
@@ -25324,7 +25360,7 @@
         <v>114</v>
       </c>
       <c r="C162" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
@@ -25335,7 +25371,7 @@
         <v>115</v>
       </c>
       <c r="C163" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -25346,7 +25382,7 @@
         <v>116</v>
       </c>
       <c r="C164" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
@@ -25357,7 +25393,7 @@
         <v>117</v>
       </c>
       <c r="C165" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
@@ -25368,7 +25404,7 @@
         <v>118</v>
       </c>
       <c r="C166" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
@@ -25379,7 +25415,7 @@
         <v>119</v>
       </c>
       <c r="C167" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
@@ -25390,7 +25426,7 @@
         <v>120</v>
       </c>
       <c r="C168" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
@@ -25401,7 +25437,7 @@
         <v>153</v>
       </c>
       <c r="C169" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -25412,7 +25448,7 @@
         <v>268</v>
       </c>
       <c r="C170" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
@@ -25423,7 +25459,7 @@
         <v>330</v>
       </c>
       <c r="C171" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -25434,7 +25470,7 @@
         <v>331</v>
       </c>
       <c r="C172" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
@@ -25445,7 +25481,7 @@
         <v>332</v>
       </c>
       <c r="C173" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
@@ -25467,7 +25503,7 @@
         <v>334</v>
       </c>
       <c r="C175" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
@@ -25478,7 +25514,7 @@
         <v>335</v>
       </c>
       <c r="C176" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
@@ -25500,7 +25536,7 @@
         <v>154</v>
       </c>
       <c r="C178" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -25511,7 +25547,7 @@
         <v>155</v>
       </c>
       <c r="C179" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -25522,7 +25558,7 @@
         <v>157</v>
       </c>
       <c r="C180" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -25533,10 +25569,10 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D181" t="s">
-        <v>767</v>
+        <v>764</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -25547,7 +25583,7 @@
         <v>159</v>
       </c>
       <c r="C182" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -25558,7 +25594,7 @@
         <v>231</v>
       </c>
       <c r="C183" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
@@ -25569,7 +25605,7 @@
         <v>356</v>
       </c>
       <c r="C184" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -25580,7 +25616,7 @@
         <v>357</v>
       </c>
       <c r="C185" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -25591,7 +25627,7 @@
         <v>358</v>
       </c>
       <c r="C186" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -25602,7 +25638,7 @@
         <v>359</v>
       </c>
       <c r="C187" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -25624,7 +25660,7 @@
         <v>169</v>
       </c>
       <c r="C189" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
@@ -25635,7 +25671,7 @@
         <v>170</v>
       </c>
       <c r="C190" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
@@ -25646,7 +25682,7 @@
         <v>171</v>
       </c>
       <c r="C191" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -25657,7 +25693,7 @@
         <v>172</v>
       </c>
       <c r="C192" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
@@ -25668,7 +25704,7 @@
         <v>173</v>
       </c>
       <c r="C193" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
@@ -25679,7 +25715,7 @@
         <v>174</v>
       </c>
       <c r="C194" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
@@ -25690,7 +25726,7 @@
         <v>215</v>
       </c>
       <c r="C195" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
@@ -25701,7 +25737,7 @@
         <v>216</v>
       </c>
       <c r="C196" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
@@ -25712,7 +25748,7 @@
         <v>217</v>
       </c>
       <c r="C197" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
@@ -25723,7 +25759,7 @@
         <v>218</v>
       </c>
       <c r="C198" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
@@ -25734,7 +25770,7 @@
         <v>219</v>
       </c>
       <c r="C199" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -25745,7 +25781,7 @@
         <v>220</v>
       </c>
       <c r="C200" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
@@ -25756,7 +25792,7 @@
         <v>221</v>
       </c>
       <c r="C201" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
@@ -25767,7 +25803,7 @@
         <v>222</v>
       </c>
       <c r="C202" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
@@ -25778,7 +25814,7 @@
         <v>223</v>
       </c>
       <c r="C203" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
@@ -25789,7 +25825,7 @@
         <v>224</v>
       </c>
       <c r="C204" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
@@ -25800,7 +25836,7 @@
         <v>225</v>
       </c>
       <c r="C205" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
@@ -25811,7 +25847,7 @@
         <v>226</v>
       </c>
       <c r="C206" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
@@ -25822,7 +25858,7 @@
         <v>367</v>
       </c>
       <c r="C207" t="s">
-        <v>637</v>
+        <v>634</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
@@ -25833,7 +25869,7 @@
         <v>368</v>
       </c>
       <c r="C208" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -25844,7 +25880,7 @@
         <v>431</v>
       </c>
       <c r="C209" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
@@ -25855,7 +25891,7 @@
         <v>432</v>
       </c>
       <c r="C210" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
@@ -25866,7 +25902,7 @@
         <v>433</v>
       </c>
       <c r="C211" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -25877,7 +25913,7 @@
         <v>434</v>
       </c>
       <c r="C212" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -25888,7 +25924,7 @@
         <v>435</v>
       </c>
       <c r="C213" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -25899,7 +25935,7 @@
         <v>436</v>
       </c>
       <c r="C214" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
@@ -25921,13 +25957,13 @@
         <v>72</v>
       </c>
       <c r="C216" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="D216" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="E216" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
@@ -25938,7 +25974,7 @@
         <v>74</v>
       </c>
       <c r="C217" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.25">
@@ -25960,7 +25996,7 @@
         <v>294</v>
       </c>
       <c r="C219" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -25971,7 +26007,7 @@
         <v>295</v>
       </c>
       <c r="C220" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -25982,7 +26018,7 @@
         <v>296</v>
       </c>
       <c r="C221" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -25993,7 +26029,7 @@
         <v>297</v>
       </c>
       <c r="C222" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -26015,7 +26051,7 @@
         <v>299</v>
       </c>
       <c r="C224" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
@@ -26026,7 +26062,7 @@
         <v>301</v>
       </c>
       <c r="C225" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
@@ -26048,7 +26084,7 @@
         <v>437</v>
       </c>
       <c r="C227" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -26059,7 +26095,7 @@
         <v>438</v>
       </c>
       <c r="C228" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
@@ -26070,7 +26106,7 @@
         <v>131</v>
       </c>
       <c r="C229" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
@@ -26081,7 +26117,7 @@
         <v>192</v>
       </c>
       <c r="C230" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
@@ -26092,7 +26128,7 @@
         <v>194</v>
       </c>
       <c r="C231" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
@@ -26103,7 +26139,7 @@
         <v>195</v>
       </c>
       <c r="C232" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
@@ -26114,7 +26150,7 @@
         <v>235</v>
       </c>
       <c r="C233" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
@@ -26125,7 +26161,7 @@
         <v>238</v>
       </c>
       <c r="C234" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
@@ -26136,7 +26172,7 @@
         <v>393</v>
       </c>
       <c r="C235" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
@@ -26147,7 +26183,7 @@
         <v>394</v>
       </c>
       <c r="C236" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
@@ -26158,7 +26194,7 @@
         <v>396</v>
       </c>
       <c r="C237" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
@@ -26169,7 +26205,7 @@
         <v>397</v>
       </c>
       <c r="C238" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
@@ -26191,7 +26227,7 @@
         <v>439</v>
       </c>
       <c r="C240" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
@@ -26312,7 +26348,7 @@
         <v>176</v>
       </c>
       <c r="C251" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
@@ -26323,7 +26359,7 @@
         <v>177</v>
       </c>
       <c r="C252" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
@@ -26334,7 +26370,7 @@
         <v>369</v>
       </c>
       <c r="C253" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
@@ -26345,7 +26381,7 @@
         <v>370</v>
       </c>
       <c r="C254" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
@@ -26356,7 +26392,7 @@
         <v>371</v>
       </c>
       <c r="C255" t="s">
-        <v>674</v>
+        <v>671</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
@@ -26367,7 +26403,7 @@
         <v>372</v>
       </c>
       <c r="C256" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
@@ -26378,7 +26414,7 @@
         <v>373</v>
       </c>
       <c r="C257" t="s">
-        <v>675</v>
+        <v>672</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
@@ -26389,7 +26425,7 @@
         <v>374</v>
       </c>
       <c r="C258" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
@@ -26400,7 +26436,7 @@
         <v>375</v>
       </c>
       <c r="C259" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
@@ -26411,7 +26447,7 @@
         <v>376</v>
       </c>
       <c r="C260" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
@@ -26422,7 +26458,7 @@
         <v>377</v>
       </c>
       <c r="C261" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
@@ -26433,7 +26469,7 @@
         <v>412</v>
       </c>
       <c r="C262" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
@@ -26455,7 +26491,7 @@
         <v>382</v>
       </c>
       <c r="C264" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
@@ -26466,7 +26502,7 @@
         <v>383</v>
       </c>
       <c r="C265" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
@@ -26477,7 +26513,7 @@
         <v>384</v>
       </c>
       <c r="C266" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
@@ -26488,7 +26524,7 @@
         <v>385</v>
       </c>
       <c r="C267" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
@@ -26499,7 +26535,7 @@
         <v>413</v>
       </c>
       <c r="C268" t="s">
-        <v>682</v>
+        <v>679</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
@@ -26521,7 +26557,7 @@
         <v>81</v>
       </c>
       <c r="C270" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
@@ -26532,7 +26568,7 @@
         <v>82</v>
       </c>
       <c r="C271" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
@@ -26543,7 +26579,7 @@
         <v>83</v>
       </c>
       <c r="C272" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
@@ -26554,7 +26590,7 @@
         <v>84</v>
       </c>
       <c r="C273" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
@@ -26565,7 +26601,7 @@
         <v>85</v>
       </c>
       <c r="C274" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
@@ -26576,7 +26612,7 @@
         <v>86</v>
       </c>
       <c r="C275" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
@@ -26587,7 +26623,7 @@
         <v>87</v>
       </c>
       <c r="C276" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
@@ -26598,7 +26634,7 @@
         <v>88</v>
       </c>
       <c r="C277" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
@@ -26609,7 +26645,7 @@
         <v>89</v>
       </c>
       <c r="C278" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
@@ -26631,7 +26667,7 @@
         <v>212</v>
       </c>
       <c r="C280" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
@@ -26642,7 +26678,7 @@
         <v>233</v>
       </c>
       <c r="C281" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
@@ -26653,7 +26689,7 @@
         <v>239</v>
       </c>
       <c r="C282" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
@@ -26664,7 +26700,7 @@
         <v>266</v>
       </c>
       <c r="C283" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
@@ -26675,7 +26711,7 @@
         <v>309</v>
       </c>
       <c r="C284" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
@@ -26686,7 +26722,7 @@
         <v>311</v>
       </c>
       <c r="C285" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
@@ -26697,7 +26733,7 @@
         <v>312</v>
       </c>
       <c r="C286" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
@@ -26730,7 +26766,7 @@
         <v>77</v>
       </c>
       <c r="C289" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
@@ -26741,7 +26777,7 @@
         <v>78</v>
       </c>
       <c r="C290" t="s">
-        <v>683</v>
+        <v>680</v>
       </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
@@ -26763,7 +26799,7 @@
         <v>305</v>
       </c>
       <c r="C292" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="293" spans="1:5" x14ac:dyDescent="0.25">
@@ -26774,7 +26810,7 @@
         <v>306</v>
       </c>
       <c r="C293" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
     </row>
     <row r="294" spans="1:5" x14ac:dyDescent="0.25">
@@ -26785,7 +26821,7 @@
         <v>307</v>
       </c>
       <c r="C294" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="295" spans="1:5" x14ac:dyDescent="0.25">
@@ -26796,7 +26832,7 @@
         <v>308</v>
       </c>
       <c r="C295" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
     </row>
     <row r="296" spans="1:5" x14ac:dyDescent="0.25">
@@ -26821,7 +26857,7 @@
         <v>30</v>
       </c>
       <c r="E297" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="298" spans="1:5" x14ac:dyDescent="0.25">
@@ -26964,7 +27000,7 @@
         <v>67</v>
       </c>
       <c r="C310" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
@@ -26975,7 +27011,7 @@
         <v>68</v>
       </c>
       <c r="C311" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
@@ -26997,7 +27033,7 @@
         <v>211</v>
       </c>
       <c r="C313" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
@@ -27008,7 +27044,7 @@
         <v>290</v>
       </c>
       <c r="C314" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
@@ -27019,7 +27055,7 @@
         <v>291</v>
       </c>
       <c r="C315" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
@@ -27030,7 +27066,7 @@
         <v>292</v>
       </c>
       <c r="C316" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
@@ -27041,7 +27077,7 @@
         <v>409</v>
       </c>
       <c r="C317" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
@@ -27052,7 +27088,7 @@
         <v>410</v>
       </c>
       <c r="C318" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
@@ -27074,7 +27110,7 @@
         <v>232</v>
       </c>
       <c r="C320" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="321" spans="1:4" x14ac:dyDescent="0.25">
@@ -27085,7 +27121,7 @@
         <v>402</v>
       </c>
       <c r="C321" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="322" spans="1:4" x14ac:dyDescent="0.25">
@@ -27096,7 +27132,7 @@
         <v>403</v>
       </c>
       <c r="C322" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="323" spans="1:4" x14ac:dyDescent="0.25">
@@ -27107,7 +27143,7 @@
         <v>404</v>
       </c>
       <c r="C323" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="324" spans="1:4" x14ac:dyDescent="0.25">
@@ -27118,7 +27154,7 @@
         <v>405</v>
       </c>
       <c r="C324" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="325" spans="1:4" x14ac:dyDescent="0.25">
@@ -27129,7 +27165,7 @@
         <v>406</v>
       </c>
       <c r="C325" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="326" spans="1:4" x14ac:dyDescent="0.25">
@@ -27140,7 +27176,7 @@
         <v>407</v>
       </c>
       <c r="C326" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="327" spans="1:4" x14ac:dyDescent="0.25">
@@ -27151,7 +27187,7 @@
         <v>32</v>
       </c>
       <c r="C327" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="328" spans="1:4" x14ac:dyDescent="0.25">
@@ -27162,10 +27198,10 @@
         <v>33</v>
       </c>
       <c r="C328" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
       <c r="D328" t="s">
-        <v>743</v>
+        <v>740</v>
       </c>
     </row>
     <row r="329" spans="1:4" x14ac:dyDescent="0.25">
@@ -27176,7 +27212,7 @@
         <v>213</v>
       </c>
       <c r="C329" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="330" spans="1:4" x14ac:dyDescent="0.25">
@@ -27187,7 +27223,7 @@
         <v>267</v>
       </c>
       <c r="C330" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="331" spans="1:4" x14ac:dyDescent="0.25">
@@ -27209,7 +27245,7 @@
         <v>137</v>
       </c>
       <c r="C332" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="333" spans="1:4" x14ac:dyDescent="0.25">
@@ -27220,7 +27256,7 @@
         <v>145</v>
       </c>
       <c r="C333" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="334" spans="1:4" x14ac:dyDescent="0.25">
@@ -27253,7 +27289,7 @@
         <v>349</v>
       </c>
       <c r="C336" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="337" spans="1:4" x14ac:dyDescent="0.25">
@@ -27264,7 +27300,7 @@
         <v>350</v>
       </c>
       <c r="C337" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.25">
@@ -27275,7 +27311,7 @@
         <v>351</v>
       </c>
       <c r="C338" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="339" spans="1:4" x14ac:dyDescent="0.25">
@@ -27286,7 +27322,7 @@
         <v>352</v>
       </c>
       <c r="C339" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="340" spans="1:4" x14ac:dyDescent="0.25">
@@ -27297,7 +27333,7 @@
         <v>408</v>
       </c>
       <c r="C340" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.25">
@@ -27308,7 +27344,7 @@
         <v>417</v>
       </c>
       <c r="C341" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.25">
@@ -27319,7 +27355,7 @@
         <v>418</v>
       </c>
       <c r="C342" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.25">
@@ -27330,7 +27366,7 @@
         <v>419</v>
       </c>
       <c r="C343" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="344" spans="1:4" x14ac:dyDescent="0.25">
@@ -27341,7 +27377,7 @@
         <v>420</v>
       </c>
       <c r="C344" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="345" spans="1:4" x14ac:dyDescent="0.25">
@@ -27352,7 +27388,7 @@
         <v>421</v>
       </c>
       <c r="C345" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="346" spans="1:4" x14ac:dyDescent="0.25">
@@ -27385,7 +27421,7 @@
         <v>347</v>
       </c>
       <c r="C348" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.25">
@@ -27396,7 +27432,7 @@
         <v>348</v>
       </c>
       <c r="C349" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.25">
@@ -27407,7 +27443,7 @@
         <v>416</v>
       </c>
       <c r="C350" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="351" spans="1:4" x14ac:dyDescent="0.25">
@@ -27418,7 +27454,7 @@
         <v>203</v>
       </c>
       <c r="C351" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="352" spans="1:4" x14ac:dyDescent="0.25">
@@ -27429,10 +27465,10 @@
         <v>7</v>
       </c>
       <c r="C352" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D352" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
@@ -27443,10 +27479,10 @@
         <v>8</v>
       </c>
       <c r="C353" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D353" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.25">
@@ -27457,10 +27493,10 @@
         <v>9</v>
       </c>
       <c r="C354" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D354" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
@@ -27471,10 +27507,10 @@
         <v>10</v>
       </c>
       <c r="C355" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D355" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
@@ -27485,10 +27521,10 @@
         <v>11</v>
       </c>
       <c r="C356" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D356" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
@@ -27499,7 +27535,7 @@
         <v>73</v>
       </c>
       <c r="C357" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
@@ -27510,7 +27546,7 @@
         <v>140</v>
       </c>
       <c r="C358" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
@@ -27521,7 +27557,7 @@
         <v>141</v>
       </c>
       <c r="C359" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
@@ -27532,7 +27568,7 @@
         <v>142</v>
       </c>
       <c r="C360" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.25">
@@ -27543,7 +27579,7 @@
         <v>199</v>
       </c>
       <c r="C361" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.25">
@@ -27554,7 +27590,7 @@
         <v>205</v>
       </c>
       <c r="C362" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="363" spans="1:4" x14ac:dyDescent="0.25">
@@ -27565,7 +27601,7 @@
         <v>206</v>
       </c>
       <c r="C363" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="364" spans="1:4" x14ac:dyDescent="0.25">
@@ -27598,7 +27634,7 @@
         <v>94</v>
       </c>
       <c r="C366" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
     </row>
     <row r="367" spans="1:4" x14ac:dyDescent="0.25">
@@ -27609,7 +27645,7 @@
         <v>95</v>
       </c>
       <c r="C367" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
@@ -27620,7 +27656,7 @@
         <v>96</v>
       </c>
       <c r="C368" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
@@ -27631,7 +27667,7 @@
         <v>97</v>
       </c>
       <c r="C369" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
@@ -27642,7 +27678,7 @@
         <v>98</v>
       </c>
       <c r="C370" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
@@ -27664,7 +27700,7 @@
         <v>314</v>
       </c>
       <c r="C372" t="s">
-        <v>647</v>
+        <v>644</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
@@ -27686,7 +27722,7 @@
         <v>63</v>
       </c>
       <c r="C374" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
@@ -27697,7 +27733,7 @@
         <v>64</v>
       </c>
       <c r="C375" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
@@ -27719,7 +27755,7 @@
         <v>281</v>
       </c>
       <c r="C377" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
@@ -27730,7 +27766,7 @@
         <v>282</v>
       </c>
       <c r="C378" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
@@ -27741,7 +27777,7 @@
         <v>283</v>
       </c>
       <c r="C379" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
@@ -27752,7 +27788,7 @@
         <v>284</v>
       </c>
       <c r="C380" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
@@ -27763,7 +27799,7 @@
         <v>285</v>
       </c>
       <c r="C381" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
@@ -27774,7 +27810,7 @@
         <v>286</v>
       </c>
       <c r="C382" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
@@ -27785,7 +27821,7 @@
         <v>441</v>
       </c>
       <c r="C383" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
@@ -27796,7 +27832,7 @@
         <v>184</v>
       </c>
       <c r="C384" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
@@ -27807,7 +27843,7 @@
         <v>185</v>
       </c>
       <c r="C385" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
@@ -27818,7 +27854,7 @@
         <v>186</v>
       </c>
       <c r="C386" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
@@ -27829,7 +27865,7 @@
         <v>187</v>
       </c>
       <c r="C387" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
@@ -27840,7 +27876,7 @@
         <v>188</v>
       </c>
       <c r="C388" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
@@ -27895,7 +27931,7 @@
         <v>227</v>
       </c>
       <c r="C393" t="s">
-        <v>768</v>
+        <v>765</v>
       </c>
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
@@ -27906,7 +27942,7 @@
         <v>228</v>
       </c>
       <c r="C394" t="s">
-        <v>769</v>
+        <v>766</v>
       </c>
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
@@ -27917,7 +27953,7 @@
         <v>229</v>
       </c>
       <c r="C395" t="s">
-        <v>770</v>
+        <v>767</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
@@ -27928,7 +27964,7 @@
         <v>230</v>
       </c>
       <c r="C396" t="s">
-        <v>771</v>
+        <v>768</v>
       </c>
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
@@ -27939,7 +27975,7 @@
         <v>249</v>
       </c>
       <c r="C397" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
@@ -27950,7 +27986,7 @@
         <v>242</v>
       </c>
       <c r="C398" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
@@ -27961,7 +27997,7 @@
         <v>274</v>
       </c>
       <c r="C399" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
@@ -28200,7 +28236,7 @@
         <v>13</v>
       </c>
       <c r="C424" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
@@ -28211,7 +28247,7 @@
         <v>14</v>
       </c>
       <c r="C425" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
@@ -28222,7 +28258,7 @@
         <v>15</v>
       </c>
       <c r="C426" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
@@ -28233,7 +28269,7 @@
         <v>16</v>
       </c>
       <c r="C427" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
@@ -28254,7 +28290,7 @@
         <v>442</v>
       </c>
       <c r="C430" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
@@ -28265,7 +28301,7 @@
         <v>443</v>
       </c>
       <c r="C431" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
@@ -28276,7 +28312,7 @@
         <v>444</v>
       </c>
       <c r="C432" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
@@ -28287,7 +28323,7 @@
         <v>143</v>
       </c>
       <c r="C433" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
@@ -28331,7 +28367,7 @@
         <v>353</v>
       </c>
       <c r="C437" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
@@ -28342,7 +28378,7 @@
         <v>75</v>
       </c>
       <c r="C438" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
   </sheetData>
@@ -28392,7 +28428,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B3">
         <v>5235</v>
@@ -28412,13 +28448,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B4">
         <v>3621</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="D4">
         <v>1230</v>
@@ -28432,7 +28468,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B5">
         <v>3412</v>
@@ -28447,7 +28483,7 @@
         <v>1977</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
     </row>
   </sheetData>
@@ -28461,7 +28497,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Room 51 Objects Room 52 Objects
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="5"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1375" uniqueCount="821">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1376" uniqueCount="822">
   <si>
     <t>Purpose</t>
   </si>
@@ -2501,6 +2501,9 @@
   </si>
   <si>
     <t>Cassette Recorder</t>
+  </si>
+  <si>
+    <t>1 = Kids Hands</t>
   </si>
 </sst>
 </file>
@@ -2832,7 +2835,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3288,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4050,8 +4053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="D126" sqref="D126"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22272,8 +22275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22408,6 +22411,9 @@
       <c r="C7" t="s">
         <v>593</v>
       </c>
+      <c r="E7" t="s">
+        <v>821</v>
+      </c>
       <c r="F7" t="s">
         <v>594</v>
       </c>
@@ -23649,7 +23655,7 @@
   <dimension ref="A1:B33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23933,8 +23939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A177" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView topLeftCell="A319" workbookViewId="0">
+      <selection activeCell="C334" sqref="C334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Room 27 Objects Room 28 Objects
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="5"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -3312,8 +3312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,8 +4074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22294,10 +22294,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I109"/>
+  <dimension ref="A1:I110"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22551,44 +22551,35 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
-        <v>246</v>
-      </c>
-      <c r="E15" t="s">
-        <v>230</v>
-      </c>
-      <c r="F15" t="s">
-        <v>634</v>
-      </c>
-      <c r="G15" t="s">
-        <v>241</v>
-      </c>
-      <c r="H15" t="s">
-        <v>434</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>811</v>
+        <v>246</v>
       </c>
       <c r="E16" t="s">
-        <v>262</v>
+        <v>230</v>
       </c>
       <c r="F16" t="s">
-        <v>244</v>
+        <v>634</v>
+      </c>
+      <c r="G16" t="s">
+        <v>241</v>
+      </c>
+      <c r="H16" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>811</v>
       </c>
       <c r="E17" t="s">
         <v>262</v>
@@ -22599,355 +22590,355 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>718</v>
+        <v>15</v>
       </c>
       <c r="E18" t="s">
-        <v>719</v>
+        <v>262</v>
       </c>
       <c r="F18" t="s">
-        <v>720</v>
-      </c>
-      <c r="G18" t="s">
-        <v>721</v>
-      </c>
-      <c r="H18" t="s">
-        <v>722</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>599</v>
+        <v>718</v>
       </c>
       <c r="E19" t="s">
-        <v>218</v>
+        <v>719</v>
       </c>
       <c r="F19" t="s">
-        <v>600</v>
+        <v>720</v>
       </c>
       <c r="G19" t="s">
-        <v>601</v>
+        <v>721</v>
+      </c>
+      <c r="H19" t="s">
+        <v>722</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>164</v>
+        <v>599</v>
+      </c>
+      <c r="E20" t="s">
+        <v>218</v>
+      </c>
+      <c r="F20" t="s">
+        <v>600</v>
+      </c>
+      <c r="G20" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
-        <v>267</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" t="s">
-        <v>153</v>
+        <v>270</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>546</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>120</v>
-      </c>
-      <c r="D37" t="s">
-        <v>614</v>
-      </c>
-      <c r="E37" t="s">
-        <v>121</v>
-      </c>
-      <c r="F37" t="s">
-        <v>124</v>
-      </c>
-      <c r="G37" t="s">
-        <v>123</v>
-      </c>
-      <c r="H37" t="s">
-        <v>122</v>
+        <v>546</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>54</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>82</v>
+        <v>614</v>
+      </c>
+      <c r="E38" t="s">
+        <v>121</v>
+      </c>
+      <c r="F38" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>704</v>
-      </c>
-      <c r="E39" t="s">
-        <v>218</v>
-      </c>
-      <c r="F39" t="s">
-        <v>219</v>
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="E40" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="F40" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>174</v>
+        <v>710</v>
       </c>
       <c r="E41" t="s">
-        <v>175</v>
+        <v>296</v>
       </c>
       <c r="F41" t="s">
-        <v>176</v>
-      </c>
-      <c r="G41" t="s">
-        <v>177</v>
-      </c>
-      <c r="H41" t="s">
-        <v>178</v>
-      </c>
-      <c r="I41" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
+        <v>174</v>
+      </c>
+      <c r="E42" t="s">
+        <v>175</v>
+      </c>
+      <c r="F42" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" t="s">
+        <v>177</v>
+      </c>
+      <c r="H42" t="s">
+        <v>178</v>
+      </c>
+      <c r="I42" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
+        <v>60</v>
+      </c>
+      <c r="C45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46">
         <v>61</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>62</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="1"/>
-      <c r="E46" t="s">
+      <c r="D47" s="1"/>
+      <c r="E47" t="s">
         <v>59</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="G47" s="2" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>63</v>
-      </c>
-      <c r="C47" t="s">
-        <v>766</v>
-      </c>
-      <c r="E47" t="s">
-        <v>230</v>
-      </c>
-      <c r="F47" t="s">
-        <v>248</v>
-      </c>
-      <c r="G47" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E48" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="F48" t="s">
-        <v>219</v>
+        <v>248</v>
+      </c>
+      <c r="G48" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="E49" t="s">
         <v>218</v>
@@ -22958,69 +22949,69 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>205</v>
+        <v>765</v>
       </c>
       <c r="E50" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="F50" t="s">
-        <v>404</v>
-      </c>
-      <c r="G50" t="s">
-        <v>231</v>
-      </c>
-      <c r="H50" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>551</v>
+        <v>205</v>
+      </c>
+      <c r="E51" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" t="s">
+        <v>404</v>
+      </c>
+      <c r="G51" t="s">
+        <v>231</v>
+      </c>
+      <c r="H51" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>68</v>
-      </c>
-      <c r="B52" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>25</v>
-      </c>
-      <c r="D52" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" t="s">
-        <v>218</v>
-      </c>
-      <c r="F52" t="s">
-        <v>27</v>
+        <v>551</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>742</v>
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
       </c>
       <c r="E53" t="s">
-        <v>743</v>
+        <v>218</v>
+      </c>
+      <c r="F53" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
         <v>7</v>
@@ -23029,276 +23020,276 @@
         <v>742</v>
       </c>
       <c r="E54" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>746</v>
+        <v>742</v>
+      </c>
+      <c r="E55" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>64</v>
-      </c>
-      <c r="E57" t="s">
-        <v>65</v>
-      </c>
-      <c r="F57" t="s">
-        <v>257</v>
-      </c>
-      <c r="G57" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B58" t="s">
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>717</v>
+        <v>64</v>
       </c>
       <c r="E58" t="s">
-        <v>219</v>
+        <v>65</v>
+      </c>
+      <c r="F58" t="s">
+        <v>257</v>
+      </c>
+      <c r="G58" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>460</v>
+        <v>717</v>
       </c>
       <c r="E59" t="s">
-        <v>280</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>209</v>
+        <v>460</v>
       </c>
       <c r="E60" t="s">
-        <v>206</v>
-      </c>
-      <c r="F60" t="s">
-        <v>725</v>
-      </c>
-      <c r="G60" t="s">
-        <v>207</v>
-      </c>
-      <c r="H60" t="s">
-        <v>284</v>
-      </c>
-      <c r="I60" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
-        <v>726</v>
+        <v>209</v>
       </c>
       <c r="E61" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F61" t="s">
-        <v>212</v>
+        <v>725</v>
+      </c>
+      <c r="G61" t="s">
+        <v>207</v>
+      </c>
+      <c r="H61" t="s">
+        <v>284</v>
+      </c>
+      <c r="I61" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
+        <v>78</v>
+      </c>
+      <c r="C62" t="s">
+        <v>726</v>
+      </c>
+      <c r="E62" t="s">
+        <v>211</v>
+      </c>
+      <c r="F62" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63">
         <v>79</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>330</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E63" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63">
+    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>80</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>332</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>218</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F64" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>81</v>
-      </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64" t="s">
-        <v>57</v>
-      </c>
-      <c r="E64" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>550</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>287</v>
-      </c>
-      <c r="F65" t="s">
-        <v>285</v>
-      </c>
-      <c r="G65" t="s">
-        <v>286</v>
-      </c>
-      <c r="H65" t="s">
-        <v>571</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>552</v>
+        <v>550</v>
+      </c>
+      <c r="E66" t="s">
+        <v>287</v>
+      </c>
+      <c r="F66" t="s">
+        <v>285</v>
+      </c>
+      <c r="G66" t="s">
+        <v>286</v>
+      </c>
+      <c r="H66" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>391</v>
-      </c>
-      <c r="E67" t="s">
-        <v>218</v>
-      </c>
-      <c r="F67" t="s">
-        <v>392</v>
+        <v>552</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>769</v>
+        <v>391</v>
       </c>
       <c r="E68" t="s">
         <v>218</v>
       </c>
       <c r="F68" t="s">
-        <v>219</v>
+        <v>392</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>818</v>
+        <v>769</v>
+      </c>
+      <c r="E69" t="s">
+        <v>218</v>
+      </c>
+      <c r="F69" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C70" t="s">
-        <v>753</v>
+        <v>818</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C71" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>90</v>
-      </c>
-      <c r="D72" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>90</v>
       </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73" t="s">
-        <v>102</v>
+      <c r="D73" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>91</v>
-      </c>
-      <c r="D74" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>91</v>
       </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
-        <v>101</v>
-      </c>
       <c r="D75" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D76" t="s">
         <v>88</v>
@@ -23306,72 +23297,72 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="B77" t="s">
+        <v>7</v>
+      </c>
+      <c r="C77" t="s">
+        <v>103</v>
+      </c>
+      <c r="D77" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>96</v>
-      </c>
-      <c r="C78" t="s">
-        <v>217</v>
-      </c>
-      <c r="E78" t="s">
-        <v>218</v>
-      </c>
-      <c r="F78" t="s">
-        <v>219</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" t="s">
-        <v>105</v>
+        <v>217</v>
+      </c>
+      <c r="E79" t="s">
+        <v>218</v>
+      </c>
+      <c r="F79" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C82" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>101</v>
-      </c>
-      <c r="C83" t="s">
-        <v>776</v>
-      </c>
-      <c r="E83" t="s">
-        <v>218</v>
-      </c>
-      <c r="F83" t="s">
-        <v>219</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" t="s">
-        <v>745</v>
+        <v>776</v>
       </c>
       <c r="E84" t="s">
         <v>218</v>
@@ -23382,170 +23373,170 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C85" t="s">
-        <v>709</v>
-      </c>
-      <c r="D85" t="s">
-        <v>74</v>
+        <v>745</v>
       </c>
       <c r="E85" t="s">
-        <v>75</v>
+        <v>218</v>
       </c>
       <c r="F85" t="s">
-        <v>706</v>
-      </c>
-      <c r="G85" t="s">
-        <v>705</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>755</v>
+        <v>709</v>
+      </c>
+      <c r="D86" t="s">
+        <v>74</v>
       </c>
       <c r="E86" t="s">
-        <v>218</v>
+        <v>75</v>
       </c>
       <c r="F86" t="s">
-        <v>219</v>
+        <v>706</v>
+      </c>
+      <c r="G86" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>105</v>
-      </c>
-      <c r="B87" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C87" t="s">
-        <v>128</v>
+        <v>755</v>
+      </c>
+      <c r="E87" t="s">
+        <v>218</v>
+      </c>
+      <c r="F87" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>714</v>
-      </c>
-      <c r="E88" t="s">
-        <v>715</v>
-      </c>
-      <c r="F88" t="s">
-        <v>127</v>
-      </c>
-      <c r="G88" t="s">
-        <v>716</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B89" t="s">
+        <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>762</v>
+        <v>714</v>
+      </c>
+      <c r="E89" t="s">
+        <v>715</v>
+      </c>
+      <c r="F89" t="s">
+        <v>127</v>
+      </c>
+      <c r="G89" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>309</v>
-      </c>
-      <c r="E90" t="s">
-        <v>305</v>
-      </c>
-      <c r="F90" t="s">
-        <v>306</v>
-      </c>
-      <c r="G90" t="s">
-        <v>307</v>
-      </c>
-      <c r="H90" t="s">
-        <v>308</v>
+        <v>762</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C91" t="s">
+        <v>309</v>
+      </c>
+      <c r="E91" t="s">
+        <v>305</v>
+      </c>
+      <c r="F91" t="s">
+        <v>306</v>
+      </c>
+      <c r="G91" t="s">
+        <v>307</v>
+      </c>
+      <c r="H91" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>110</v>
-      </c>
-      <c r="C92" t="s">
-        <v>485</v>
-      </c>
-      <c r="E92" t="s">
-        <v>218</v>
-      </c>
-      <c r="F92" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
+        <v>485</v>
+      </c>
+      <c r="E93" t="s">
+        <v>218</v>
+      </c>
+      <c r="F93" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>116</v>
-      </c>
-      <c r="C96" t="s">
-        <v>828</v>
-      </c>
-      <c r="E96" t="s">
-        <v>218</v>
-      </c>
-      <c r="F96" t="s">
-        <v>219</v>
+        <v>114</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="C97" t="s">
+        <v>828</v>
+      </c>
+      <c r="E97" t="s">
+        <v>218</v>
+      </c>
+      <c r="F97" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>118</v>
-      </c>
-      <c r="C98" t="s">
-        <v>778</v>
-      </c>
-      <c r="E98" t="s">
-        <v>262</v>
-      </c>
-      <c r="F98" t="s">
-        <v>244</v>
+        <v>117</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C99" t="s">
-        <v>817</v>
+        <v>778</v>
       </c>
       <c r="E99" t="s">
         <v>262</v>
@@ -23556,10 +23547,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C100" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="E100" t="s">
         <v>262</v>
@@ -23570,109 +23561,123 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>122</v>
-      </c>
-      <c r="B101" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C101" t="s">
-        <v>73</v>
-      </c>
-      <c r="D101" t="s">
-        <v>71</v>
+        <v>816</v>
       </c>
       <c r="E101" t="s">
-        <v>69</v>
+        <v>262</v>
       </c>
       <c r="F101" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B102" t="s">
+        <v>6</v>
+      </c>
+      <c r="C102" t="s">
+        <v>73</v>
+      </c>
+      <c r="D102" t="s">
+        <v>71</v>
+      </c>
+      <c r="E102" t="s">
+        <v>69</v>
+      </c>
+      <c r="F102" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>126</v>
       </c>
-      <c r="C103" t="s">
-        <v>598</v>
-      </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>127</v>
-      </c>
-      <c r="B104" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C104" t="s">
-        <v>20</v>
-      </c>
-      <c r="D104" t="s">
-        <v>22</v>
-      </c>
-      <c r="E104" t="s">
-        <v>21</v>
-      </c>
-      <c r="F104" t="s">
-        <v>26</v>
+        <v>598</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B105" t="s">
+        <v>7</v>
       </c>
       <c r="C105" t="s">
-        <v>808</v>
+        <v>20</v>
+      </c>
+      <c r="D105" t="s">
+        <v>22</v>
       </c>
       <c r="E105" t="s">
-        <v>218</v>
+        <v>21</v>
       </c>
       <c r="F105" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C106" t="s">
-        <v>754</v>
+        <v>808</v>
+      </c>
+      <c r="E106" t="s">
+        <v>218</v>
+      </c>
+      <c r="F106" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C107" t="s">
-        <v>756</v>
-      </c>
-      <c r="E107" t="s">
-        <v>218</v>
-      </c>
-      <c r="F107" t="s">
-        <v>219</v>
+        <v>754</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C108" t="s">
-        <v>592</v>
+        <v>756</v>
       </c>
       <c r="E108" t="s">
+        <v>218</v>
+      </c>
+      <c r="F108" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
+        <v>136</v>
+      </c>
+      <c r="C109" t="s">
+        <v>592</v>
+      </c>
+      <c r="E109" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110">
         <v>137</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C110" t="s">
         <v>562</v>
       </c>
     </row>
@@ -23998,8 +24003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A202" workbookViewId="0">
-      <selection activeCell="C224" sqref="C224"/>
+    <sheetView topLeftCell="A324" workbookViewId="0">
+      <selection activeCell="C329" sqref="C329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29101,7 +29106,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Room 29 - 42 Objects
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1387" uniqueCount="829">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="832">
   <si>
     <t>Purpose</t>
   </si>
@@ -2525,6 +2525,15 @@
   </si>
   <si>
     <t>Ednas Phone Number exposed</t>
+  </si>
+  <si>
+    <t>Telescope: Dimes Available</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -2856,7 +2865,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3312,8 +3321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4074,8 +4083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22294,10 +22303,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I110"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22553,6 +22562,9 @@
       <c r="A15">
         <v>26</v>
       </c>
+      <c r="C15" t="s">
+        <v>829</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -23509,48 +23521,39 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>116</v>
-      </c>
-      <c r="C97" t="s">
-        <v>828</v>
-      </c>
-      <c r="E97" t="s">
-        <v>218</v>
-      </c>
-      <c r="F97" t="s">
-        <v>219</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="C98" t="s">
+        <v>828</v>
+      </c>
+      <c r="E98" t="s">
+        <v>218</v>
+      </c>
+      <c r="F98" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>118</v>
-      </c>
-      <c r="C99" t="s">
-        <v>778</v>
-      </c>
-      <c r="E99" t="s">
-        <v>262</v>
-      </c>
-      <c r="F99" t="s">
-        <v>244</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C100" t="s">
-        <v>817</v>
+        <v>778</v>
       </c>
       <c r="E100" t="s">
         <v>262</v>
@@ -23561,10 +23564,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C101" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="E101" t="s">
         <v>262</v>
@@ -23575,109 +23578,123 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>122</v>
-      </c>
-      <c r="B102" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C102" t="s">
-        <v>73</v>
-      </c>
-      <c r="D102" t="s">
-        <v>71</v>
+        <v>816</v>
       </c>
       <c r="E102" t="s">
-        <v>69</v>
+        <v>262</v>
       </c>
       <c r="F102" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
+      </c>
+      <c r="C103" t="s">
+        <v>73</v>
+      </c>
+      <c r="D103" t="s">
+        <v>71</v>
+      </c>
+      <c r="E103" t="s">
+        <v>69</v>
+      </c>
+      <c r="F103" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>126</v>
       </c>
-      <c r="C104" t="s">
-        <v>598</v>
-      </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>127</v>
-      </c>
-      <c r="B105" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C105" t="s">
-        <v>20</v>
-      </c>
-      <c r="D105" t="s">
-        <v>22</v>
-      </c>
-      <c r="E105" t="s">
-        <v>21</v>
-      </c>
-      <c r="F105" t="s">
-        <v>26</v>
+        <v>598</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>808</v>
+        <v>20</v>
+      </c>
+      <c r="D106" t="s">
+        <v>22</v>
       </c>
       <c r="E106" t="s">
-        <v>218</v>
+        <v>21</v>
       </c>
       <c r="F106" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C107" t="s">
-        <v>754</v>
+        <v>808</v>
+      </c>
+      <c r="E107" t="s">
+        <v>218</v>
+      </c>
+      <c r="F107" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C108" t="s">
-        <v>756</v>
-      </c>
-      <c r="E108" t="s">
-        <v>218</v>
-      </c>
-      <c r="F108" t="s">
-        <v>219</v>
+        <v>754</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C109" t="s">
-        <v>592</v>
+        <v>756</v>
       </c>
       <c r="E109" t="s">
+        <v>218</v>
+      </c>
+      <c r="F109" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
+        <v>136</v>
+      </c>
+      <c r="C110" t="s">
+        <v>592</v>
+      </c>
+      <c r="E110" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111">
         <v>137</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>562</v>
       </c>
     </row>
@@ -23694,8 +23711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24003,8 +24020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A324" workbookViewId="0">
-      <selection activeCell="C329" sqref="C329"/>
+    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
+      <selection activeCell="D401" sqref="D401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28577,6 +28594,9 @@
       <c r="B402">
         <v>287</v>
       </c>
+      <c r="C402" t="s">
+        <v>831</v>
+      </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A403">
@@ -28585,6 +28605,9 @@
       <c r="B403">
         <v>288</v>
       </c>
+      <c r="C403">
+        <v>0</v>
+      </c>
     </row>
     <row r="404" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A404">
@@ -28593,6 +28616,9 @@
       <c r="B404">
         <v>289</v>
       </c>
+      <c r="C404" t="s">
+        <v>830</v>
+      </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A405">
@@ -28601,6 +28627,9 @@
       <c r="B405">
         <v>422</v>
       </c>
+      <c r="C405">
+        <v>1</v>
+      </c>
     </row>
     <row r="406" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A406">
@@ -28609,6 +28638,9 @@
       <c r="B406">
         <v>423</v>
       </c>
+      <c r="C406">
+        <v>3</v>
+      </c>
     </row>
     <row r="407" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A407">
@@ -28617,6 +28649,9 @@
       <c r="B407">
         <v>424</v>
       </c>
+      <c r="C407">
+        <v>4</v>
+      </c>
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A408">
@@ -28625,6 +28660,9 @@
       <c r="B408">
         <v>425</v>
       </c>
+      <c r="C408">
+        <v>5</v>
+      </c>
     </row>
     <row r="409" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A409">
@@ -28633,6 +28671,9 @@
       <c r="B409">
         <v>426</v>
       </c>
+      <c r="C409">
+        <v>6</v>
+      </c>
     </row>
     <row r="410" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A410">
@@ -28652,6 +28693,9 @@
       <c r="B411">
         <v>428</v>
       </c>
+      <c r="C411">
+        <v>7</v>
+      </c>
     </row>
     <row r="412" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A412">
@@ -28660,6 +28704,9 @@
       <c r="B412">
         <v>429</v>
       </c>
+      <c r="C412">
+        <v>8</v>
+      </c>
     </row>
     <row r="413" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A413">
@@ -28667,6 +28714,9 @@
       </c>
       <c r="B413">
         <v>430</v>
+      </c>
+      <c r="C413">
+        <v>9</v>
       </c>
     </row>
     <row r="414" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Room 43 - 52 Objects
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="5"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="832">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="836">
   <si>
     <t>Purpose</t>
   </si>
@@ -2329,9 +2329,6 @@
     <t>Give Script: Object-ID</t>
   </si>
   <si>
-    <t>Cutscene: 3 Guys Who Pub Anything: Receive Mail Trigger+D32</t>
-  </si>
-  <si>
     <t>Envelope Stamped</t>
   </si>
   <si>
@@ -2534,6 +2531,21 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>10 = *</t>
+  </si>
+  <si>
+    <t>0 = 0</t>
+  </si>
+  <si>
+    <t>11 = #</t>
+  </si>
+  <si>
+    <t>08 = in mailbox</t>
+  </si>
+  <si>
+    <t>Cutscene: 3 Guys Who Pub Anything: Receive Mail Trigger</t>
   </si>
 </sst>
 </file>
@@ -3134,15 +3146,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>783</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B2" s="3">
         <v>4</v>
@@ -3150,7 +3162,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -3158,7 +3170,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B4" s="3">
         <v>6</v>
@@ -3166,7 +3178,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B5" s="3">
         <v>7</v>
@@ -3177,15 +3189,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3201,7 +3213,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="B11" s="3">
         <v>2</v>
@@ -3209,7 +3221,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B12" s="3">
         <v>3</v>
@@ -3217,7 +3229,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
@@ -3225,7 +3237,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -3233,7 +3245,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B15" s="3">
         <v>6</v>
@@ -3241,7 +3253,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="B16" s="3">
         <v>7</v>
@@ -3249,7 +3261,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="B17" s="3">
         <v>8</v>
@@ -3257,7 +3269,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="B18" s="3">
         <v>9</v>
@@ -3265,50 +3277,50 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
   </sheetData>
@@ -3321,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4083,8 +4095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4180,7 +4192,7 @@
         <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4191,7 +4203,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4735,7 +4747,7 @@
         <v>18</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" s="2"/>
@@ -21625,7 +21637,7 @@
         <v>18</v>
       </c>
       <c r="D101" t="s">
-        <v>763</v>
+        <v>835</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -21995,7 +22007,7 @@
         <v>18</v>
       </c>
       <c r="D133" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
@@ -22303,10 +22315,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22442,7 +22454,7 @@
         <v>593</v>
       </c>
       <c r="E7" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F7" t="s">
         <v>594</v>
@@ -22563,7 +22575,7 @@
         <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -22591,7 +22603,7 @@
         <v>28</v>
       </c>
       <c r="C17" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E17" t="s">
         <v>262</v>
@@ -22789,182 +22801,185 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C38" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
       <c r="D38" t="s">
-        <v>614</v>
+        <v>831</v>
       </c>
       <c r="E38" t="s">
-        <v>121</v>
+        <v>832</v>
       </c>
       <c r="F38" t="s">
-        <v>124</v>
-      </c>
-      <c r="G38" t="s">
-        <v>123</v>
-      </c>
-      <c r="H38" t="s">
-        <v>122</v>
+        <v>833</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>120</v>
       </c>
       <c r="D39" t="s">
-        <v>82</v>
+        <v>614</v>
+      </c>
+      <c r="E39" t="s">
+        <v>121</v>
+      </c>
+      <c r="F39" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" t="s">
+        <v>123</v>
+      </c>
+      <c r="H39" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>704</v>
-      </c>
-      <c r="E40" t="s">
-        <v>218</v>
-      </c>
-      <c r="F40" t="s">
-        <v>219</v>
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>710</v>
+        <v>704</v>
       </c>
       <c r="E41" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
       <c r="F41" t="s">
-        <v>297</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>174</v>
+        <v>710</v>
       </c>
       <c r="E42" t="s">
-        <v>175</v>
+        <v>296</v>
       </c>
       <c r="F42" t="s">
-        <v>176</v>
-      </c>
-      <c r="G42" t="s">
-        <v>177</v>
-      </c>
-      <c r="H42" t="s">
-        <v>178</v>
-      </c>
-      <c r="I42" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>160</v>
+        <v>174</v>
+      </c>
+      <c r="E43" t="s">
+        <v>175</v>
+      </c>
+      <c r="F43" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" t="s">
+        <v>177</v>
+      </c>
+      <c r="H43" t="s">
+        <v>178</v>
+      </c>
+      <c r="I43" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>61</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>62</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>247</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>63</v>
-      </c>
-      <c r="C48" t="s">
-        <v>766</v>
-      </c>
-      <c r="E48" t="s">
-        <v>230</v>
-      </c>
-      <c r="F48" t="s">
-        <v>248</v>
-      </c>
-      <c r="G48" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="E49" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="F49" t="s">
-        <v>219</v>
+        <v>248</v>
+      </c>
+      <c r="G49" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="E50" t="s">
         <v>218</v>
@@ -22975,69 +22990,69 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>205</v>
+        <v>764</v>
       </c>
       <c r="E51" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="F51" t="s">
-        <v>404</v>
-      </c>
-      <c r="G51" t="s">
-        <v>231</v>
-      </c>
-      <c r="H51" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>551</v>
+        <v>205</v>
+      </c>
+      <c r="E52" t="s">
+        <v>230</v>
+      </c>
+      <c r="F52" t="s">
+        <v>404</v>
+      </c>
+      <c r="G52" t="s">
+        <v>231</v>
+      </c>
+      <c r="H52" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>68</v>
-      </c>
-      <c r="B53" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" t="s">
-        <v>218</v>
-      </c>
-      <c r="F53" t="s">
-        <v>27</v>
+        <v>551</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>742</v>
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>743</v>
+        <v>218</v>
+      </c>
+      <c r="F54" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -23046,276 +23061,276 @@
         <v>742</v>
       </c>
       <c r="E55" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>746</v>
+        <v>742</v>
+      </c>
+      <c r="E56" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
-      </c>
-      <c r="E58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F58" t="s">
-        <v>257</v>
-      </c>
-      <c r="G58" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>717</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>219</v>
+        <v>65</v>
+      </c>
+      <c r="F59" t="s">
+        <v>257</v>
+      </c>
+      <c r="G59" t="s">
+        <v>752</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>460</v>
+        <v>717</v>
       </c>
       <c r="E60" t="s">
-        <v>280</v>
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>209</v>
+        <v>460</v>
       </c>
       <c r="E61" t="s">
-        <v>206</v>
-      </c>
-      <c r="F61" t="s">
-        <v>725</v>
-      </c>
-      <c r="G61" t="s">
-        <v>207</v>
-      </c>
-      <c r="H61" t="s">
-        <v>284</v>
-      </c>
-      <c r="I61" t="s">
-        <v>208</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>726</v>
+        <v>209</v>
       </c>
       <c r="E62" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="F62" t="s">
-        <v>212</v>
+        <v>725</v>
+      </c>
+      <c r="G62" t="s">
+        <v>207</v>
+      </c>
+      <c r="H62" t="s">
+        <v>284</v>
+      </c>
+      <c r="I62" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>78</v>
+      </c>
+      <c r="C63" t="s">
+        <v>726</v>
+      </c>
+      <c r="E63" t="s">
+        <v>211</v>
+      </c>
+      <c r="F63" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>79</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>330</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>80</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>332</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>218</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>219</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>81</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>550</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>287</v>
-      </c>
-      <c r="F66" t="s">
-        <v>285</v>
-      </c>
-      <c r="G66" t="s">
-        <v>286</v>
-      </c>
-      <c r="H66" t="s">
-        <v>571</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>552</v>
+        <v>550</v>
+      </c>
+      <c r="E67" t="s">
+        <v>287</v>
+      </c>
+      <c r="F67" t="s">
+        <v>285</v>
+      </c>
+      <c r="G67" t="s">
+        <v>286</v>
+      </c>
+      <c r="H67" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
-        <v>391</v>
-      </c>
-      <c r="E68" t="s">
-        <v>218</v>
-      </c>
-      <c r="F68" t="s">
-        <v>392</v>
+        <v>552</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>769</v>
+        <v>391</v>
       </c>
       <c r="E69" t="s">
         <v>218</v>
       </c>
       <c r="F69" t="s">
-        <v>219</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>818</v>
+        <v>768</v>
+      </c>
+      <c r="E70" t="s">
+        <v>218</v>
+      </c>
+      <c r="F70" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>753</v>
+        <v>817</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>89</v>
+        <v>87</v>
+      </c>
+      <c r="C72" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>90</v>
-      </c>
-      <c r="D73" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90</v>
       </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>102</v>
+      <c r="D74" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>91</v>
-      </c>
-      <c r="D75" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>91</v>
       </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>101</v>
-      </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D77" t="s">
         <v>88</v>
@@ -23323,72 +23338,72 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>96</v>
-      </c>
-      <c r="C79" t="s">
-        <v>217</v>
-      </c>
-      <c r="E79" t="s">
-        <v>218</v>
-      </c>
-      <c r="F79" t="s">
-        <v>219</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>217</v>
+      </c>
+      <c r="E80" t="s">
+        <v>218</v>
+      </c>
+      <c r="F80" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>101</v>
-      </c>
-      <c r="C84" t="s">
-        <v>776</v>
-      </c>
-      <c r="E84" t="s">
-        <v>218</v>
-      </c>
-      <c r="F84" t="s">
-        <v>219</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>745</v>
+        <v>775</v>
       </c>
       <c r="E85" t="s">
         <v>218</v>
@@ -23399,175 +23414,175 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
-        <v>709</v>
-      </c>
-      <c r="D86" t="s">
-        <v>74</v>
+        <v>745</v>
       </c>
       <c r="E86" t="s">
-        <v>75</v>
+        <v>218</v>
       </c>
       <c r="F86" t="s">
-        <v>706</v>
-      </c>
-      <c r="G86" t="s">
-        <v>705</v>
+        <v>219</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>755</v>
+        <v>709</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
       </c>
       <c r="E87" t="s">
-        <v>218</v>
+        <v>75</v>
       </c>
       <c r="F87" t="s">
-        <v>219</v>
+        <v>706</v>
+      </c>
+      <c r="G87" t="s">
+        <v>705</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>105</v>
-      </c>
-      <c r="B88" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>755</v>
+      </c>
+      <c r="E88" t="s">
+        <v>218</v>
+      </c>
+      <c r="F88" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>714</v>
-      </c>
-      <c r="E89" t="s">
-        <v>715</v>
-      </c>
-      <c r="F89" t="s">
-        <v>127</v>
-      </c>
-      <c r="G89" t="s">
-        <v>716</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>762</v>
+        <v>714</v>
+      </c>
+      <c r="E90" t="s">
+        <v>715</v>
+      </c>
+      <c r="F90" t="s">
+        <v>127</v>
+      </c>
+      <c r="G90" t="s">
+        <v>716</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91" t="s">
-        <v>309</v>
-      </c>
-      <c r="E91" t="s">
-        <v>305</v>
-      </c>
-      <c r="F91" t="s">
-        <v>306</v>
-      </c>
-      <c r="G91" t="s">
-        <v>307</v>
-      </c>
-      <c r="H91" t="s">
-        <v>308</v>
+        <v>762</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>109</v>
+        <v>108</v>
+      </c>
+      <c r="C92" t="s">
+        <v>309</v>
+      </c>
+      <c r="E92" t="s">
+        <v>305</v>
+      </c>
+      <c r="F92" t="s">
+        <v>306</v>
+      </c>
+      <c r="G92" t="s">
+        <v>307</v>
+      </c>
+      <c r="H92" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>110</v>
-      </c>
-      <c r="C93" t="s">
-        <v>485</v>
-      </c>
-      <c r="E93" t="s">
-        <v>218</v>
-      </c>
-      <c r="F93" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C94" t="s">
+        <v>485</v>
+      </c>
+      <c r="E94" t="s">
+        <v>218</v>
+      </c>
+      <c r="F94" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>116</v>
-      </c>
-      <c r="C98" t="s">
-        <v>828</v>
-      </c>
-      <c r="E98" t="s">
-        <v>218</v>
-      </c>
-      <c r="F98" t="s">
-        <v>219</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="C99" t="s">
+        <v>827</v>
+      </c>
+      <c r="E99" t="s">
+        <v>218</v>
+      </c>
+      <c r="F99" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>118</v>
-      </c>
-      <c r="C100" t="s">
-        <v>778</v>
-      </c>
-      <c r="E100" t="s">
-        <v>262</v>
-      </c>
-      <c r="F100" t="s">
-        <v>244</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>817</v>
+        <v>777</v>
       </c>
       <c r="E101" t="s">
         <v>262</v>
@@ -23578,7 +23593,7 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C102" t="s">
         <v>816</v>
@@ -23592,109 +23607,123 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>122</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C103" t="s">
-        <v>73</v>
-      </c>
-      <c r="D103" t="s">
-        <v>71</v>
+        <v>815</v>
       </c>
       <c r="E103" t="s">
-        <v>69</v>
+        <v>262</v>
       </c>
       <c r="F103" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" t="s">
+        <v>73</v>
+      </c>
+      <c r="D104" t="s">
+        <v>71</v>
+      </c>
+      <c r="E104" t="s">
+        <v>69</v>
+      </c>
+      <c r="F104" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>126</v>
       </c>
-      <c r="C105" t="s">
-        <v>598</v>
-      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>127</v>
-      </c>
-      <c r="B106" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
-      </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" t="s">
-        <v>21</v>
-      </c>
-      <c r="F106" t="s">
-        <v>26</v>
+        <v>598</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>808</v>
+        <v>20</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
       </c>
       <c r="E107" t="s">
-        <v>218</v>
+        <v>21</v>
       </c>
       <c r="F107" t="s">
-        <v>219</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
-        <v>754</v>
+        <v>807</v>
+      </c>
+      <c r="E108" t="s">
+        <v>218</v>
+      </c>
+      <c r="F108" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C109" t="s">
-        <v>756</v>
-      </c>
-      <c r="E109" t="s">
-        <v>218</v>
-      </c>
-      <c r="F109" t="s">
-        <v>219</v>
+        <v>754</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C110" t="s">
-        <v>592</v>
+        <v>756</v>
       </c>
       <c r="E110" t="s">
+        <v>218</v>
+      </c>
+      <c r="F110" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
+        <v>136</v>
+      </c>
+      <c r="C111" t="s">
+        <v>592</v>
+      </c>
+      <c r="E111" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>137</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>562</v>
       </c>
     </row>
@@ -23712,7 +23741,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23981,7 +24010,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -23989,7 +24018,7 @@
         <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -23997,7 +24026,7 @@
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -24005,7 +24034,7 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
   </sheetData>
@@ -24020,8 +24049,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A386" workbookViewId="0">
-      <selection activeCell="D401" sqref="D401"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24080,7 +24109,7 @@
         <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -24122,7 +24151,7 @@
         <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -24136,7 +24165,7 @@
         <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -24174,6 +24203,9 @@
       <c r="C10" t="s">
         <v>42</v>
       </c>
+      <c r="D10" t="s">
+        <v>834</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -24421,7 +24453,7 @@
         <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -24443,7 +24475,7 @@
         <v>41</v>
       </c>
       <c r="C33" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -24454,7 +24486,7 @@
         <v>42</v>
       </c>
       <c r="C34" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -24540,7 +24572,7 @@
         <v>383</v>
       </c>
       <c r="D41" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -24692,7 +24724,7 @@
         <v>446</v>
       </c>
       <c r="C54" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -26128,7 +26160,7 @@
         <v>158</v>
       </c>
       <c r="C181" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D181" t="s">
         <v>757</v>
@@ -27163,7 +27195,7 @@
         <v>429</v>
       </c>
       <c r="D274" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -27232,7 +27264,7 @@
         <v>429</v>
       </c>
       <c r="D280" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -27246,7 +27278,7 @@
         <v>432</v>
       </c>
       <c r="D281" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -27257,7 +27289,7 @@
         <v>239</v>
       </c>
       <c r="C282" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
@@ -28595,7 +28627,7 @@
         <v>287</v>
       </c>
       <c r="C402" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="403" spans="1:8" x14ac:dyDescent="0.25">
@@ -28617,7 +28649,7 @@
         <v>289</v>
       </c>
       <c r="C404" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
     <row r="405" spans="1:8" x14ac:dyDescent="0.25">
@@ -29119,16 +29151,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -29136,13 +29168,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C2" t="s">
+        <v>813</v>
+      </c>
+      <c r="D2" t="s">
         <v>814</v>
-      </c>
-      <c r="D2" t="s">
-        <v>815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Room 7 - 12 Entry / Exit scripts
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -3333,8 +3333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4095,8 +4095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="D157" sqref="D157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22317,8 +22317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23740,8 +23740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Room 13 -  31 Entry / Exit Scripts
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="3"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="838">
   <si>
     <t>Purpose</t>
   </si>
@@ -2546,6 +2546,12 @@
   </si>
   <si>
     <t>Cutscene: 3 Guys Who Pub Anything: Receive Mail Trigger</t>
+  </si>
+  <si>
+    <t>Tentacle Mating Call</t>
+  </si>
+  <si>
+    <t>Bad Melody</t>
   </si>
 </sst>
 </file>
@@ -2877,7 +2883,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3334,7 +3340,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4095,8 +4101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D157" sqref="D157"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22317,8 +22323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23738,7 +23744,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
@@ -24037,6 +24043,22 @@
         <v>824</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>25</v>
+      </c>
+      <c r="B37" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>837</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:B32">
     <sortCondition ref="A2:A32"/>
@@ -24049,8 +24071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView topLeftCell="A419" workbookViewId="0">
+      <selection activeCell="C434" sqref="C434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finish Room Entry/Exit scripts
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="2"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20625" windowHeight="10260" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Scripts!$A$1:$F$149</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1397" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="840">
   <si>
     <t>Purpose</t>
   </si>
@@ -2552,6 +2551,12 @@
   </si>
   <si>
     <t>Bad Melody</t>
+  </si>
+  <si>
+    <t>08 = ?</t>
+  </si>
+  <si>
+    <t>Machine power down</t>
   </si>
 </sst>
 </file>
@@ -2883,7 +2888,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4101,8 +4106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D122" sqref="D122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22323,8 +22328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C73" sqref="C73"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23744,15 +23749,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -23765,58 +23770,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>574</v>
+        <v>824</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>368</v>
+        <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>712</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>567</v>
+        <v>712</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>567</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -23824,244 +23829,252 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>724</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>566</v>
+        <v>724</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>615</v>
+        <v>566</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>698</v>
+        <v>823</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>697</v>
+        <v>615</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>696</v>
+        <v>821</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>603</v>
+        <v>698</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>613</v>
+        <v>697</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>730</v>
+        <v>696</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>731</v>
+        <v>836</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B19" t="s">
-        <v>430</v>
+        <v>603</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B20" t="s">
-        <v>546</v>
+        <v>818</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>563</v>
+        <v>613</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>403</v>
+        <v>730</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B23" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>723</v>
+        <v>430</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>732</v>
+        <v>546</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B26" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B27" t="s">
-        <v>587</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>728</v>
+        <v>737</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B29" t="s">
-        <v>572</v>
+        <v>723</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>616</v>
+        <v>732</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
-        <v>196</v>
+        <v>837</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>729</v>
+        <v>565</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>818</v>
+        <v>587</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>20</v>
+        <v>55</v>
       </c>
       <c r="B34" t="s">
-        <v>821</v>
+        <v>728</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="B35" t="s">
-        <v>823</v>
+        <v>572</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="B36" t="s">
-        <v>824</v>
+        <v>839</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B37" t="s">
-        <v>836</v>
+        <v>616</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>837</v>
+        <v>196</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>69</v>
+      </c>
+      <c r="B39" t="s">
+        <v>729</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B32">
-    <sortCondition ref="A2:A32"/>
+  <sortState ref="A2:B38">
+    <sortCondition ref="A2:A38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24071,7 +24084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A419" workbookViewId="0">
+    <sheetView topLeftCell="A402" workbookViewId="0">
       <selection activeCell="C434" sqref="C434"/>
     </sheetView>
   </sheetViews>
@@ -28460,7 +28473,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="385" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>38</v>
       </c>
@@ -28471,7 +28484,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="386" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>38</v>
       </c>
@@ -28482,7 +28495,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="387" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>38</v>
       </c>
@@ -28493,7 +28506,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="388" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>38</v>
       </c>
@@ -28504,7 +28517,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="389" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>38</v>
       </c>
@@ -28515,7 +28528,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>38</v>
       </c>
@@ -28526,7 +28539,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>38</v>
       </c>
@@ -28537,7 +28550,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>38</v>
       </c>
@@ -28548,7 +28561,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>38</v>
       </c>
@@ -28559,7 +28572,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>39</v>
       </c>
@@ -28570,7 +28583,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>39</v>
       </c>
@@ -28581,7 +28594,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>39</v>
       </c>
@@ -28592,7 +28605,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>39</v>
       </c>
@@ -28603,7 +28616,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>40</v>
       </c>
@@ -28613,8 +28626,11 @@
       <c r="C398" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D398" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>41</v>
       </c>
@@ -28625,7 +28641,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Script-1: Comment the room light variables, and the pin codes
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20625" windowHeight="10260" firstSheet="2" activeTab="10"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="20625" windowHeight="10260" tabRatio="593" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="842">
   <si>
     <t>Purpose</t>
   </si>
@@ -2557,6 +2557,12 @@
   </si>
   <si>
     <t>Power Off Check</t>
+  </si>
+  <si>
+    <t>Light Off</t>
+  </si>
+  <si>
+    <t>Light Always On</t>
   </si>
 </sst>
 </file>
@@ -3112,11 +3118,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -3130,10 +3139,16 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>840</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>841</v>
       </c>
     </row>
   </sheetData>
@@ -3145,8 +3160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3361,7 +3376,7 @@
   <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4122,7 +4137,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD157"/>
   <sheetViews>
-    <sheetView topLeftCell="A136" workbookViewId="0">
+    <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="D158" sqref="D158"/>
     </sheetView>
   </sheetViews>
@@ -22337,10 +22352,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I112"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22500,132 +22515,138 @@
       <c r="A9">
         <v>20</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
+      <c r="C9" t="s">
+        <v>606</v>
+      </c>
+      <c r="E9" t="s">
+        <v>607</v>
+      </c>
+      <c r="F9" t="s">
+        <v>608</v>
+      </c>
+      <c r="G9" t="s">
+        <v>609</v>
+      </c>
+      <c r="H9" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>606</v>
+        <v>236</v>
       </c>
       <c r="E10" t="s">
-        <v>607</v>
+        <v>229</v>
       </c>
       <c r="F10" t="s">
-        <v>608</v>
+        <v>633</v>
       </c>
       <c r="G10" t="s">
-        <v>609</v>
+        <v>240</v>
       </c>
       <c r="H10" t="s">
-        <v>610</v>
+        <v>433</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>262</v>
       </c>
       <c r="E11" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>633</v>
-      </c>
-      <c r="G11" t="s">
-        <v>240</v>
-      </c>
-      <c r="H11" t="s">
-        <v>433</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>262</v>
+        <v>238</v>
       </c>
       <c r="E12" t="s">
-        <v>261</v>
+        <v>229</v>
       </c>
       <c r="F12" t="s">
-        <v>243</v>
+        <v>633</v>
+      </c>
+      <c r="G12" t="s">
+        <v>240</v>
+      </c>
+      <c r="H12" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>238</v>
+        <v>611</v>
       </c>
       <c r="E13" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F13" t="s">
-        <v>633</v>
-      </c>
-      <c r="G13" t="s">
-        <v>240</v>
-      </c>
-      <c r="H13" t="s">
-        <v>433</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="s">
-        <v>611</v>
-      </c>
-      <c r="E14" t="s">
-        <v>217</v>
-      </c>
-      <c r="F14" t="s">
-        <v>218</v>
+        <v>827</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>827</v>
+        <v>245</v>
+      </c>
+      <c r="E15" t="s">
+        <v>229</v>
+      </c>
+      <c r="F15" t="s">
+        <v>633</v>
+      </c>
+      <c r="G15" t="s">
+        <v>240</v>
+      </c>
+      <c r="H15" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>245</v>
+        <v>809</v>
       </c>
       <c r="E16" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="F16" t="s">
-        <v>633</v>
-      </c>
-      <c r="G16" t="s">
-        <v>240</v>
-      </c>
-      <c r="H16" t="s">
-        <v>433</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C17" t="s">
-        <v>809</v>
+        <v>15</v>
       </c>
       <c r="E17" t="s">
         <v>261</v>
@@ -22636,372 +22657,372 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>717</v>
       </c>
       <c r="E18" t="s">
-        <v>261</v>
+        <v>718</v>
       </c>
       <c r="F18" t="s">
-        <v>243</v>
+        <v>719</v>
+      </c>
+      <c r="G18" t="s">
+        <v>720</v>
+      </c>
+      <c r="H18" t="s">
+        <v>721</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>717</v>
+        <v>598</v>
       </c>
       <c r="E19" t="s">
-        <v>718</v>
+        <v>217</v>
       </c>
       <c r="F19" t="s">
-        <v>719</v>
+        <v>599</v>
       </c>
       <c r="G19" t="s">
-        <v>720</v>
-      </c>
-      <c r="H19" t="s">
-        <v>721</v>
+        <v>600</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>598</v>
-      </c>
-      <c r="E20" t="s">
-        <v>217</v>
-      </c>
-      <c r="F20" t="s">
-        <v>599</v>
-      </c>
-      <c r="G20" t="s">
-        <v>600</v>
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" t="s">
-        <v>151</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C31" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C32" t="s">
-        <v>269</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C33" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>153</v>
+        <v>545</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C37" t="s">
-        <v>545</v>
+        <v>170</v>
+      </c>
+      <c r="D37" t="s">
+        <v>830</v>
+      </c>
+      <c r="E37" t="s">
+        <v>831</v>
+      </c>
+      <c r="F37" t="s">
+        <v>832</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="D38" t="s">
-        <v>830</v>
+        <v>613</v>
       </c>
       <c r="E38" t="s">
-        <v>831</v>
+        <v>121</v>
       </c>
       <c r="F38" t="s">
-        <v>832</v>
+        <v>124</v>
+      </c>
+      <c r="G38" t="s">
+        <v>123</v>
+      </c>
+      <c r="H38" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>50</v>
+        <v>54</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
       </c>
       <c r="C39" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="D39" t="s">
-        <v>613</v>
-      </c>
-      <c r="E39" t="s">
-        <v>121</v>
-      </c>
-      <c r="F39" t="s">
-        <v>124</v>
-      </c>
-      <c r="G39" t="s">
-        <v>123</v>
-      </c>
-      <c r="H39" t="s">
-        <v>122</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>54</v>
-      </c>
-      <c r="B40" t="s">
-        <v>7</v>
+        <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>81</v>
-      </c>
-      <c r="D40" t="s">
-        <v>82</v>
+        <v>703</v>
+      </c>
+      <c r="E40" t="s">
+        <v>217</v>
+      </c>
+      <c r="F40" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C41" t="s">
-        <v>703</v>
+        <v>709</v>
       </c>
       <c r="E41" t="s">
-        <v>217</v>
+        <v>295</v>
       </c>
       <c r="F41" t="s">
-        <v>218</v>
+        <v>296</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>709</v>
+        <v>173</v>
       </c>
       <c r="E42" t="s">
-        <v>295</v>
+        <v>174</v>
       </c>
       <c r="F42" t="s">
-        <v>296</v>
+        <v>175</v>
+      </c>
+      <c r="G42" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" t="s">
+        <v>177</v>
+      </c>
+      <c r="I42" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>173</v>
-      </c>
-      <c r="E43" t="s">
-        <v>174</v>
-      </c>
-      <c r="F43" t="s">
-        <v>175</v>
-      </c>
-      <c r="G43" t="s">
-        <v>176</v>
-      </c>
-      <c r="H43" t="s">
-        <v>177</v>
-      </c>
-      <c r="I43" t="s">
-        <v>178</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C45" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>61</v>
+      </c>
+      <c r="C46" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>62</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C46" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>61</v>
-      </c>
-      <c r="C47" t="s">
-        <v>162</v>
+      <c r="G47" s="2" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>62</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D48" s="1"/>
+      <c r="A48">
+        <v>63</v>
+      </c>
+      <c r="C48" t="s">
+        <v>764</v>
+      </c>
       <c r="E48" t="s">
-        <v>59</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>246</v>
+        <v>229</v>
+      </c>
+      <c r="F48" t="s">
+        <v>247</v>
+      </c>
+      <c r="G48" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="E49" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F49" t="s">
-        <v>247</v>
-      </c>
-      <c r="G49" t="s">
-        <v>248</v>
+        <v>218</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="E50" t="s">
         <v>217</v>
@@ -23012,69 +23033,69 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>763</v>
+        <v>204</v>
       </c>
       <c r="E51" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="F51" t="s">
-        <v>218</v>
+        <v>403</v>
+      </c>
+      <c r="G51" t="s">
+        <v>230</v>
+      </c>
+      <c r="H51" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s">
-        <v>204</v>
-      </c>
-      <c r="E52" t="s">
-        <v>229</v>
-      </c>
-      <c r="F52" t="s">
-        <v>403</v>
-      </c>
-      <c r="G52" t="s">
-        <v>230</v>
-      </c>
-      <c r="H52" t="s">
-        <v>231</v>
+        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>67</v>
+        <v>68</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>550</v>
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" t="s">
+        <v>217</v>
+      </c>
+      <c r="F53" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>25</v>
-      </c>
-      <c r="D54" t="s">
-        <v>22</v>
+        <v>741</v>
       </c>
       <c r="E54" t="s">
-        <v>217</v>
-      </c>
-      <c r="F54" t="s">
-        <v>27</v>
+        <v>742</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -23083,276 +23104,276 @@
         <v>741</v>
       </c>
       <c r="E55" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>741</v>
-      </c>
-      <c r="E56" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>746</v>
+        <v>64</v>
+      </c>
+      <c r="E58" t="s">
+        <v>65</v>
+      </c>
+      <c r="F58" t="s">
+        <v>256</v>
+      </c>
+      <c r="G58" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>73</v>
-      </c>
-      <c r="B59" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>716</v>
       </c>
       <c r="E59" t="s">
-        <v>65</v>
-      </c>
-      <c r="F59" t="s">
-        <v>256</v>
-      </c>
-      <c r="G59" t="s">
-        <v>751</v>
+        <v>218</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C60" t="s">
-        <v>716</v>
+        <v>459</v>
       </c>
       <c r="E60" t="s">
-        <v>218</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C61" t="s">
-        <v>459</v>
+        <v>208</v>
       </c>
       <c r="E61" t="s">
-        <v>279</v>
+        <v>205</v>
+      </c>
+      <c r="F61" t="s">
+        <v>724</v>
+      </c>
+      <c r="G61" t="s">
+        <v>206</v>
+      </c>
+      <c r="H61" t="s">
+        <v>283</v>
+      </c>
+      <c r="I61" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C62" t="s">
-        <v>208</v>
+        <v>725</v>
       </c>
       <c r="E62" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
       <c r="F62" t="s">
-        <v>724</v>
-      </c>
-      <c r="G62" t="s">
-        <v>206</v>
-      </c>
-      <c r="H62" t="s">
-        <v>283</v>
-      </c>
-      <c r="I62" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C63" t="s">
-        <v>725</v>
+        <v>329</v>
       </c>
       <c r="E63" t="s">
-        <v>210</v>
-      </c>
-      <c r="F63" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C64" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E64" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="F64" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>80</v>
+        <v>81</v>
+      </c>
+      <c r="B65" t="s">
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>331</v>
+        <v>57</v>
       </c>
       <c r="E65" t="s">
-        <v>217</v>
-      </c>
-      <c r="F65" t="s">
-        <v>218</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>81</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>57</v>
+        <v>549</v>
       </c>
       <c r="E66" t="s">
-        <v>56</v>
+        <v>286</v>
+      </c>
+      <c r="F66" t="s">
+        <v>284</v>
+      </c>
+      <c r="G66" t="s">
+        <v>285</v>
+      </c>
+      <c r="H66" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C67" t="s">
-        <v>549</v>
-      </c>
-      <c r="E67" t="s">
-        <v>286</v>
-      </c>
-      <c r="F67" t="s">
-        <v>284</v>
-      </c>
-      <c r="G67" t="s">
-        <v>285</v>
-      </c>
-      <c r="H67" t="s">
-        <v>570</v>
+        <v>551</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C68" t="s">
-        <v>551</v>
+        <v>390</v>
+      </c>
+      <c r="E68" t="s">
+        <v>217</v>
+      </c>
+      <c r="F68" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
-        <v>390</v>
+        <v>767</v>
       </c>
       <c r="E69" t="s">
         <v>217</v>
       </c>
       <c r="F69" t="s">
-        <v>391</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C70" t="s">
-        <v>767</v>
-      </c>
-      <c r="E70" t="s">
-        <v>217</v>
-      </c>
-      <c r="F70" t="s">
-        <v>218</v>
+        <v>816</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C71" t="s">
-        <v>816</v>
+        <v>752</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>87</v>
-      </c>
-      <c r="C72" t="s">
-        <v>752</v>
+        <v>89</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>89</v>
+        <v>90</v>
+      </c>
+      <c r="D73" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90</v>
       </c>
-      <c r="D74" t="s">
-        <v>85</v>
+      <c r="B74" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>90</v>
-      </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75" t="s">
-        <v>102</v>
+        <v>91</v>
+      </c>
+      <c r="D75" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>91</v>
       </c>
+      <c r="B76" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" t="s">
+        <v>101</v>
+      </c>
       <c r="D76" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D77" t="s">
         <v>88</v>
@@ -23360,72 +23381,72 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>92</v>
-      </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78" t="s">
-        <v>103</v>
-      </c>
-      <c r="D78" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>94</v>
+        <v>96</v>
+      </c>
+      <c r="C79" t="s">
+        <v>216</v>
+      </c>
+      <c r="E79" t="s">
+        <v>217</v>
+      </c>
+      <c r="F79" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C80" t="s">
-        <v>216</v>
-      </c>
-      <c r="E80" t="s">
-        <v>217</v>
-      </c>
-      <c r="F80" t="s">
-        <v>218</v>
+        <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C81" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>99</v>
-      </c>
-      <c r="C83" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="C84" t="s">
+        <v>774</v>
+      </c>
+      <c r="E84" t="s">
+        <v>217</v>
+      </c>
+      <c r="F84" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C85" t="s">
-        <v>774</v>
+        <v>744</v>
       </c>
       <c r="E85" t="s">
         <v>217</v>
@@ -23436,175 +23457,175 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C86" t="s">
-        <v>744</v>
+        <v>708</v>
+      </c>
+      <c r="D86" t="s">
+        <v>74</v>
       </c>
       <c r="E86" t="s">
-        <v>217</v>
+        <v>75</v>
       </c>
       <c r="F86" t="s">
-        <v>218</v>
+        <v>705</v>
+      </c>
+      <c r="G86" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C87" t="s">
-        <v>708</v>
-      </c>
-      <c r="D87" t="s">
-        <v>74</v>
+        <v>754</v>
       </c>
       <c r="E87" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="F87" t="s">
-        <v>705</v>
-      </c>
-      <c r="G87" t="s">
-        <v>704</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>104</v>
+        <v>105</v>
+      </c>
+      <c r="B88" t="s">
+        <v>7</v>
       </c>
       <c r="C88" t="s">
-        <v>754</v>
-      </c>
-      <c r="E88" t="s">
-        <v>217</v>
-      </c>
-      <c r="F88" t="s">
-        <v>218</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>128</v>
+        <v>713</v>
+      </c>
+      <c r="E89" t="s">
+        <v>714</v>
+      </c>
+      <c r="F89" t="s">
+        <v>127</v>
+      </c>
+      <c r="G89" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>106</v>
-      </c>
-      <c r="B90" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="C90" t="s">
-        <v>713</v>
-      </c>
-      <c r="E90" t="s">
-        <v>714</v>
-      </c>
-      <c r="F90" t="s">
-        <v>127</v>
-      </c>
-      <c r="G90" t="s">
-        <v>715</v>
+        <v>761</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C91" t="s">
-        <v>761</v>
+        <v>308</v>
+      </c>
+      <c r="E91" t="s">
+        <v>304</v>
+      </c>
+      <c r="F91" t="s">
+        <v>305</v>
+      </c>
+      <c r="G91" t="s">
+        <v>306</v>
+      </c>
+      <c r="H91" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>108</v>
-      </c>
-      <c r="C92" t="s">
-        <v>308</v>
-      </c>
-      <c r="E92" t="s">
-        <v>304</v>
-      </c>
-      <c r="F92" t="s">
-        <v>305</v>
-      </c>
-      <c r="G92" t="s">
-        <v>306</v>
-      </c>
-      <c r="H92" t="s">
-        <v>307</v>
+        <v>109</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
+        <v>484</v>
+      </c>
+      <c r="E93" t="s">
+        <v>217</v>
+      </c>
+      <c r="F93" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>110</v>
-      </c>
-      <c r="C94" t="s">
-        <v>484</v>
-      </c>
-      <c r="E94" t="s">
-        <v>217</v>
-      </c>
-      <c r="F94" t="s">
-        <v>218</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="C98" t="s">
+        <v>826</v>
+      </c>
+      <c r="E98" t="s">
+        <v>217</v>
+      </c>
+      <c r="F98" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>116</v>
-      </c>
-      <c r="C99" t="s">
-        <v>826</v>
-      </c>
-      <c r="E99" t="s">
-        <v>217</v>
-      </c>
-      <c r="F99" t="s">
-        <v>218</v>
+        <v>117</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="C100" t="s">
+        <v>776</v>
+      </c>
+      <c r="E100" t="s">
+        <v>261</v>
+      </c>
+      <c r="F100" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C101" t="s">
-        <v>776</v>
+        <v>815</v>
       </c>
       <c r="E101" t="s">
         <v>261</v>
@@ -23615,10 +23636,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C102" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="E102" t="s">
         <v>261</v>
@@ -23629,123 +23650,109 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>120</v>
+        <v>122</v>
+      </c>
+      <c r="B103" t="s">
+        <v>6</v>
       </c>
       <c r="C103" t="s">
-        <v>814</v>
+        <v>73</v>
+      </c>
+      <c r="D103" t="s">
+        <v>71</v>
       </c>
       <c r="E103" t="s">
-        <v>261</v>
+        <v>69</v>
       </c>
       <c r="F103" t="s">
-        <v>243</v>
+        <v>70</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>122</v>
-      </c>
-      <c r="B104" t="s">
-        <v>6</v>
-      </c>
-      <c r="C104" t="s">
-        <v>73</v>
-      </c>
-      <c r="D104" t="s">
-        <v>71</v>
-      </c>
-      <c r="E104" t="s">
-        <v>69</v>
-      </c>
-      <c r="F104" t="s">
-        <v>70</v>
+        <v>126</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>126</v>
       </c>
+      <c r="C105" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>126</v>
+        <v>127</v>
+      </c>
+      <c r="B106" t="s">
+        <v>7</v>
       </c>
       <c r="C106" t="s">
-        <v>597</v>
+        <v>20</v>
+      </c>
+      <c r="D106" t="s">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>21</v>
+      </c>
+      <c r="F106" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>127</v>
-      </c>
-      <c r="B107" t="s">
-        <v>7</v>
+        <v>128</v>
       </c>
       <c r="C107" t="s">
-        <v>20</v>
-      </c>
-      <c r="D107" t="s">
-        <v>22</v>
+        <v>806</v>
       </c>
       <c r="E107" t="s">
-        <v>21</v>
+        <v>217</v>
       </c>
       <c r="F107" t="s">
-        <v>26</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="C108" t="s">
-        <v>806</v>
-      </c>
-      <c r="E108" t="s">
-        <v>217</v>
-      </c>
-      <c r="F108" t="s">
-        <v>218</v>
+        <v>753</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C109" t="s">
-        <v>753</v>
+        <v>755</v>
+      </c>
+      <c r="E109" t="s">
+        <v>217</v>
+      </c>
+      <c r="F109" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C110" t="s">
-        <v>755</v>
+        <v>591</v>
       </c>
       <c r="E110" t="s">
-        <v>217</v>
-      </c>
-      <c r="F110" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C111" t="s">
-        <v>591</v>
-      </c>
-      <c r="E111" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112">
-        <v>137</v>
-      </c>
-      <c r="C112" t="s">
         <v>561</v>
       </c>
     </row>
@@ -24095,8 +24102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A402" workbookViewId="0">
-      <selection activeCell="C434" sqref="C434"/>
+    <sheetView topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix variable 62 type
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.200\home\Archive\Robs Projects\Maniac.Mansion.Disassembly\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="20625" windowHeight="10260" tabRatio="593" activeTab="9"/>
+    <workbookView xWindow="1110" yWindow="0" windowWidth="37290" windowHeight="18420" tabRatio="593" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -3118,7 +3118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -22354,8 +22354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22970,7 +22970,7 @@
         <v>62</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>6</v>
+        <v>134</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Name Meteor Lock variable
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="37290" windowHeight="18420" tabRatio="593" activeTab="3"/>
+    <workbookView xWindow="1110" yWindow="0" windowWidth="22830" windowHeight="10230" tabRatio="593" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="845">
   <si>
     <t>Purpose</t>
   </si>
@@ -2563,6 +2563,15 @@
   </si>
   <si>
     <t>Light Always On</t>
+  </si>
+  <si>
+    <t>2 = Loose</t>
+  </si>
+  <si>
+    <t>Meteor Locked</t>
+  </si>
+  <si>
+    <t>1=Locked?</t>
   </si>
 </sst>
 </file>
@@ -22354,8 +22363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23322,6 +23331,15 @@
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>89</v>
+      </c>
+      <c r="C72" t="s">
+        <v>843</v>
+      </c>
+      <c r="E72" t="s">
+        <v>842</v>
+      </c>
+      <c r="F72" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix/Improve comments across a number of scripts
</commit_message>
<xml_diff>
--- a/ManiacMansion.xlsx
+++ b/ManiacMansion.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="0" windowWidth="22830" windowHeight="10230" tabRatio="593" activeTab="3"/>
+    <workbookView xWindow="1110" yWindow="0" windowWidth="22830" windowHeight="10230" tabRatio="593" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Actors" sheetId="6" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="846">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="852">
   <si>
     <t>Purpose</t>
   </si>
@@ -2575,6 +2575,24 @@
   </si>
   <si>
     <t>Nurse Edna: Out of room</t>
+  </si>
+  <si>
+    <t>Pin Entry Correct</t>
+  </si>
+  <si>
+    <t>0 = Yes</t>
+  </si>
+  <si>
+    <t>1 = No</t>
+  </si>
+  <si>
+    <t>Dr. Fred / Nurse Edna Trigger Enabled</t>
+  </si>
+  <si>
+    <t>Keypad Input Complete</t>
+  </si>
+  <si>
+    <t>08 = Fixed</t>
   </si>
 </sst>
 </file>
@@ -3387,8 +3405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4150,7 +4168,7 @@
   <dimension ref="A1:XFD157"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="D158" sqref="D158"/>
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22364,10 +22382,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="G86" sqref="G86"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22837,7 +22855,13 @@
         <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>545</v>
+        <v>846</v>
+      </c>
+      <c r="E36" t="s">
+        <v>847</v>
+      </c>
+      <c r="F36" t="s">
+        <v>848</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -22882,159 +22906,159 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>54</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" t="s">
-        <v>82</v>
+        <v>850</v>
+      </c>
+      <c r="E39" t="s">
+        <v>217</v>
+      </c>
+      <c r="F39" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="B40" t="s">
+        <v>7</v>
       </c>
       <c r="C40" t="s">
-        <v>703</v>
-      </c>
-      <c r="E40" t="s">
-        <v>217</v>
-      </c>
-      <c r="F40" t="s">
-        <v>218</v>
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>709</v>
+        <v>703</v>
       </c>
       <c r="E41" t="s">
-        <v>295</v>
+        <v>217</v>
       </c>
       <c r="F41" t="s">
-        <v>296</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
-        <v>173</v>
+        <v>709</v>
       </c>
       <c r="E42" t="s">
-        <v>174</v>
+        <v>295</v>
       </c>
       <c r="F42" t="s">
-        <v>175</v>
-      </c>
-      <c r="G42" t="s">
-        <v>176</v>
-      </c>
-      <c r="H42" t="s">
-        <v>177</v>
-      </c>
-      <c r="I42" t="s">
-        <v>178</v>
+        <v>296</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>159</v>
+        <v>173</v>
+      </c>
+      <c r="E43" t="s">
+        <v>174</v>
+      </c>
+      <c r="F43" t="s">
+        <v>175</v>
+      </c>
+      <c r="G43" t="s">
+        <v>176</v>
+      </c>
+      <c r="H43" t="s">
+        <v>177</v>
+      </c>
+      <c r="I43" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
+        <v>60</v>
+      </c>
+      <c r="C46" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47">
         <v>61</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>62</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="1"/>
-      <c r="E47" t="s">
+      <c r="D48" s="1"/>
+      <c r="E48" t="s">
         <v>59</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G47" s="2" t="s">
+      <c r="G48" s="2" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>63</v>
-      </c>
-      <c r="C48" t="s">
-        <v>764</v>
-      </c>
-      <c r="E48" t="s">
-        <v>229</v>
-      </c>
-      <c r="F48" t="s">
-        <v>247</v>
-      </c>
-      <c r="G48" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C49" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E49" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="F49" t="s">
-        <v>218</v>
+        <v>247</v>
+      </c>
+      <c r="G49" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="E50" t="s">
         <v>217</v>
@@ -23045,69 +23069,69 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C51" t="s">
-        <v>204</v>
+        <v>763</v>
       </c>
       <c r="E51" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="F51" t="s">
-        <v>403</v>
-      </c>
-      <c r="G51" t="s">
-        <v>230</v>
-      </c>
-      <c r="H51" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C52" t="s">
-        <v>550</v>
+        <v>204</v>
+      </c>
+      <c r="E52" t="s">
+        <v>229</v>
+      </c>
+      <c r="F52" t="s">
+        <v>403</v>
+      </c>
+      <c r="G52" t="s">
+        <v>230</v>
+      </c>
+      <c r="H52" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>68</v>
-      </c>
-      <c r="B53" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>25</v>
-      </c>
-      <c r="D53" t="s">
-        <v>22</v>
-      </c>
-      <c r="E53" t="s">
-        <v>217</v>
-      </c>
-      <c r="F53" t="s">
-        <v>27</v>
+        <v>550</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B54" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>741</v>
+        <v>25</v>
+      </c>
+      <c r="D54" t="s">
+        <v>22</v>
       </c>
       <c r="E54" t="s">
-        <v>742</v>
+        <v>217</v>
+      </c>
+      <c r="F54" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
         <v>7</v>
@@ -23116,285 +23140,285 @@
         <v>741</v>
       </c>
       <c r="E55" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B56" t="s">
         <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>745</v>
+        <v>741</v>
+      </c>
+      <c r="E56" t="s">
+        <v>743</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B58" t="s">
         <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>64</v>
-      </c>
-      <c r="E58" t="s">
-        <v>65</v>
-      </c>
-      <c r="F58" t="s">
-        <v>256</v>
-      </c>
-      <c r="G58" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="B59" t="s">
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>716</v>
+        <v>64</v>
       </c>
       <c r="E59" t="s">
-        <v>218</v>
+        <v>65</v>
+      </c>
+      <c r="F59" t="s">
+        <v>256</v>
+      </c>
+      <c r="G59" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C60" t="s">
-        <v>459</v>
+        <v>716</v>
       </c>
       <c r="E60" t="s">
-        <v>279</v>
+        <v>218</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" t="s">
-        <v>208</v>
+        <v>459</v>
       </c>
       <c r="E61" t="s">
-        <v>205</v>
-      </c>
-      <c r="F61" t="s">
-        <v>724</v>
-      </c>
-      <c r="G61" t="s">
-        <v>206</v>
-      </c>
-      <c r="H61" t="s">
-        <v>283</v>
-      </c>
-      <c r="I61" t="s">
-        <v>207</v>
+        <v>279</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C62" t="s">
-        <v>725</v>
+        <v>208</v>
       </c>
       <c r="E62" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F62" t="s">
-        <v>211</v>
+        <v>724</v>
+      </c>
+      <c r="G62" t="s">
+        <v>206</v>
+      </c>
+      <c r="H62" t="s">
+        <v>283</v>
+      </c>
+      <c r="I62" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
+        <v>78</v>
+      </c>
+      <c r="C63" t="s">
+        <v>725</v>
+      </c>
+      <c r="E63" t="s">
+        <v>210</v>
+      </c>
+      <c r="F63" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64">
         <v>79</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C64" t="s">
         <v>329</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E64" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64">
+    <row r="65" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65">
         <v>80</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>331</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E65" t="s">
         <v>217</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F65" t="s">
         <v>218</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>81</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65" t="s">
-        <v>57</v>
-      </c>
-      <c r="E65" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="B66" t="s">
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>549</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>286</v>
-      </c>
-      <c r="F66" t="s">
-        <v>284</v>
-      </c>
-      <c r="G66" t="s">
-        <v>285</v>
-      </c>
-      <c r="H66" t="s">
-        <v>570</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>551</v>
+        <v>549</v>
+      </c>
+      <c r="E67" t="s">
+        <v>286</v>
+      </c>
+      <c r="F67" t="s">
+        <v>284</v>
+      </c>
+      <c r="G67" t="s">
+        <v>285</v>
+      </c>
+      <c r="H67" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
-        <v>390</v>
-      </c>
-      <c r="E68" t="s">
-        <v>217</v>
-      </c>
-      <c r="F68" t="s">
-        <v>391</v>
+        <v>551</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>767</v>
+        <v>390</v>
       </c>
       <c r="E69" t="s">
         <v>217</v>
       </c>
       <c r="F69" t="s">
-        <v>218</v>
+        <v>391</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C70" t="s">
-        <v>816</v>
+        <v>767</v>
+      </c>
+      <c r="E70" t="s">
+        <v>217</v>
+      </c>
+      <c r="F70" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C71" t="s">
-        <v>752</v>
+        <v>816</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C72" t="s">
-        <v>843</v>
-      </c>
-      <c r="E72" t="s">
-        <v>842</v>
-      </c>
-      <c r="F72" t="s">
-        <v>844</v>
+        <v>752</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>90</v>
-      </c>
-      <c r="D73" t="s">
-        <v>85</v>
+        <v>89</v>
+      </c>
+      <c r="C73" t="s">
+        <v>843</v>
+      </c>
+      <c r="E73" t="s">
+        <v>842</v>
+      </c>
+      <c r="F73" t="s">
+        <v>844</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>90</v>
       </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>102</v>
+      <c r="D74" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>91</v>
-      </c>
-      <c r="D75" t="s">
-        <v>85</v>
+        <v>90</v>
+      </c>
+      <c r="B75" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>91</v>
       </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" t="s">
-        <v>101</v>
-      </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D77" t="s">
         <v>88</v>
@@ -23402,72 +23426,72 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>94</v>
+        <v>92</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>103</v>
+      </c>
+      <c r="D78" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>96</v>
-      </c>
-      <c r="C79" t="s">
-        <v>216</v>
-      </c>
-      <c r="E79" t="s">
-        <v>217</v>
-      </c>
-      <c r="F79" t="s">
-        <v>218</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C80" t="s">
-        <v>105</v>
+        <v>216</v>
+      </c>
+      <c r="E80" t="s">
+        <v>217</v>
+      </c>
+      <c r="F80" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C83" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>101</v>
-      </c>
-      <c r="C84" t="s">
-        <v>774</v>
-      </c>
-      <c r="E84" t="s">
-        <v>217</v>
-      </c>
-      <c r="F84" t="s">
-        <v>218</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C85" t="s">
-        <v>744</v>
+        <v>774</v>
       </c>
       <c r="E85" t="s">
         <v>217</v>
@@ -23478,151 +23502,160 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C86" t="s">
-        <v>708</v>
-      </c>
-      <c r="D86" t="s">
-        <v>74</v>
+        <v>744</v>
       </c>
       <c r="E86" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="F86" t="s">
-        <v>705</v>
-      </c>
-      <c r="G86" t="s">
-        <v>704</v>
+        <v>218</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C87" t="s">
-        <v>754</v>
+        <v>708</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
       </c>
       <c r="E87" t="s">
-        <v>217</v>
+        <v>75</v>
       </c>
       <c r="F87" t="s">
-        <v>218</v>
+        <v>705</v>
+      </c>
+      <c r="G87" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>105</v>
-      </c>
-      <c r="B88" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C88" t="s">
-        <v>128</v>
+        <v>754</v>
+      </c>
+      <c r="E88" t="s">
+        <v>217</v>
+      </c>
+      <c r="F88" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B89" t="s">
         <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>713</v>
-      </c>
-      <c r="E89" t="s">
-        <v>714</v>
-      </c>
-      <c r="F89" t="s">
-        <v>127</v>
-      </c>
-      <c r="G89" t="s">
-        <v>715</v>
+        <v>128</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>107</v>
+        <v>106</v>
+      </c>
+      <c r="B90" t="s">
+        <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>761</v>
+        <v>713</v>
+      </c>
+      <c r="E90" t="s">
+        <v>714</v>
+      </c>
+      <c r="F90" t="s">
+        <v>127</v>
+      </c>
+      <c r="G90" t="s">
+        <v>715</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C91" t="s">
-        <v>308</v>
-      </c>
-      <c r="E91" t="s">
-        <v>304</v>
-      </c>
-      <c r="F91" t="s">
-        <v>305</v>
-      </c>
-      <c r="G91" t="s">
-        <v>306</v>
-      </c>
-      <c r="H91" t="s">
-        <v>307</v>
+        <v>761</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C92" t="s">
-        <v>845</v>
+        <v>308</v>
       </c>
       <c r="E92" t="s">
-        <v>217</v>
+        <v>304</v>
       </c>
       <c r="F92" t="s">
-        <v>391</v>
+        <v>305</v>
+      </c>
+      <c r="G92" t="s">
+        <v>306</v>
+      </c>
+      <c r="H92" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C93" t="s">
-        <v>484</v>
+        <v>845</v>
       </c>
       <c r="E93" t="s">
         <v>217</v>
       </c>
       <c r="F93" t="s">
-        <v>218</v>
+        <v>391</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>111</v>
+        <v>110</v>
+      </c>
+      <c r="C94" t="s">
+        <v>484</v>
+      </c>
+      <c r="E94" t="s">
+        <v>217</v>
+      </c>
+      <c r="F94" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C98" t="s">
-        <v>826</v>
+        <v>849</v>
       </c>
       <c r="E98" t="s">
         <v>217</v>
@@ -23633,29 +23666,29 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>117</v>
+        <v>116</v>
+      </c>
+      <c r="C99" t="s">
+        <v>826</v>
+      </c>
+      <c r="E99" t="s">
+        <v>217</v>
+      </c>
+      <c r="F99" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>118</v>
-      </c>
-      <c r="C100" t="s">
-        <v>776</v>
-      </c>
-      <c r="E100" t="s">
-        <v>261</v>
-      </c>
-      <c r="F100" t="s">
-        <v>243</v>
+        <v>117</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C101" t="s">
-        <v>815</v>
+        <v>776</v>
       </c>
       <c r="E101" t="s">
         <v>261</v>
@@ -23666,10 +23699,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C102" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="E102" t="s">
         <v>261</v>
@@ -23680,109 +23713,123 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>122</v>
-      </c>
-      <c r="B103" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="C103" t="s">
-        <v>73</v>
-      </c>
-      <c r="D103" t="s">
-        <v>71</v>
+        <v>814</v>
       </c>
       <c r="E103" t="s">
-        <v>69</v>
+        <v>261</v>
       </c>
       <c r="F103" t="s">
-        <v>70</v>
+        <v>243</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>126</v>
+        <v>122</v>
+      </c>
+      <c r="B104" t="s">
+        <v>6</v>
+      </c>
+      <c r="C104" t="s">
+        <v>73</v>
+      </c>
+      <c r="D104" t="s">
+        <v>71</v>
+      </c>
+      <c r="E104" t="s">
+        <v>69</v>
+      </c>
+      <c r="F104" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>126</v>
       </c>
-      <c r="C105" t="s">
-        <v>597</v>
-      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>127</v>
-      </c>
-      <c r="B106" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="C106" t="s">
-        <v>20</v>
-      </c>
-      <c r="D106" t="s">
-        <v>22</v>
-      </c>
-      <c r="E106" t="s">
-        <v>21</v>
-      </c>
-      <c r="F106" t="s">
-        <v>26</v>
+        <v>597</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>128</v>
+        <v>127</v>
+      </c>
+      <c r="B107" t="s">
+        <v>7</v>
       </c>
       <c r="C107" t="s">
-        <v>806</v>
+        <v>20</v>
+      </c>
+      <c r="D107" t="s">
+        <v>22</v>
       </c>
       <c r="E107" t="s">
-        <v>217</v>
+        <v>21</v>
       </c>
       <c r="F107" t="s">
-        <v>218</v>
+        <v>26</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C108" t="s">
-        <v>753</v>
+        <v>806</v>
+      </c>
+      <c r="E108" t="s">
+        <v>217</v>
+      </c>
+      <c r="F108" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C109" t="s">
-        <v>755</v>
-      </c>
-      <c r="E109" t="s">
-        <v>217</v>
-      </c>
-      <c r="F109" t="s">
-        <v>218</v>
+        <v>753</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C110" t="s">
-        <v>591</v>
+        <v>755</v>
       </c>
       <c r="E110" t="s">
+        <v>217</v>
+      </c>
+      <c r="F110" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
+        <v>136</v>
+      </c>
+      <c r="C111" t="s">
+        <v>591</v>
+      </c>
+      <c r="E111" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112">
         <v>137</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C112" t="s">
         <v>561</v>
       </c>
     </row>
@@ -24132,8 +24179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H439"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25913,7 +25960,7 @@
         <v>656</v>
       </c>
       <c r="D151" t="s">
-        <v>568</v>
+        <v>851</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>